<commit_message>
Code for the Participant Details Page for Fanconi
</commit_message>
<xml_diff>
--- a/src/test/java/CHARMS/resources/data.xlsx
+++ b/src/test/java/CHARMS/resources/data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jains18/git/CBIIT-Test-Automation/CBIIT-Test-Automation/src/test/java/ServiceNow/CHARMS/Resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jains18/git/CBIIT-Test-Automation/CBIIT-Test-Automation/src/test/java/CHARMS/Resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E6A6E57-6855-424D-B948-921861DCE4C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEB6D4EE-562D-834F-91FE-8C3F1DEBBD78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4240" yWindow="760" windowWidth="26000" windowHeight="17640" xr2:uid="{B3E53782-D40D-CC47-BA00-27DFD8C445AF}"/>
+    <workbookView xWindow="4280" yWindow="500" windowWidth="26000" windowHeight="17640" xr2:uid="{B3E53782-D40D-CC47-BA00-27DFD8C445AF}"/>
   </bookViews>
   <sheets>
     <sheet name="FanconiScreener" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="Cancer" sheetId="6" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">FanconiScreener!$A$1:$EJ$13</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">FanconiScreener!$A$1:$EP$13</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1213" uniqueCount="433">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1223" uniqueCount="443">
   <si>
     <t>Yes</t>
   </si>
@@ -1340,6 +1340,36 @@
   </si>
   <si>
     <t>Other genes/syndromes</t>
+  </si>
+  <si>
+    <t>Caucasian (white), Black/African American, Native Hawaiian/Other Pacific Islander, American Indian/Alaskan Native, Asian, Other (please specify)</t>
+  </si>
+  <si>
+    <t>VitalStatus</t>
+  </si>
+  <si>
+    <t>Not answered</t>
+  </si>
+  <si>
+    <t>DOD</t>
+  </si>
+  <si>
+    <t>AreYouTheLegalGuardianOfThisPerson</t>
+  </si>
+  <si>
+    <t>sj.fanconitester1@yopmail.com</t>
+  </si>
+  <si>
+    <t>sj.fanconitester2@yopmail.com</t>
+  </si>
+  <si>
+    <t>RegistrationEmailAddress</t>
+  </si>
+  <si>
+    <t>ProxyEmailAddress</t>
+  </si>
+  <si>
+    <t>CalculatedAge</t>
   </si>
 </sst>
 </file>
@@ -1957,11 +1987,11 @@
   <sheetPr>
     <tabColor theme="5" tint="0.59999389629810485"/>
   </sheetPr>
-  <dimension ref="A1:EJ18"/>
+  <dimension ref="A1:EP18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BV1" zoomScale="113" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="BY2" sqref="BY2:BY13"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="113" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1980,47 +2010,48 @@
     <col min="15" max="15" width="8.5" style="3" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="10.1640625" style="3" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="7.83203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="13.33203125" style="3" customWidth="1"/>
-    <col min="19" max="19" width="16" style="3" customWidth="1"/>
-    <col min="20" max="20" width="13.1640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="13.1640625" style="3" customWidth="1"/>
-    <col min="22" max="22" width="12.83203125" style="3" customWidth="1"/>
+    <col min="18" max="20" width="13.33203125" style="3" customWidth="1"/>
+    <col min="21" max="21" width="16" style="3" customWidth="1"/>
+    <col min="22" max="22" width="13.1640625" style="3" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="13.1640625" style="3" customWidth="1"/>
-    <col min="24" max="24" width="8" style="3" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="22.83203125" style="3" customWidth="1"/>
-    <col min="26" max="26" width="17.6640625" style="3" customWidth="1"/>
-    <col min="27" max="27" width="19" style="3" customWidth="1"/>
-    <col min="28" max="28" width="13.5" style="3" customWidth="1"/>
-    <col min="29" max="29" width="5.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="7.6640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="33.33203125" style="3" customWidth="1"/>
-    <col min="32" max="32" width="30.6640625" style="3" customWidth="1"/>
-    <col min="33" max="33" width="17.83203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="15.83203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="17.33203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="20.6640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="22.5" style="3" customWidth="1"/>
-    <col min="38" max="38" width="18" style="3" customWidth="1"/>
-    <col min="39" max="39" width="12.5" style="3" customWidth="1"/>
-    <col min="40" max="40" width="16" style="3" customWidth="1"/>
-    <col min="41" max="41" width="16.5" style="3" customWidth="1"/>
-    <col min="42" max="42" width="7" style="3" customWidth="1"/>
-    <col min="43" max="43" width="12.6640625" style="3" customWidth="1"/>
-    <col min="44" max="44" width="10.83203125" style="3" customWidth="1"/>
-    <col min="45" max="45" width="28.6640625" style="3" customWidth="1"/>
-    <col min="46" max="46" width="20.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="36.5" style="3" customWidth="1"/>
-    <col min="48" max="48" width="20.33203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="49" max="58" width="20.33203125" style="3" customWidth="1"/>
-    <col min="59" max="59" width="16.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="60" max="60" width="20.1640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="61" max="62" width="20.1640625" style="3" customWidth="1"/>
-    <col min="63" max="113" width="20.83203125" style="3"/>
-    <col min="114" max="114" width="38.33203125" style="3" customWidth="1"/>
-    <col min="115" max="16384" width="20.83203125" style="3"/>
+    <col min="24" max="24" width="12.83203125" style="3" customWidth="1"/>
+    <col min="25" max="25" width="13.1640625" style="3" customWidth="1"/>
+    <col min="26" max="26" width="8" style="3" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="8" style="3" customWidth="1"/>
+    <col min="28" max="28" width="22.83203125" style="3" customWidth="1"/>
+    <col min="29" max="29" width="17.6640625" style="3" customWidth="1"/>
+    <col min="30" max="30" width="19" style="3" customWidth="1"/>
+    <col min="31" max="31" width="13.5" style="3" customWidth="1"/>
+    <col min="32" max="32" width="5.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="7.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="33.33203125" style="3" customWidth="1"/>
+    <col min="35" max="37" width="30.6640625" style="3" customWidth="1"/>
+    <col min="38" max="38" width="17.83203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="15.83203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="17.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="20.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="22.5" style="3" customWidth="1"/>
+    <col min="43" max="43" width="18" style="3" customWidth="1"/>
+    <col min="44" max="44" width="12.5" style="3" customWidth="1"/>
+    <col min="45" max="45" width="16" style="3" customWidth="1"/>
+    <col min="46" max="46" width="16.5" style="3" customWidth="1"/>
+    <col min="47" max="47" width="7" style="3" customWidth="1"/>
+    <col min="48" max="48" width="12.6640625" style="3" customWidth="1"/>
+    <col min="49" max="49" width="10.83203125" style="3" customWidth="1"/>
+    <col min="50" max="51" width="28.6640625" style="3" customWidth="1"/>
+    <col min="52" max="52" width="20.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="36.5" style="3" customWidth="1"/>
+    <col min="54" max="54" width="20.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="55" max="64" width="20.33203125" style="3" customWidth="1"/>
+    <col min="65" max="65" width="16.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="66" max="66" width="20.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="67" max="68" width="20.1640625" style="3" customWidth="1"/>
+    <col min="69" max="119" width="20.83203125" style="3"/>
+    <col min="120" max="120" width="38.33203125" style="3" customWidth="1"/>
+    <col min="121" max="16384" width="20.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:140" s="13" customFormat="1" ht="85" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:146" s="13" customFormat="1" ht="85" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
         <v>193</v>
       </c>
@@ -2075,374 +2106,392 @@
       <c r="R1" s="9" t="s">
         <v>128</v>
       </c>
-      <c r="S1" s="10" t="s">
+      <c r="S1" s="9" t="s">
+        <v>436</v>
+      </c>
+      <c r="T1" s="9" t="s">
+        <v>442</v>
+      </c>
+      <c r="U1" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="T1" s="10" t="s">
+      <c r="V1" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="U1" s="10" t="s">
+      <c r="W1" s="10" t="s">
         <v>184</v>
       </c>
-      <c r="V1" s="10" t="s">
+      <c r="X1" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="W1" s="10" t="s">
+      <c r="Y1" s="10" t="s">
         <v>185</v>
       </c>
-      <c r="X1" s="11" t="s">
+      <c r="Z1" s="11" t="s">
         <v>198</v>
       </c>
-      <c r="Y1" s="7" t="s">
+      <c r="AA1" s="11" t="s">
+        <v>434</v>
+      </c>
+      <c r="AB1" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="Z1" s="7" t="s">
+      <c r="AC1" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="AA1" s="7" t="s">
+      <c r="AD1" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="AB1" s="7" t="s">
+      <c r="AE1" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="AC1" s="7" t="s">
+      <c r="AF1" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="AD1" s="7" t="s">
+      <c r="AG1" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="AE1" s="12" t="s">
+      <c r="AH1" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="AF1" s="12" t="s">
+      <c r="AI1" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="AG1" s="14" t="s">
+      <c r="AJ1" s="12" t="s">
+        <v>440</v>
+      </c>
+      <c r="AK1" s="12" t="s">
+        <v>441</v>
+      </c>
+      <c r="AL1" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="AH1" s="14" t="s">
+      <c r="AM1" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="AI1" s="14" t="s">
+      <c r="AN1" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="AJ1" s="14" t="s">
+      <c r="AO1" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="AK1" s="15" t="s">
+      <c r="AP1" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="AL1" s="15" t="s">
+      <c r="AQ1" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="AM1" s="15" t="s">
+      <c r="AR1" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="AN1" s="15" t="s">
+      <c r="AS1" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="AO1" s="15" t="s">
+      <c r="AT1" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="AP1" s="15" t="s">
+      <c r="AU1" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="AQ1" s="15" t="s">
+      <c r="AV1" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="AR1" s="15" t="s">
+      <c r="AW1" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="AS1" s="15" t="s">
+      <c r="AX1" s="15" t="s">
         <v>191</v>
       </c>
-      <c r="AT1" s="16" t="s">
+      <c r="AY1" s="15" t="s">
+        <v>437</v>
+      </c>
+      <c r="AZ1" s="16" t="s">
         <v>203</v>
       </c>
-      <c r="AU1" s="16" t="s">
+      <c r="BA1" s="16" t="s">
         <v>247</v>
       </c>
-      <c r="AV1" s="16" t="s">
+      <c r="BB1" s="16" t="s">
         <v>54</v>
       </c>
-      <c r="AW1" s="16" t="s">
+      <c r="BC1" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="AX1" s="16" t="s">
+      <c r="BD1" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="AY1" s="16" t="s">
+      <c r="BE1" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="AZ1" s="16" t="s">
+      <c r="BF1" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="BA1" s="16" t="s">
+      <c r="BG1" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="BB1" s="16" t="s">
+      <c r="BH1" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="BC1" s="16" t="s">
+      <c r="BI1" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="BD1" s="16" t="s">
+      <c r="BJ1" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="BE1" s="16" t="s">
+      <c r="BK1" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="BF1" s="16" t="s">
+      <c r="BL1" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="BG1" s="13" t="s">
+      <c r="BM1" s="13" t="s">
         <v>204</v>
       </c>
-      <c r="BH1" s="13" t="s">
+      <c r="BN1" s="13" t="s">
         <v>208</v>
       </c>
-      <c r="BI1" s="13" t="s">
+      <c r="BO1" s="13" t="s">
         <v>209</v>
       </c>
-      <c r="BJ1" s="13" t="s">
+      <c r="BP1" s="13" t="s">
         <v>210</v>
       </c>
-      <c r="BK1" s="13" t="s">
+      <c r="BQ1" s="13" t="s">
         <v>205</v>
       </c>
-      <c r="BL1" s="13" t="s">
+      <c r="BR1" s="13" t="s">
         <v>206</v>
       </c>
-      <c r="BM1" s="13" t="s">
+      <c r="BS1" s="13" t="s">
         <v>207</v>
       </c>
-      <c r="BN1" s="13" t="s">
+      <c r="BT1" s="13" t="s">
         <v>367</v>
       </c>
-      <c r="BO1" s="13" t="s">
+      <c r="BU1" s="13" t="s">
         <v>366</v>
       </c>
-      <c r="BP1" s="13" t="s">
+      <c r="BV1" s="13" t="s">
         <v>212</v>
       </c>
-      <c r="BQ1" s="13" t="s">
+      <c r="BW1" s="13" t="s">
         <v>266</v>
       </c>
-      <c r="BR1" s="13" t="s">
+      <c r="BX1" s="13" t="s">
         <v>267</v>
       </c>
-      <c r="BS1" s="13" t="s">
+      <c r="BY1" s="13" t="s">
         <v>211</v>
       </c>
-      <c r="BT1" s="13" t="s">
+      <c r="BZ1" s="13" t="s">
         <v>213</v>
       </c>
-      <c r="BU1" s="13" t="s">
+      <c r="CA1" s="13" t="s">
         <v>214</v>
       </c>
-      <c r="BV1" s="13" t="s">
+      <c r="CB1" s="13" t="s">
         <v>368</v>
       </c>
-      <c r="BW1" s="13" t="s">
+      <c r="CC1" s="13" t="s">
         <v>188</v>
       </c>
-      <c r="BX1" s="13" t="s">
+      <c r="CD1" s="13" t="s">
         <v>189</v>
       </c>
-      <c r="BY1" s="13" t="s">
+      <c r="CE1" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="BZ1" s="13" t="s">
+      <c r="CF1" s="13" t="s">
         <v>69</v>
       </c>
-      <c r="CA1" s="13" t="s">
+      <c r="CG1" s="13" t="s">
         <v>70</v>
       </c>
-      <c r="CB1" s="13" t="s">
+      <c r="CH1" s="13" t="s">
         <v>71</v>
       </c>
-      <c r="CC1" s="13" t="s">
+      <c r="CI1" s="13" t="s">
         <v>72</v>
       </c>
-      <c r="CD1" s="13" t="s">
+      <c r="CJ1" s="13" t="s">
         <v>215</v>
       </c>
-      <c r="CE1" s="13" t="s">
+      <c r="CK1" s="13" t="s">
         <v>216</v>
       </c>
-      <c r="CF1" s="13" t="s">
+      <c r="CL1" s="13" t="s">
         <v>217</v>
       </c>
-      <c r="CG1" s="13" t="s">
+      <c r="CM1" s="13" t="s">
         <v>218</v>
       </c>
-      <c r="CH1" s="13" t="s">
+      <c r="CN1" s="13" t="s">
         <v>240</v>
       </c>
-      <c r="CI1" s="13" t="s">
+      <c r="CO1" s="13" t="s">
         <v>241</v>
       </c>
-      <c r="CJ1" s="13" t="s">
+      <c r="CP1" s="13" t="s">
         <v>242</v>
       </c>
-      <c r="CK1" s="13" t="s">
+      <c r="CQ1" s="13" t="s">
         <v>243</v>
       </c>
-      <c r="CL1" s="13" t="s">
+      <c r="CR1" s="13" t="s">
         <v>244</v>
       </c>
-      <c r="CM1" s="13" t="s">
+      <c r="CS1" s="13" t="s">
         <v>219</v>
       </c>
-      <c r="CN1" s="13" t="s">
+      <c r="CT1" s="13" t="s">
         <v>220</v>
       </c>
-      <c r="CO1" s="13" t="s">
+      <c r="CU1" s="13" t="s">
         <v>230</v>
       </c>
-      <c r="CP1" s="13" t="s">
+      <c r="CV1" s="13" t="s">
         <v>229</v>
       </c>
-      <c r="CQ1" s="13" t="s">
+      <c r="CW1" s="13" t="s">
         <v>228</v>
       </c>
-      <c r="CR1" s="13" t="s">
+      <c r="CX1" s="13" t="s">
         <v>231</v>
       </c>
-      <c r="CS1" s="13" t="s">
+      <c r="CY1" s="13" t="s">
         <v>81</v>
       </c>
-      <c r="CT1" s="13" t="s">
+      <c r="CZ1" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="CU1" s="13" t="s">
+      <c r="DA1" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="CV1" s="13" t="s">
+      <c r="DB1" s="13" t="s">
         <v>86</v>
       </c>
-      <c r="CW1" s="13" t="s">
+      <c r="DC1" s="13" t="s">
         <v>87</v>
       </c>
-      <c r="CX1" s="13" t="s">
+      <c r="DD1" s="13" t="s">
         <v>91</v>
       </c>
-      <c r="CY1" s="13" t="s">
+      <c r="DE1" s="13" t="s">
         <v>90</v>
       </c>
-      <c r="CZ1" s="13" t="s">
+      <c r="DF1" s="13" t="s">
         <v>92</v>
       </c>
-      <c r="DA1" s="13" t="s">
+      <c r="DG1" s="13" t="s">
         <v>221</v>
       </c>
-      <c r="DB1" s="13" t="s">
+      <c r="DH1" s="13" t="s">
         <v>225</v>
       </c>
-      <c r="DC1" s="13" t="s">
+      <c r="DI1" s="13" t="s">
         <v>110</v>
       </c>
-      <c r="DD1" s="13" t="s">
+      <c r="DJ1" s="13" t="s">
         <v>226</v>
       </c>
-      <c r="DE1" s="13" t="s">
+      <c r="DK1" s="13" t="s">
         <v>362</v>
       </c>
-      <c r="DF1" s="13" t="s">
+      <c r="DL1" s="13" t="s">
         <v>114</v>
       </c>
-      <c r="DG1" s="13" t="s">
+      <c r="DM1" s="13" t="s">
         <v>116</v>
       </c>
-      <c r="DH1" s="13" t="s">
+      <c r="DN1" s="13" t="s">
         <v>118</v>
       </c>
-      <c r="DI1" s="13" t="s">
+      <c r="DO1" s="13" t="s">
         <v>227</v>
       </c>
-      <c r="DJ1" s="13" t="s">
+      <c r="DP1" s="13" t="s">
         <v>245</v>
       </c>
-      <c r="DK1" s="13" t="s">
+      <c r="DQ1" s="13" t="s">
         <v>232</v>
       </c>
-      <c r="DL1" s="13" t="s">
+      <c r="DR1" s="13" t="s">
         <v>233</v>
       </c>
-      <c r="DM1" s="13" t="s">
+      <c r="DS1" s="13" t="s">
         <v>234</v>
       </c>
-      <c r="DN1" s="13" t="s">
+      <c r="DT1" s="13" t="s">
         <v>235</v>
       </c>
-      <c r="DO1" s="13" t="s">
+      <c r="DU1" s="13" t="s">
         <v>236</v>
       </c>
-      <c r="DP1" s="13" t="s">
+      <c r="DV1" s="13" t="s">
         <v>237</v>
       </c>
-      <c r="DQ1" s="13" t="s">
+      <c r="DW1" s="13" t="s">
         <v>238</v>
       </c>
-      <c r="DR1" s="13" t="s">
+      <c r="DX1" s="13" t="s">
         <v>239</v>
       </c>
-      <c r="DS1" s="17" t="s">
+      <c r="DY1" s="17" t="s">
         <v>265</v>
       </c>
-      <c r="DT1" s="17" t="s">
+      <c r="DZ1" s="17" t="s">
         <v>248</v>
       </c>
-      <c r="DU1" s="17" t="s">
+      <c r="EA1" s="17" t="s">
         <v>249</v>
       </c>
-      <c r="DV1" s="17" t="s">
+      <c r="EB1" s="17" t="s">
         <v>250</v>
       </c>
-      <c r="DW1" s="17" t="s">
+      <c r="EC1" s="17" t="s">
         <v>251</v>
       </c>
-      <c r="DX1" s="17" t="s">
+      <c r="ED1" s="17" t="s">
         <v>252</v>
       </c>
-      <c r="DY1" s="17" t="s">
+      <c r="EE1" s="17" t="s">
         <v>253</v>
       </c>
-      <c r="DZ1" s="17" t="s">
+      <c r="EF1" s="17" t="s">
         <v>254</v>
       </c>
-      <c r="EA1" s="17" t="s">
+      <c r="EG1" s="17" t="s">
         <v>255</v>
       </c>
-      <c r="EB1" s="17" t="s">
+      <c r="EH1" s="17" t="s">
         <v>256</v>
       </c>
-      <c r="EC1" s="17" t="s">
+      <c r="EI1" s="17" t="s">
         <v>257</v>
       </c>
-      <c r="ED1" s="17" t="s">
+      <c r="EJ1" s="17" t="s">
         <v>259</v>
       </c>
-      <c r="EE1" s="17" t="s">
+      <c r="EK1" s="17" t="s">
         <v>258</v>
       </c>
-      <c r="EF1" s="17" t="s">
+      <c r="EL1" s="17" t="s">
         <v>260</v>
       </c>
-      <c r="EG1" s="17" t="s">
+      <c r="EM1" s="17" t="s">
         <v>261</v>
       </c>
-      <c r="EH1" s="17" t="s">
+      <c r="EN1" s="17" t="s">
         <v>262</v>
       </c>
-      <c r="EI1" s="17" t="s">
+      <c r="EO1" s="17" t="s">
         <v>263</v>
       </c>
-      <c r="EJ1" s="17" t="s">
+      <c r="EP1" s="17" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="2" spans="1:140" s="21" customFormat="1" ht="85" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:146" s="21" customFormat="1" ht="85" x14ac:dyDescent="0.2">
       <c r="A2" s="21" t="s">
         <v>38</v>
       </c>
@@ -2470,300 +2519,296 @@
       <c r="R2" s="22" t="s">
         <v>269</v>
       </c>
-      <c r="S2" s="21" t="s">
+      <c r="S2" s="22"/>
+      <c r="T2" s="22">
+        <v>76</v>
+      </c>
+      <c r="U2" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="T2" s="21" t="s">
+      <c r="V2" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="V2" s="21" t="s">
+      <c r="X2" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="X2" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="Y2" s="21" t="s">
+      <c r="Z2" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="AA2" s="21" t="s">
+        <v>435</v>
+      </c>
+      <c r="AB2" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="Z2" s="21" t="s">
+      <c r="AC2" s="21" t="s">
         <v>199</v>
       </c>
-      <c r="AA2" s="21" t="s">
+      <c r="AD2" s="21" t="s">
         <v>200</v>
       </c>
-      <c r="AB2" s="21" t="s">
+      <c r="AE2" s="21" t="s">
         <v>201</v>
       </c>
-      <c r="AC2" s="21" t="s">
+      <c r="AF2" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="AD2" s="21">
+      <c r="AG2" s="21">
         <v>28907</v>
       </c>
-      <c r="AE2" s="18" t="s">
+      <c r="AH2" s="18" t="s">
         <v>303</v>
       </c>
-      <c r="AF2" s="18" t="s">
+      <c r="AI2" s="18" t="s">
         <v>303</v>
       </c>
-      <c r="AG2" s="21">
+      <c r="AJ2" s="19" t="s">
+        <v>438</v>
+      </c>
+      <c r="AK2" s="19"/>
+      <c r="AL2" s="21">
         <v>3015774089</v>
       </c>
-      <c r="AH2" s="21">
+      <c r="AM2" s="21">
         <v>3014524258</v>
       </c>
-      <c r="AI2" s="21">
+      <c r="AN2" s="21">
         <v>3015567865</v>
       </c>
-      <c r="AJ2" s="21">
+      <c r="AO2" s="21">
         <v>3015774089</v>
       </c>
-      <c r="AK2" s="21" t="s">
+      <c r="AP2" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="AL2" s="21" t="s">
+      <c r="AQ2" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="AM2" s="21" t="s">
+      <c r="AR2" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="AN2" s="21" t="s">
+      <c r="AS2" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="AO2" s="21" t="s">
+      <c r="AT2" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="AP2" s="21" t="s">
+      <c r="AU2" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="AQ2" s="21" t="s">
+      <c r="AV2" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="AR2" s="21" t="s">
+      <c r="AW2" s="21" t="s">
         <v>40</v>
       </c>
-      <c r="AS2" s="21" t="s">
-        <v>192</v>
-      </c>
-      <c r="AT2" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="AU2" s="21" t="s">
+      <c r="AX2" s="21" t="s">
+        <v>433</v>
+      </c>
+      <c r="AY2" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="AZ2" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="BA2" s="21" t="s">
         <v>304</v>
       </c>
-      <c r="AV2" s="21" t="s">
+      <c r="BB2" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="AW2" s="21" t="s">
+      <c r="BC2" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="AX2" s="21" t="s">
+      <c r="BD2" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="AY2" s="21" t="s">
+      <c r="BE2" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="AZ2" s="21" t="s">
+      <c r="BF2" s="21" t="s">
         <v>56</v>
       </c>
-      <c r="BA2" s="21" t="s">
+      <c r="BG2" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="BB2" s="21" t="s">
+      <c r="BH2" s="21" t="s">
         <v>57</v>
       </c>
-      <c r="BC2" s="21" t="s">
+      <c r="BI2" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="BD2" s="21" t="s">
+      <c r="BJ2" s="21" t="s">
         <v>58</v>
       </c>
-      <c r="BE2" s="21" t="s">
+      <c r="BK2" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="BF2" s="21" t="s">
+      <c r="BL2" s="21" t="s">
         <v>59</v>
       </c>
-      <c r="BG2" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="BH2" s="21" t="s">
+      <c r="BM2" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="BN2" s="21" t="s">
         <v>64</v>
       </c>
-      <c r="BJ2" s="21">
+      <c r="BP2" s="21">
         <v>91</v>
       </c>
-      <c r="BK2" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="BL2" s="21" t="s">
+      <c r="BQ2" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="BR2" s="21" t="s">
         <v>65</v>
       </c>
-      <c r="BP2" s="21" t="s">
+      <c r="BV2" s="21" t="s">
         <v>66</v>
       </c>
-      <c r="BQ2" s="23" t="s">
+      <c r="BW2" s="23" t="s">
         <v>268</v>
       </c>
-      <c r="BR2" s="23" t="s">
+      <c r="BX2" s="23" t="s">
         <v>268</v>
       </c>
-      <c r="BS2" s="21" t="s">
+      <c r="BY2" s="21" t="s">
         <v>67</v>
       </c>
-      <c r="BT2" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="BU2" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="BY2" s="21" t="s">
+      <c r="BZ2" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="CA2" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="CE2" s="21" t="s">
         <v>432</v>
       </c>
-      <c r="BZ2" s="21" t="s">
+      <c r="CF2" s="21" t="s">
         <v>75</v>
       </c>
-      <c r="CA2" s="21" t="s">
+      <c r="CG2" s="21" t="s">
         <v>73</v>
       </c>
-      <c r="CB2" s="21" t="s">
+      <c r="CH2" s="21" t="s">
         <v>74</v>
       </c>
-      <c r="CC2" s="21" t="s">
+      <c r="CI2" s="21" t="s">
         <v>73</v>
       </c>
-      <c r="CD2" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="CE2" s="21" t="s">
+      <c r="CJ2" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="CK2" s="21" t="s">
         <v>67</v>
       </c>
-      <c r="CF2" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="CG2" s="21" t="s">
+      <c r="CL2" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="CM2" s="21" t="s">
         <v>78</v>
       </c>
-      <c r="CH2" s="21" t="s">
+      <c r="CN2" s="21" t="s">
         <v>77</v>
       </c>
-      <c r="CI2" s="21">
+      <c r="CO2" s="21">
         <v>1997</v>
       </c>
-      <c r="CK2" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="CL2" s="21" t="s">
+      <c r="CQ2" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="CR2" s="21" t="s">
         <v>76</v>
       </c>
-      <c r="CM2" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="CN2" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="CO2" s="21" t="s">
+      <c r="CS2" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="CT2" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="CU2" s="21" t="s">
         <v>79</v>
       </c>
-      <c r="CQ2" s="21">
+      <c r="CW2" s="21">
         <v>101</v>
       </c>
-      <c r="CR2" s="21" t="s">
+      <c r="CX2" s="21" t="s">
         <v>80</v>
       </c>
-      <c r="CS2" s="21" t="s">
+      <c r="CY2" s="21" t="s">
         <v>82</v>
       </c>
-      <c r="CT2" s="21" t="s">
+      <c r="CZ2" s="21" t="s">
         <v>78</v>
       </c>
-      <c r="CU2" s="21" t="s">
+      <c r="DA2" s="21" t="s">
         <v>85</v>
       </c>
-      <c r="CV2" s="21">
+      <c r="DB2" s="21">
         <v>1985</v>
       </c>
-      <c r="CX2" s="21" t="s">
+      <c r="DD2" s="21" t="s">
         <v>88</v>
       </c>
-      <c r="CY2" s="21" t="s">
+      <c r="DE2" s="21" t="s">
         <v>89</v>
       </c>
-      <c r="CZ2" s="21" t="s">
+      <c r="DF2" s="21" t="s">
         <v>93</v>
       </c>
-      <c r="DA2" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="DB2" s="21" t="s">
+      <c r="DG2" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="DH2" s="21" t="s">
         <v>109</v>
       </c>
-      <c r="DC2" s="21" t="s">
+      <c r="DI2" s="21" t="s">
         <v>111</v>
       </c>
-      <c r="DD2" s="21" t="s">
+      <c r="DJ2" s="21" t="s">
         <v>112</v>
       </c>
-      <c r="DE2" s="21" t="s">
+      <c r="DK2" s="21" t="s">
         <v>113</v>
       </c>
-      <c r="DF2" s="21" t="s">
+      <c r="DL2" s="21" t="s">
         <v>115</v>
       </c>
-      <c r="DG2" s="21" t="s">
+      <c r="DM2" s="21" t="s">
         <v>117</v>
       </c>
-      <c r="DH2" s="21">
+      <c r="DN2" s="21">
         <v>3028976789</v>
       </c>
-      <c r="DI2" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="DJ2" s="21" t="s">
+      <c r="DO2" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="DP2" s="21" t="s">
         <v>246</v>
       </c>
-      <c r="DK2" s="21" t="s">
+      <c r="DQ2" s="21" t="s">
         <v>123</v>
       </c>
-      <c r="DL2" s="21" t="s">
+      <c r="DR2" s="21" t="s">
         <v>122</v>
       </c>
-      <c r="DM2" s="21" t="s">
+      <c r="DS2" s="21" t="s">
         <v>124</v>
       </c>
-      <c r="DN2" s="21" t="s">
+      <c r="DT2" s="21" t="s">
         <v>121</v>
       </c>
-      <c r="DO2" s="21" t="s">
+      <c r="DU2" s="21" t="s">
         <v>125</v>
       </c>
-      <c r="DP2" s="21" t="s">
+      <c r="DV2" s="21" t="s">
         <v>120</v>
       </c>
-      <c r="DQ2" s="21" t="s">
+      <c r="DW2" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="DR2" s="21" t="s">
+      <c r="DX2" s="21" t="s">
         <v>119</v>
       </c>
-      <c r="DS2" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="DT2" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="DU2" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="DV2" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="DW2" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="DX2" s="21" t="s">
-        <v>0</v>
-      </c>
       <c r="DY2" s="21" t="s">
         <v>0</v>
       </c>
@@ -2782,26 +2827,44 @@
       <c r="ED2" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="EE2" s="27" t="s">
+      <c r="EE2" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="EF2" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="EG2" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="EH2" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="EI2" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="EJ2" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="EK2" s="27" t="s">
         <v>425</v>
       </c>
-      <c r="EF2" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="EG2" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="EH2" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="EI2" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="EJ2" s="21" t="s">
+      <c r="EL2" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="EM2" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="EN2" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="EO2" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="EP2" s="21" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:140" s="21" customFormat="1" ht="46" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:146" s="21" customFormat="1" ht="46" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="21" t="s">
         <v>38</v>
       </c>
@@ -2829,231 +2892,219 @@
       <c r="R3" s="22" t="s">
         <v>419</v>
       </c>
-      <c r="S3" s="21" t="s">
+      <c r="S3" s="22"/>
+      <c r="T3" s="22"/>
+      <c r="U3" s="21" t="s">
         <v>144</v>
       </c>
-      <c r="T3" s="21" t="s">
+      <c r="V3" s="21" t="s">
         <v>144</v>
       </c>
-      <c r="V3" s="21" t="s">
+      <c r="X3" s="21" t="s">
         <v>167</v>
       </c>
-      <c r="X3" s="21" t="s">
-        <v>137</v>
-      </c>
-      <c r="Y3" s="21" t="s">
+      <c r="Z3" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="AB3" s="21" t="s">
         <v>169</v>
       </c>
-      <c r="AE3" s="18" t="s">
+      <c r="AH3" s="18" t="s">
         <v>145</v>
       </c>
-      <c r="AF3" s="18" t="s">
+      <c r="AI3" s="18" t="s">
         <v>145</v>
       </c>
-      <c r="AG3" s="21">
+      <c r="AJ3" s="19" t="s">
+        <v>439</v>
+      </c>
+      <c r="AK3" s="19"/>
+      <c r="AL3" s="21">
         <v>3015774089</v>
       </c>
-      <c r="AH3" s="21">
+      <c r="AM3" s="21">
         <v>3014524258</v>
       </c>
-      <c r="AI3" s="21">
+      <c r="AN3" s="21">
         <v>3015567865</v>
       </c>
-      <c r="AJ3" s="21">
+      <c r="AO3" s="21">
         <v>3014524258</v>
       </c>
-      <c r="AK3" s="21" t="s">
+      <c r="AP3" s="21" t="s">
         <v>146</v>
       </c>
-      <c r="AL3" s="21" t="s">
+      <c r="AQ3" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="AM3" s="21" t="s">
+      <c r="AR3" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="AN3" s="21" t="s">
+      <c r="AS3" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="AO3" s="21" t="s">
+      <c r="AT3" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="AP3" s="21" t="s">
+      <c r="AU3" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="AQ3" s="21" t="s">
+      <c r="AV3" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="AR3" s="21" t="s">
+      <c r="AW3" s="21" t="s">
         <v>40</v>
       </c>
-      <c r="AS3" s="21" t="s">
+      <c r="AX3" s="21" t="s">
         <v>192</v>
       </c>
-      <c r="AT3" s="21" t="s">
-        <v>137</v>
-      </c>
-      <c r="BG3" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="BH3" s="21" t="s">
+      <c r="AZ3" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="BM3" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="BN3" s="21" t="s">
         <v>149</v>
       </c>
-      <c r="BI3" s="22" t="s">
+      <c r="BO3" s="22" t="s">
         <v>300</v>
       </c>
-      <c r="BK3" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="BL3" s="21" t="s">
+      <c r="BQ3" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="BR3" s="21" t="s">
         <v>150</v>
       </c>
-      <c r="BP3" s="21" t="s">
+      <c r="BV3" s="21" t="s">
         <v>151</v>
       </c>
-      <c r="BS3" s="21" t="s">
+      <c r="BY3" s="21" t="s">
         <v>152</v>
       </c>
-      <c r="BT3" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="BU3" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="BY3" s="21" t="s">
+      <c r="BZ3" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="CA3" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="CE3" s="21" t="s">
         <v>432</v>
       </c>
-      <c r="BZ3" s="21" t="s">
+      <c r="CF3" s="21" t="s">
         <v>75</v>
       </c>
-      <c r="CA3" s="21" t="s">
+      <c r="CG3" s="21" t="s">
         <v>153</v>
       </c>
-      <c r="CB3" s="21" t="s">
+      <c r="CH3" s="21" t="s">
         <v>74</v>
       </c>
-      <c r="CC3" s="21" t="s">
+      <c r="CI3" s="21" t="s">
         <v>153</v>
       </c>
-      <c r="CD3" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="CE3" s="21" t="s">
+      <c r="CJ3" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="CK3" s="21" t="s">
         <v>152</v>
       </c>
-      <c r="CF3" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="CG3" s="21" t="s">
+      <c r="CL3" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="CM3" s="21" t="s">
         <v>79</v>
       </c>
-      <c r="CJ3" s="21">
+      <c r="CP3" s="21">
         <v>100</v>
       </c>
-      <c r="CK3" s="21" t="s">
-        <v>137</v>
-      </c>
-      <c r="CL3" s="21" t="s">
+      <c r="CQ3" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="CR3" s="21" t="s">
         <v>76</v>
       </c>
-      <c r="CM3" s="21" t="s">
-        <v>137</v>
-      </c>
-      <c r="CN3" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="CO3" s="21" t="s">
+      <c r="CS3" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="CT3" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="CU3" s="21" t="s">
         <v>149</v>
       </c>
-      <c r="CP3" s="22" t="s">
+      <c r="CV3" s="22" t="s">
         <v>328</v>
       </c>
-      <c r="CR3" s="21" t="s">
+      <c r="CX3" s="21" t="s">
         <v>80</v>
       </c>
-      <c r="CS3" s="21" t="s">
+      <c r="CY3" s="21" t="s">
         <v>82</v>
       </c>
-      <c r="CT3" s="21" t="s">
+      <c r="CZ3" s="21" t="s">
         <v>79</v>
       </c>
-      <c r="CW3" s="21">
+      <c r="DC3" s="21">
         <v>102</v>
       </c>
-      <c r="CX3" s="21" t="s">
+      <c r="DD3" s="21" t="s">
         <v>154</v>
       </c>
-      <c r="CY3" s="21" t="s">
+      <c r="DE3" s="21" t="s">
         <v>155</v>
       </c>
-      <c r="CZ3" s="21" t="s">
+      <c r="DF3" s="21" t="s">
         <v>156</v>
       </c>
-      <c r="DA3" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="DB3" s="21" t="s">
+      <c r="DG3" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="DH3" s="21" t="s">
         <v>159</v>
       </c>
-      <c r="DD3" s="21" t="s">
+      <c r="DJ3" s="21" t="s">
         <v>160</v>
       </c>
-      <c r="DF3" s="21" t="s">
+      <c r="DL3" s="21" t="s">
         <v>326</v>
       </c>
-      <c r="DG3" s="21" t="s">
+      <c r="DM3" s="21" t="s">
         <v>327</v>
       </c>
-      <c r="DH3" s="21">
+      <c r="DN3" s="21">
         <v>3028976789</v>
       </c>
-      <c r="DI3" s="21" t="s">
-        <v>137</v>
-      </c>
-      <c r="DJ3" s="21" t="s">
+      <c r="DO3" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="DP3" s="21" t="s">
         <v>246</v>
       </c>
-      <c r="DK3" s="21" t="s">
+      <c r="DQ3" s="21" t="s">
         <v>123</v>
       </c>
-      <c r="DL3" s="21" t="s">
+      <c r="DR3" s="21" t="s">
         <v>122</v>
       </c>
-      <c r="DM3" s="21" t="s">
+      <c r="DS3" s="21" t="s">
         <v>124</v>
       </c>
-      <c r="DN3" s="21" t="s">
+      <c r="DT3" s="21" t="s">
         <v>121</v>
       </c>
-      <c r="DO3" s="21" t="s">
+      <c r="DU3" s="21" t="s">
         <v>125</v>
       </c>
-      <c r="DP3" s="21" t="s">
+      <c r="DV3" s="21" t="s">
         <v>120</v>
       </c>
-      <c r="DQ3" s="21" t="s">
+      <c r="DW3" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="DR3" s="21" t="s">
+      <c r="DX3" s="21" t="s">
         <v>119</v>
       </c>
-      <c r="DS3" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="DT3" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="DU3" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="DV3" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="DW3" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="DX3" s="21" t="s">
-        <v>0</v>
-      </c>
       <c r="DY3" s="21" t="s">
         <v>0</v>
       </c>
@@ -3072,26 +3123,44 @@
       <c r="ED3" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="EE3" s="27" t="s">
+      <c r="EE3" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="EF3" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="EG3" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="EH3" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="EI3" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="EJ3" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="EK3" s="27" t="s">
         <v>425</v>
       </c>
-      <c r="EF3" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="EG3" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="EH3" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="EI3" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="EJ3" s="21" t="s">
+      <c r="EL3" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="EM3" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="EN3" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="EO3" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="EP3" s="21" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:140" s="21" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:146" s="21" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A4" s="21" t="s">
         <v>38</v>
       </c>
@@ -3119,204 +3188,190 @@
       <c r="R4" s="22" t="s">
         <v>420</v>
       </c>
-      <c r="S4" s="21" t="s">
-        <v>148</v>
-      </c>
-      <c r="T4" s="21" t="s">
+      <c r="S4" s="22"/>
+      <c r="T4" s="22"/>
+      <c r="U4" s="21" t="s">
+        <v>148</v>
+      </c>
+      <c r="V4" s="21" t="s">
         <v>166</v>
       </c>
-      <c r="V4" s="21" t="s">
+      <c r="X4" s="21" t="s">
         <v>168</v>
       </c>
-      <c r="X4" s="21" t="s">
-        <v>137</v>
-      </c>
-      <c r="Y4" s="21" t="s">
+      <c r="Z4" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="AB4" s="21" t="s">
         <v>330</v>
       </c>
-      <c r="AE4" s="19" t="s">
+      <c r="AH4" s="19" t="s">
         <v>147</v>
       </c>
-      <c r="AF4" s="18" t="s">
+      <c r="AI4" s="18" t="s">
         <v>147</v>
       </c>
-      <c r="AG4" s="21">
+      <c r="AJ4" s="18"/>
+      <c r="AK4" s="18"/>
+      <c r="AL4" s="21">
         <v>3015774089</v>
       </c>
-      <c r="AH4" s="21">
+      <c r="AM4" s="21">
         <v>3014524258</v>
       </c>
-      <c r="AI4" s="21">
+      <c r="AN4" s="21">
         <v>3015567865</v>
       </c>
-      <c r="AJ4" s="21">
+      <c r="AO4" s="21">
         <v>3015567865</v>
       </c>
-      <c r="AK4" s="21" t="s">
-        <v>148</v>
-      </c>
-      <c r="AL4" s="21" t="s">
+      <c r="AP4" s="21" t="s">
+        <v>148</v>
+      </c>
+      <c r="AQ4" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="AS4" s="21" t="s">
+      <c r="AX4" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="AT4" s="21" t="s">
-        <v>137</v>
-      </c>
-      <c r="BG4" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="BH4" s="21" t="s">
-        <v>148</v>
-      </c>
-      <c r="BK4" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="BL4" s="21" t="s">
+      <c r="AZ4" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="BM4" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="BN4" s="21" t="s">
+        <v>148</v>
+      </c>
+      <c r="BQ4" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="BR4" s="21" t="s">
         <v>171</v>
       </c>
-      <c r="BP4" s="21" t="s">
+      <c r="BV4" s="21" t="s">
         <v>66</v>
       </c>
-      <c r="BS4" s="21" t="s">
+      <c r="BY4" s="21" t="s">
         <v>172</v>
       </c>
-      <c r="BT4" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="BU4" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="BY4" s="21" t="s">
+      <c r="BZ4" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="CA4" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="CE4" s="21" t="s">
         <v>432</v>
       </c>
-      <c r="BZ4" s="21" t="s">
+      <c r="CF4" s="21" t="s">
         <v>75</v>
       </c>
-      <c r="CA4" s="21" t="s">
-        <v>148</v>
-      </c>
-      <c r="CB4" s="21" t="s">
+      <c r="CG4" s="21" t="s">
+        <v>148</v>
+      </c>
+      <c r="CH4" s="21" t="s">
         <v>74</v>
       </c>
-      <c r="CC4" s="21" t="s">
-        <v>148</v>
-      </c>
-      <c r="CD4" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="CE4" s="21" t="s">
+      <c r="CI4" s="21" t="s">
+        <v>148</v>
+      </c>
+      <c r="CJ4" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="CK4" s="21" t="s">
         <v>172</v>
       </c>
-      <c r="CF4" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="CG4" s="21" t="s">
+      <c r="CL4" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="CM4" s="21" t="s">
         <v>173</v>
       </c>
-      <c r="CK4" s="21" t="s">
+      <c r="CQ4" s="21" t="s">
         <v>173</v>
       </c>
-      <c r="CL4" s="21" t="s">
+      <c r="CR4" s="21" t="s">
         <v>76</v>
       </c>
-      <c r="CM4" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="CN4" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="CO4" s="21" t="s">
-        <v>148</v>
-      </c>
-      <c r="CR4" s="21" t="s">
+      <c r="CS4" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="CT4" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="CU4" s="21" t="s">
+        <v>148</v>
+      </c>
+      <c r="CX4" s="21" t="s">
         <v>80</v>
       </c>
-      <c r="CS4" s="21" t="s">
+      <c r="CY4" s="21" t="s">
         <v>82</v>
       </c>
-      <c r="CT4" s="21" t="s">
+      <c r="CZ4" s="21" t="s">
         <v>173</v>
       </c>
-      <c r="CX4" s="21" t="s">
+      <c r="DD4" s="21" t="s">
         <v>174</v>
       </c>
-      <c r="CY4" s="21" t="s">
+      <c r="DE4" s="21" t="s">
         <v>363</v>
       </c>
-      <c r="CZ4" s="21" t="s">
+      <c r="DF4" s="21" t="s">
         <v>175</v>
       </c>
-      <c r="DA4" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="DB4" s="21" t="s">
+      <c r="DG4" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="DH4" s="21" t="s">
         <v>109</v>
       </c>
-      <c r="DC4" s="21" t="s">
+      <c r="DI4" s="21" t="s">
         <v>111</v>
       </c>
-      <c r="DD4" s="23" t="s">
+      <c r="DJ4" s="23" t="s">
         <v>178</v>
       </c>
-      <c r="DF4" s="21" t="s">
+      <c r="DL4" s="21" t="s">
         <v>326</v>
       </c>
-      <c r="DG4" s="21" t="s">
+      <c r="DM4" s="21" t="s">
         <v>327</v>
       </c>
-      <c r="DH4" s="21">
+      <c r="DN4" s="21">
         <v>3028976789</v>
       </c>
-      <c r="DI4" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="DJ4" s="21" t="s">
+      <c r="DO4" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="DP4" s="21" t="s">
         <v>246</v>
       </c>
-      <c r="DK4" s="21" t="s">
+      <c r="DQ4" s="21" t="s">
         <v>123</v>
       </c>
-      <c r="DL4" s="21" t="s">
+      <c r="DR4" s="21" t="s">
         <v>122</v>
       </c>
-      <c r="DM4" s="21" t="s">
+      <c r="DS4" s="21" t="s">
         <v>124</v>
       </c>
-      <c r="DN4" s="21" t="s">
+      <c r="DT4" s="21" t="s">
         <v>121</v>
       </c>
-      <c r="DO4" s="21" t="s">
+      <c r="DU4" s="21" t="s">
         <v>125</v>
       </c>
-      <c r="DP4" s="21" t="s">
+      <c r="DV4" s="21" t="s">
         <v>120</v>
       </c>
-      <c r="DQ4" s="21" t="s">
+      <c r="DW4" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="DR4" s="21" t="s">
+      <c r="DX4" s="21" t="s">
         <v>119</v>
       </c>
-      <c r="DS4" s="21" t="s">
-        <v>137</v>
-      </c>
-      <c r="DT4" s="21" t="s">
-        <v>137</v>
-      </c>
-      <c r="DU4" s="21" t="s">
-        <v>137</v>
-      </c>
-      <c r="DV4" s="21" t="s">
-        <v>137</v>
-      </c>
-      <c r="DW4" s="21" t="s">
-        <v>137</v>
-      </c>
-      <c r="DX4" s="21" t="s">
-        <v>137</v>
-      </c>
       <c r="DY4" s="21" t="s">
         <v>137</v>
       </c>
@@ -3335,26 +3390,44 @@
       <c r="ED4" s="21" t="s">
         <v>137</v>
       </c>
-      <c r="EE4" s="27" t="s">
+      <c r="EE4" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="EF4" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="EG4" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="EH4" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="EI4" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="EJ4" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="EK4" s="27" t="s">
         <v>425</v>
       </c>
-      <c r="EF4" s="21" t="s">
-        <v>137</v>
-      </c>
-      <c r="EG4" s="21" t="s">
-        <v>137</v>
-      </c>
-      <c r="EH4" s="21" t="s">
-        <v>137</v>
-      </c>
-      <c r="EI4" s="21" t="s">
-        <v>137</v>
-      </c>
-      <c r="EJ4" s="21" t="s">
+      <c r="EL4" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="EM4" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="EN4" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="EO4" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="EP4" s="21" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="5" spans="1:140" s="21" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:146" s="21" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A5" s="21" t="s">
         <v>38</v>
       </c>
@@ -3382,213 +3455,199 @@
       <c r="R5" s="22" t="s">
         <v>421</v>
       </c>
-      <c r="S5" s="21" t="s">
+      <c r="S5" s="22"/>
+      <c r="T5" s="22"/>
+      <c r="U5" s="21" t="s">
         <v>170</v>
-      </c>
-      <c r="T5" s="21" t="s">
-        <v>183</v>
-      </c>
-      <c r="U5" s="21" t="s">
-        <v>329</v>
       </c>
       <c r="V5" s="21" t="s">
         <v>183</v>
       </c>
       <c r="W5" s="21" t="s">
+        <v>329</v>
+      </c>
+      <c r="X5" s="21" t="s">
+        <v>183</v>
+      </c>
+      <c r="Y5" s="21" t="s">
         <v>202</v>
       </c>
-      <c r="X5" s="21" t="s">
-        <v>137</v>
-      </c>
-      <c r="Y5" s="21" t="s">
+      <c r="Z5" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="AB5" s="21" t="s">
         <v>182</v>
       </c>
-      <c r="AE5" s="19" t="s">
+      <c r="AH5" s="19" t="s">
         <v>165</v>
       </c>
-      <c r="AF5" s="19" t="s">
+      <c r="AI5" s="19" t="s">
         <v>165</v>
       </c>
-      <c r="AG5" s="21">
+      <c r="AJ5" s="19"/>
+      <c r="AK5" s="19"/>
+      <c r="AL5" s="21">
         <v>3015774089</v>
       </c>
-      <c r="AH5" s="21">
+      <c r="AM5" s="21">
         <v>3014524258</v>
       </c>
-      <c r="AI5" s="21">
+      <c r="AN5" s="21">
         <v>3015567865</v>
       </c>
-      <c r="AJ5" s="21">
+      <c r="AO5" s="21">
         <v>3015567865</v>
       </c>
-      <c r="AK5" s="21" t="s">
-        <v>148</v>
-      </c>
-      <c r="AL5" s="21" t="s">
-        <v>148</v>
-      </c>
-      <c r="AT5" s="21" t="s">
-        <v>137</v>
-      </c>
-      <c r="BG5" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="BH5" s="21" t="s">
-        <v>148</v>
-      </c>
-      <c r="BK5" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="BL5" s="21" t="s">
+      <c r="AP5" s="21" t="s">
+        <v>148</v>
+      </c>
+      <c r="AQ5" s="21" t="s">
+        <v>148</v>
+      </c>
+      <c r="AZ5" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="BM5" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="BN5" s="21" t="s">
+        <v>148</v>
+      </c>
+      <c r="BQ5" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="BR5" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="BM5" s="21" t="s">
+      <c r="BS5" s="21" t="s">
         <v>187</v>
       </c>
-      <c r="BP5" s="21" t="s">
+      <c r="BV5" s="21" t="s">
         <v>66</v>
       </c>
-      <c r="BS5" s="21" t="s">
+      <c r="BY5" s="21" t="s">
         <v>67</v>
       </c>
-      <c r="BT5" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="BU5" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="BY5" s="21" t="s">
+      <c r="BZ5" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="CA5" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="CE5" s="21" t="s">
         <v>432</v>
       </c>
-      <c r="BZ5" s="21" t="s">
+      <c r="CF5" s="21" t="s">
         <v>75</v>
       </c>
-      <c r="CA5" s="21" t="s">
-        <v>148</v>
-      </c>
-      <c r="CB5" s="21" t="s">
+      <c r="CG5" s="21" t="s">
+        <v>148</v>
+      </c>
+      <c r="CH5" s="21" t="s">
         <v>74</v>
       </c>
-      <c r="CC5" s="21" t="s">
-        <v>148</v>
-      </c>
-      <c r="CD5" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="CE5" s="21" t="s">
+      <c r="CI5" s="21" t="s">
+        <v>148</v>
+      </c>
+      <c r="CJ5" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="CK5" s="21" t="s">
         <v>172</v>
       </c>
-      <c r="CF5" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="CG5" s="21" t="s">
+      <c r="CL5" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="CM5" s="21" t="s">
         <v>173</v>
       </c>
-      <c r="CK5" s="21" t="s">
+      <c r="CQ5" s="21" t="s">
         <v>173</v>
       </c>
-      <c r="CL5" s="21" t="s">
+      <c r="CR5" s="21" t="s">
         <v>76</v>
       </c>
-      <c r="CM5" s="21" t="s">
-        <v>137</v>
-      </c>
-      <c r="CN5" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="CO5" s="21" t="s">
+      <c r="CS5" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="CT5" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="CU5" s="21" t="s">
         <v>149</v>
       </c>
-      <c r="CP5" s="22" t="s">
+      <c r="CV5" s="22" t="s">
         <v>361</v>
       </c>
-      <c r="CR5" s="21" t="s">
+      <c r="CX5" s="21" t="s">
         <v>80</v>
       </c>
-      <c r="CS5" s="21" t="s">
+      <c r="CY5" s="21" t="s">
         <v>82</v>
       </c>
-      <c r="CT5" s="21" t="s">
+      <c r="CZ5" s="21" t="s">
         <v>173</v>
       </c>
-      <c r="CX5" s="21" t="s">
+      <c r="DD5" s="21" t="s">
         <v>363</v>
       </c>
-      <c r="CY5" s="21" t="s">
+      <c r="DE5" s="21" t="s">
         <v>363</v>
       </c>
-      <c r="CZ5" s="21" t="s">
+      <c r="DF5" s="21" t="s">
         <v>363</v>
       </c>
-      <c r="DA5" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="DB5" s="21" t="s">
+      <c r="DG5" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="DH5" s="21" t="s">
         <v>159</v>
       </c>
-      <c r="DD5" s="21" t="s">
+      <c r="DJ5" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="DE5" s="21" t="s">
+      <c r="DK5" s="21" t="s">
         <v>356</v>
       </c>
-      <c r="DF5" s="21" t="s">
+      <c r="DL5" s="21" t="s">
         <v>326</v>
       </c>
-      <c r="DG5" s="21" t="s">
+      <c r="DM5" s="21" t="s">
         <v>327</v>
       </c>
-      <c r="DH5" s="21">
+      <c r="DN5" s="21">
         <v>3028976789</v>
       </c>
-      <c r="DI5" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="DJ5" s="21" t="s">
+      <c r="DO5" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="DP5" s="21" t="s">
         <v>246</v>
       </c>
-      <c r="DK5" s="21" t="s">
+      <c r="DQ5" s="21" t="s">
         <v>123</v>
       </c>
-      <c r="DL5" s="21" t="s">
+      <c r="DR5" s="21" t="s">
         <v>122</v>
       </c>
-      <c r="DM5" s="21" t="s">
+      <c r="DS5" s="21" t="s">
         <v>124</v>
       </c>
-      <c r="DN5" s="21" t="s">
+      <c r="DT5" s="21" t="s">
         <v>121</v>
       </c>
-      <c r="DO5" s="21" t="s">
+      <c r="DU5" s="21" t="s">
         <v>125</v>
       </c>
-      <c r="DP5" s="21" t="s">
+      <c r="DV5" s="21" t="s">
         <v>120</v>
       </c>
-      <c r="DQ5" s="21" t="s">
+      <c r="DW5" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="DR5" s="21" t="s">
+      <c r="DX5" s="21" t="s">
         <v>119</v>
       </c>
-      <c r="DS5" s="21" t="s">
-        <v>148</v>
-      </c>
-      <c r="DT5" s="21" t="s">
-        <v>148</v>
-      </c>
-      <c r="DU5" s="21" t="s">
-        <v>148</v>
-      </c>
-      <c r="DV5" s="21" t="s">
-        <v>148</v>
-      </c>
-      <c r="DW5" s="21" t="s">
-        <v>148</v>
-      </c>
-      <c r="DX5" s="21" t="s">
-        <v>148</v>
-      </c>
       <c r="DY5" s="21" t="s">
         <v>148</v>
       </c>
@@ -3607,26 +3666,44 @@
       <c r="ED5" s="21" t="s">
         <v>148</v>
       </c>
-      <c r="EE5" s="27" t="s">
+      <c r="EE5" s="21" t="s">
+        <v>148</v>
+      </c>
+      <c r="EF5" s="21" t="s">
+        <v>148</v>
+      </c>
+      <c r="EG5" s="21" t="s">
+        <v>148</v>
+      </c>
+      <c r="EH5" s="21" t="s">
+        <v>148</v>
+      </c>
+      <c r="EI5" s="21" t="s">
+        <v>148</v>
+      </c>
+      <c r="EJ5" s="21" t="s">
+        <v>148</v>
+      </c>
+      <c r="EK5" s="27" t="s">
         <v>425</v>
       </c>
-      <c r="EF5" s="21" t="s">
-        <v>148</v>
-      </c>
-      <c r="EG5" s="21" t="s">
-        <v>148</v>
-      </c>
-      <c r="EH5" s="21" t="s">
-        <v>148</v>
-      </c>
-      <c r="EI5" s="21" t="s">
-        <v>148</v>
-      </c>
-      <c r="EJ5" s="21" t="s">
+      <c r="EL5" s="21" t="s">
+        <v>148</v>
+      </c>
+      <c r="EM5" s="21" t="s">
+        <v>148</v>
+      </c>
+      <c r="EN5" s="21" t="s">
+        <v>148</v>
+      </c>
+      <c r="EO5" s="21" t="s">
+        <v>148</v>
+      </c>
+      <c r="EP5" s="21" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="6" spans="1:140" s="21" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:146" s="21" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A6" s="21" t="s">
         <v>38</v>
       </c>
@@ -3654,146 +3731,130 @@
       <c r="R6" s="22" t="s">
         <v>409</v>
       </c>
-      <c r="S6" s="21" t="s">
-        <v>148</v>
-      </c>
-      <c r="T6" s="21" t="s">
+      <c r="S6" s="22"/>
+      <c r="T6" s="22"/>
+      <c r="U6" s="21" t="s">
         <v>148</v>
       </c>
       <c r="V6" s="21" t="s">
         <v>148</v>
       </c>
       <c r="X6" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="Y6" s="21" t="s">
+        <v>148</v>
+      </c>
+      <c r="Z6" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="AB6" s="21" t="s">
         <v>364</v>
       </c>
-      <c r="AE6" s="18" t="s">
+      <c r="AH6" s="18" t="s">
         <v>181</v>
       </c>
-      <c r="AF6" s="21" t="s">
+      <c r="AI6" s="21" t="s">
         <v>181</v>
       </c>
-      <c r="AG6" s="21">
+      <c r="AL6" s="21">
         <v>3015774089</v>
       </c>
-      <c r="AH6" s="21">
+      <c r="AM6" s="21">
         <v>3014524258</v>
       </c>
-      <c r="AI6" s="21">
+      <c r="AN6" s="21">
         <v>3015567865</v>
       </c>
-      <c r="AJ6" s="21">
+      <c r="AO6" s="21">
         <v>3015774089</v>
       </c>
-      <c r="AK6" s="21" t="s">
+      <c r="AP6" s="21" t="s">
         <v>170</v>
       </c>
-      <c r="AL6" s="21" t="s">
+      <c r="AQ6" s="21" t="s">
         <v>170</v>
       </c>
-      <c r="AT6" s="21" t="s">
-        <v>148</v>
-      </c>
-      <c r="BG6" s="21" t="s">
-        <v>137</v>
-      </c>
-      <c r="BI6" s="24"/>
-      <c r="BK6" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="BL6" s="21" t="s">
-        <v>148</v>
-      </c>
-      <c r="BP6" s="21" t="s">
+      <c r="AZ6" s="21" t="s">
+        <v>148</v>
+      </c>
+      <c r="BM6" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="BO6" s="24"/>
+      <c r="BQ6" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="BR6" s="21" t="s">
+        <v>148</v>
+      </c>
+      <c r="BV6" s="21" t="s">
         <v>151</v>
       </c>
-      <c r="BS6" s="21" t="s">
+      <c r="BY6" s="21" t="s">
         <v>67</v>
       </c>
-      <c r="BT6" s="21" t="s">
-        <v>148</v>
-      </c>
-      <c r="BY6" s="21" t="s">
+      <c r="BZ6" s="21" t="s">
+        <v>148</v>
+      </c>
+      <c r="CE6" s="21" t="s">
         <v>432</v>
       </c>
-      <c r="CF6" s="21" t="s">
-        <v>148</v>
-      </c>
-      <c r="CP6" s="24"/>
-      <c r="DA6" s="21" t="s">
-        <v>148</v>
-      </c>
-      <c r="DB6" s="21" t="s">
+      <c r="CL6" s="21" t="s">
+        <v>148</v>
+      </c>
+      <c r="CV6" s="24"/>
+      <c r="DG6" s="21" t="s">
+        <v>148</v>
+      </c>
+      <c r="DH6" s="21" t="s">
         <v>109</v>
       </c>
-      <c r="DC6" s="21" t="s">
+      <c r="DI6" s="21" t="s">
         <v>177</v>
       </c>
-      <c r="DD6" s="21" t="s">
+      <c r="DJ6" s="21" t="s">
         <v>357</v>
       </c>
-      <c r="DE6" s="21" t="s">
+      <c r="DK6" s="21" t="s">
         <v>358</v>
       </c>
-      <c r="DF6" s="21" t="s">
+      <c r="DL6" s="21" t="s">
         <v>115</v>
       </c>
-      <c r="DG6" s="21" t="s">
+      <c r="DM6" s="21" t="s">
         <v>117</v>
       </c>
-      <c r="DH6" s="21">
+      <c r="DN6" s="21">
         <v>3028976789</v>
       </c>
-      <c r="DI6" s="21" t="s">
-        <v>137</v>
-      </c>
-      <c r="DJ6" s="21" t="s">
+      <c r="DO6" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="DP6" s="21" t="s">
         <v>246</v>
       </c>
-      <c r="DK6" s="21" t="s">
+      <c r="DQ6" s="21" t="s">
         <v>123</v>
       </c>
-      <c r="DL6" s="21" t="s">
+      <c r="DR6" s="21" t="s">
         <v>122</v>
       </c>
-      <c r="DM6" s="21" t="s">
+      <c r="DS6" s="21" t="s">
         <v>124</v>
       </c>
-      <c r="DN6" s="21" t="s">
+      <c r="DT6" s="21" t="s">
         <v>121</v>
       </c>
-      <c r="DO6" s="21" t="s">
+      <c r="DU6" s="21" t="s">
         <v>125</v>
       </c>
-      <c r="DP6" s="21" t="s">
+      <c r="DV6" s="21" t="s">
         <v>120</v>
       </c>
-      <c r="DQ6" s="21" t="s">
+      <c r="DW6" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="DR6" s="21" t="s">
+      <c r="DX6" s="21" t="s">
         <v>119</v>
       </c>
-      <c r="DS6" s="21" t="s">
-        <v>137</v>
-      </c>
-      <c r="DT6" s="21" t="s">
-        <v>137</v>
-      </c>
-      <c r="DU6" s="21" t="s">
-        <v>137</v>
-      </c>
-      <c r="DV6" s="21" t="s">
-        <v>137</v>
-      </c>
-      <c r="DW6" s="21" t="s">
-        <v>137</v>
-      </c>
-      <c r="DX6" s="21" t="s">
-        <v>137</v>
-      </c>
       <c r="DY6" s="21" t="s">
         <v>137</v>
       </c>
@@ -3812,26 +3873,44 @@
       <c r="ED6" s="21" t="s">
         <v>137</v>
       </c>
-      <c r="EE6" s="27" t="s">
+      <c r="EE6" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="EF6" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="EG6" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="EH6" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="EI6" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="EJ6" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="EK6" s="27" t="s">
         <v>425</v>
       </c>
-      <c r="EF6" s="21" t="s">
-        <v>137</v>
-      </c>
-      <c r="EG6" s="21" t="s">
-        <v>137</v>
-      </c>
-      <c r="EH6" s="21" t="s">
-        <v>137</v>
-      </c>
-      <c r="EI6" s="21" t="s">
-        <v>137</v>
-      </c>
-      <c r="EJ6" s="21" t="s">
+      <c r="EL6" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="EM6" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="EN6" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="EO6" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="EP6" s="21" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="7" spans="1:140" s="21" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:146" s="21" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A7" s="21" t="s">
         <v>38</v>
       </c>
@@ -3859,161 +3938,147 @@
       <c r="R7" s="22" t="s">
         <v>410</v>
       </c>
-      <c r="S7" s="21" t="s">
-        <v>170</v>
-      </c>
-      <c r="T7" s="21" t="s">
+      <c r="S7" s="22"/>
+      <c r="T7" s="22"/>
+      <c r="U7" s="21" t="s">
         <v>170</v>
       </c>
       <c r="V7" s="21" t="s">
         <v>170</v>
       </c>
       <c r="X7" s="21" t="s">
-        <v>137</v>
-      </c>
-      <c r="Y7" s="21" t="s">
+        <v>170</v>
+      </c>
+      <c r="Z7" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="AB7" s="21" t="s">
         <v>186</v>
       </c>
-      <c r="AE7" s="18" t="s">
+      <c r="AH7" s="18" t="s">
         <v>323</v>
       </c>
-      <c r="AF7" s="18" t="s">
+      <c r="AI7" s="18" t="s">
         <v>323</v>
       </c>
-      <c r="AG7" s="21">
+      <c r="AJ7" s="18"/>
+      <c r="AK7" s="18"/>
+      <c r="AL7" s="21">
         <v>3015774089</v>
       </c>
-      <c r="AH7" s="21">
+      <c r="AM7" s="21">
         <v>3014524258</v>
       </c>
-      <c r="AI7" s="21">
+      <c r="AN7" s="21">
         <v>3015567865</v>
       </c>
-      <c r="AJ7" s="21">
+      <c r="AO7" s="21">
         <v>3014524258</v>
       </c>
-      <c r="AK7" s="21" t="s">
+      <c r="AP7" s="21" t="s">
         <v>170</v>
       </c>
-      <c r="AL7" s="21" t="s">
+      <c r="AQ7" s="21" t="s">
         <v>170</v>
       </c>
-      <c r="AT7" s="21" t="s">
-        <v>137</v>
-      </c>
-      <c r="BG7" s="21" t="s">
-        <v>137</v>
-      </c>
-      <c r="BI7" s="24"/>
-      <c r="BK7" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="BL7" s="21" t="s">
+      <c r="AZ7" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="BM7" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="BO7" s="24"/>
+      <c r="BQ7" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="BR7" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="BM7" s="21" t="s">
+      <c r="BS7" s="21" t="s">
         <v>187</v>
       </c>
-      <c r="BN7" s="21" t="s">
+      <c r="BT7" s="21" t="s">
         <v>365</v>
       </c>
-      <c r="BO7" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="BP7" s="21" t="s">
+      <c r="BU7" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="BV7" s="21" t="s">
         <v>66</v>
       </c>
-      <c r="BS7" s="21" t="s">
+      <c r="BY7" s="21" t="s">
         <v>67</v>
       </c>
-      <c r="BT7" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="BU7" s="21" t="s">
-        <v>137</v>
-      </c>
-      <c r="BV7" s="21" t="s">
+      <c r="BZ7" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="CA7" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="CB7" s="21" t="s">
         <v>369</v>
       </c>
-      <c r="BY7" s="21" t="s">
+      <c r="CE7" s="21" t="s">
         <v>432</v>
       </c>
-      <c r="CD7" s="21" t="s">
-        <v>137</v>
-      </c>
-      <c r="CF7" s="21" t="s">
-        <v>137</v>
-      </c>
-      <c r="CP7" s="24"/>
-      <c r="DA7" s="21" t="s">
-        <v>137</v>
-      </c>
-      <c r="DB7" s="21" t="s">
+      <c r="CJ7" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="CL7" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="CV7" s="24"/>
+      <c r="DG7" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="DH7" s="21" t="s">
         <v>109</v>
       </c>
-      <c r="DC7" s="21" t="s">
+      <c r="DI7" s="21" t="s">
         <v>111</v>
       </c>
-      <c r="DD7" s="21" t="s">
+      <c r="DJ7" s="21" t="s">
         <v>359</v>
       </c>
-      <c r="DF7" s="21" t="s">
+      <c r="DL7" s="21" t="s">
         <v>115</v>
       </c>
-      <c r="DG7" s="21" t="s">
+      <c r="DM7" s="21" t="s">
         <v>117</v>
       </c>
-      <c r="DH7" s="21">
+      <c r="DN7" s="21">
         <v>3028976789</v>
       </c>
-      <c r="DI7" s="21" t="s">
-        <v>137</v>
-      </c>
-      <c r="DJ7" s="21" t="s">
+      <c r="DO7" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="DP7" s="21" t="s">
         <v>246</v>
       </c>
-      <c r="DK7" s="21" t="s">
+      <c r="DQ7" s="21" t="s">
         <v>123</v>
       </c>
-      <c r="DL7" s="21" t="s">
+      <c r="DR7" s="21" t="s">
         <v>122</v>
       </c>
-      <c r="DM7" s="21" t="s">
+      <c r="DS7" s="21" t="s">
         <v>124</v>
       </c>
-      <c r="DN7" s="21" t="s">
+      <c r="DT7" s="21" t="s">
         <v>121</v>
       </c>
-      <c r="DO7" s="21" t="s">
+      <c r="DU7" s="21" t="s">
         <v>125</v>
       </c>
-      <c r="DP7" s="21" t="s">
+      <c r="DV7" s="21" t="s">
         <v>120</v>
       </c>
-      <c r="DQ7" s="21" t="s">
+      <c r="DW7" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="DR7" s="21" t="s">
+      <c r="DX7" s="21" t="s">
         <v>119</v>
       </c>
-      <c r="DS7" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="DT7" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="DU7" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="DV7" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="DW7" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="DX7" s="21" t="s">
-        <v>0</v>
-      </c>
       <c r="DY7" s="21" t="s">
         <v>0</v>
       </c>
@@ -4032,26 +4097,44 @@
       <c r="ED7" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="EE7" s="27" t="s">
+      <c r="EE7" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="EF7" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="EG7" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="EH7" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="EI7" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="EJ7" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="EK7" s="27" t="s">
         <v>425</v>
       </c>
-      <c r="EF7" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="EG7" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="EH7" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="EI7" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="EJ7" s="21" t="s">
+      <c r="EL7" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="EM7" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="EN7" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="EO7" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="EP7" s="21" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:140" s="21" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:146" s="21" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A8" s="21" t="s">
         <v>38</v>
       </c>
@@ -4079,149 +4162,135 @@
       <c r="R8" s="22" t="s">
         <v>407</v>
       </c>
-      <c r="S8" s="21" t="s">
-        <v>148</v>
-      </c>
-      <c r="T8" s="21" t="s">
+      <c r="S8" s="22"/>
+      <c r="T8" s="22"/>
+      <c r="U8" s="21" t="s">
+        <v>148</v>
+      </c>
+      <c r="V8" s="21" t="s">
         <v>170</v>
       </c>
-      <c r="V8" s="21" t="s">
-        <v>148</v>
-      </c>
       <c r="X8" s="21" t="s">
-        <v>137</v>
-      </c>
-      <c r="Y8" s="21" t="s">
+        <v>148</v>
+      </c>
+      <c r="Z8" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="AB8" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="Z8" s="21" t="s">
+      <c r="AC8" s="21" t="s">
         <v>199</v>
       </c>
-      <c r="AA8" s="21" t="s">
+      <c r="AD8" s="21" t="s">
         <v>200</v>
       </c>
-      <c r="AB8" s="21" t="s">
+      <c r="AE8" s="21" t="s">
         <v>201</v>
       </c>
-      <c r="AC8" s="21" t="s">
+      <c r="AF8" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="AD8" s="21">
+      <c r="AG8" s="21">
         <v>28907</v>
       </c>
-      <c r="AE8" s="18" t="s">
+      <c r="AH8" s="18" t="s">
         <v>324</v>
       </c>
-      <c r="AF8" s="18" t="s">
+      <c r="AI8" s="18" t="s">
         <v>324</v>
       </c>
-      <c r="AG8" s="21">
+      <c r="AJ8" s="18"/>
+      <c r="AK8" s="18"/>
+      <c r="AL8" s="21">
         <v>3015774089</v>
       </c>
-      <c r="AH8" s="21">
+      <c r="AM8" s="21">
         <v>3014524258</v>
       </c>
-      <c r="AI8" s="21">
+      <c r="AN8" s="21">
         <v>3015567865</v>
       </c>
-      <c r="AJ8" s="21">
+      <c r="AO8" s="21">
         <v>3015567865</v>
       </c>
-      <c r="AK8" s="21" t="s">
-        <v>148</v>
-      </c>
-      <c r="AL8" s="21" t="s">
+      <c r="AP8" s="21" t="s">
+        <v>148</v>
+      </c>
+      <c r="AQ8" s="21" t="s">
         <v>170</v>
       </c>
-      <c r="AT8" s="21" t="s">
-        <v>137</v>
-      </c>
-      <c r="BG8" s="21" t="s">
-        <v>137</v>
-      </c>
-      <c r="BJ8" s="24"/>
-      <c r="BK8" s="21" t="s">
-        <v>137</v>
-      </c>
-      <c r="BT8" s="21" t="s">
-        <v>137</v>
-      </c>
-      <c r="BY8" s="21" t="s">
+      <c r="AZ8" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="BM8" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="BP8" s="24"/>
+      <c r="BQ8" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="BZ8" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="CE8" s="21" t="s">
         <v>432</v>
       </c>
-      <c r="CF8" s="21" t="s">
-        <v>137</v>
-      </c>
-      <c r="CP8" s="24"/>
-      <c r="DA8" s="21" t="s">
-        <v>137</v>
-      </c>
-      <c r="DB8" s="21" t="s">
+      <c r="CL8" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="CV8" s="24"/>
+      <c r="DG8" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="DH8" s="21" t="s">
         <v>159</v>
       </c>
-      <c r="DD8" s="21" t="s">
+      <c r="DJ8" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="DE8" s="21" t="s">
+      <c r="DK8" s="21" t="s">
         <v>360</v>
       </c>
-      <c r="DF8" s="21" t="s">
+      <c r="DL8" s="21" t="s">
         <v>115</v>
       </c>
-      <c r="DG8" s="21" t="s">
+      <c r="DM8" s="21" t="s">
         <v>117</v>
       </c>
-      <c r="DH8" s="21">
+      <c r="DN8" s="21">
         <v>3028976789</v>
       </c>
-      <c r="DI8" s="21" t="s">
-        <v>137</v>
-      </c>
-      <c r="DJ8" s="21" t="s">
+      <c r="DO8" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="DP8" s="21" t="s">
         <v>246</v>
       </c>
-      <c r="DK8" s="21" t="s">
+      <c r="DQ8" s="21" t="s">
         <v>123</v>
       </c>
-      <c r="DL8" s="21" t="s">
+      <c r="DR8" s="21" t="s">
         <v>122</v>
       </c>
-      <c r="DM8" s="21" t="s">
+      <c r="DS8" s="21" t="s">
         <v>124</v>
       </c>
-      <c r="DN8" s="21" t="s">
+      <c r="DT8" s="21" t="s">
         <v>121</v>
       </c>
-      <c r="DO8" s="21" t="s">
+      <c r="DU8" s="21" t="s">
         <v>125</v>
       </c>
-      <c r="DP8" s="21" t="s">
+      <c r="DV8" s="21" t="s">
         <v>120</v>
       </c>
-      <c r="DQ8" s="21" t="s">
+      <c r="DW8" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="DR8" s="21" t="s">
+      <c r="DX8" s="21" t="s">
         <v>119</v>
       </c>
-      <c r="DS8" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="DT8" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="DU8" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="DV8" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="DW8" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="DX8" s="21" t="s">
-        <v>0</v>
-      </c>
       <c r="DY8" s="21" t="s">
         <v>0</v>
       </c>
@@ -4240,26 +4309,44 @@
       <c r="ED8" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="EE8" s="27" t="s">
+      <c r="EE8" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="EF8" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="EG8" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="EH8" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="EI8" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="EJ8" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="EK8" s="27" t="s">
         <v>425</v>
       </c>
-      <c r="EF8" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="EG8" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="EH8" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="EI8" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="EJ8" s="21" t="s">
+      <c r="EL8" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="EM8" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="EN8" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="EO8" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="EP8" s="21" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:140" s="21" customFormat="1" ht="68" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:146" s="21" customFormat="1" ht="68" x14ac:dyDescent="0.2">
       <c r="A9" s="21" t="s">
         <v>38</v>
       </c>
@@ -4287,214 +4374,200 @@
       <c r="R9" s="22" t="s">
         <v>408</v>
       </c>
-      <c r="S9" s="21" t="s">
+      <c r="S9" s="22"/>
+      <c r="T9" s="22"/>
+      <c r="U9" s="21" t="s">
         <v>170</v>
       </c>
-      <c r="T9" s="21" t="s">
+      <c r="V9" s="21" t="s">
         <v>166</v>
       </c>
-      <c r="V9" s="21" t="s">
+      <c r="X9" s="21" t="s">
         <v>168</v>
       </c>
-      <c r="X9" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="Y9" s="21" t="s">
+      <c r="Z9" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="AB9" s="21" t="s">
         <v>381</v>
       </c>
-      <c r="AE9" s="18" t="s">
+      <c r="AH9" s="18" t="s">
         <v>325</v>
       </c>
-      <c r="AF9" s="18" t="s">
+      <c r="AI9" s="18" t="s">
         <v>325</v>
       </c>
-      <c r="AG9" s="21">
+      <c r="AJ9" s="18"/>
+      <c r="AK9" s="18"/>
+      <c r="AL9" s="21">
         <v>3015774089</v>
       </c>
-      <c r="AH9" s="21">
+      <c r="AM9" s="21">
         <v>3014524258</v>
       </c>
-      <c r="AI9" s="21">
+      <c r="AN9" s="21">
         <v>3015567865</v>
       </c>
-      <c r="AJ9" s="21">
+      <c r="AO9" s="21">
         <v>3015567865</v>
       </c>
-      <c r="AK9" s="21" t="s">
-        <v>148</v>
-      </c>
-      <c r="AL9" s="21" t="s">
-        <v>148</v>
-      </c>
-      <c r="AT9" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="AU9" s="21" t="s">
+      <c r="AP9" s="21" t="s">
+        <v>148</v>
+      </c>
+      <c r="AQ9" s="21" t="s">
+        <v>148</v>
+      </c>
+      <c r="AZ9" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="BA9" s="21" t="s">
         <v>304</v>
       </c>
-      <c r="AV9" s="21" t="s">
+      <c r="BB9" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="AW9" s="21" t="s">
+      <c r="BC9" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="AX9" s="21" t="s">
+      <c r="BD9" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="AY9" s="21" t="s">
+      <c r="BE9" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="AZ9" s="21" t="s">
+      <c r="BF9" s="21" t="s">
         <v>56</v>
       </c>
-      <c r="BA9" s="21" t="s">
+      <c r="BG9" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="BB9" s="21" t="s">
+      <c r="BH9" s="21" t="s">
         <v>57</v>
       </c>
-      <c r="BC9" s="21" t="s">
+      <c r="BI9" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="BD9" s="21" t="s">
+      <c r="BJ9" s="21" t="s">
         <v>58</v>
       </c>
-      <c r="BE9" s="21" t="s">
+      <c r="BK9" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="BF9" s="21" t="s">
+      <c r="BL9" s="21" t="s">
         <v>59</v>
       </c>
-      <c r="BG9" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="BH9" s="21" t="s">
+      <c r="BM9" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="BN9" s="21" t="s">
         <v>64</v>
       </c>
-      <c r="BJ9" s="21">
+      <c r="BP9" s="21">
         <v>119</v>
       </c>
-      <c r="BK9" s="21" t="s">
-        <v>148</v>
-      </c>
-      <c r="BT9" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="BU9" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="BY9" s="21" t="s">
+      <c r="BQ9" s="21" t="s">
+        <v>148</v>
+      </c>
+      <c r="BZ9" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="CA9" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="CE9" s="21" t="s">
         <v>432</v>
       </c>
-      <c r="BZ9" s="21" t="s">
+      <c r="CF9" s="21" t="s">
         <v>75</v>
       </c>
-      <c r="CA9" s="21" t="s">
-        <v>148</v>
-      </c>
-      <c r="CB9" s="21" t="s">
+      <c r="CG9" s="21" t="s">
+        <v>148</v>
+      </c>
+      <c r="CH9" s="21" t="s">
         <v>74</v>
       </c>
-      <c r="CC9" s="21" t="s">
-        <v>148</v>
-      </c>
-      <c r="CD9" s="21" t="s">
-        <v>148</v>
-      </c>
-      <c r="CF9" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="CG9" s="21" t="s">
+      <c r="CI9" s="21" t="s">
+        <v>148</v>
+      </c>
+      <c r="CJ9" s="21" t="s">
+        <v>148</v>
+      </c>
+      <c r="CL9" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="CM9" s="21" t="s">
         <v>79</v>
       </c>
-      <c r="CJ9" s="21">
+      <c r="CP9" s="21">
         <v>102</v>
       </c>
-      <c r="CK9" s="21" t="s">
-        <v>137</v>
-      </c>
-      <c r="CL9" s="21" t="s">
+      <c r="CQ9" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="CR9" s="21" t="s">
         <v>383</v>
       </c>
-      <c r="CM9" s="21" t="s">
-        <v>137</v>
-      </c>
-      <c r="CN9" s="21" t="s">
-        <v>137</v>
-      </c>
-      <c r="CP9" s="24"/>
-      <c r="CR9" s="21" t="s">
-        <v>137</v>
-      </c>
-      <c r="DA9" s="21" t="s">
-        <v>137</v>
-      </c>
-      <c r="DB9" s="21" t="s">
+      <c r="CS9" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="CT9" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="CV9" s="24"/>
+      <c r="CX9" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="DG9" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="DH9" s="21" t="s">
         <v>109</v>
       </c>
-      <c r="DC9" s="21" t="s">
+      <c r="DI9" s="21" t="s">
         <v>111</v>
       </c>
-      <c r="DD9" s="23" t="s">
+      <c r="DJ9" s="23" t="s">
         <v>178</v>
       </c>
-      <c r="DF9" s="21" t="s">
+      <c r="DL9" s="21" t="s">
         <v>115</v>
       </c>
-      <c r="DG9" s="21" t="s">
+      <c r="DM9" s="21" t="s">
         <v>117</v>
       </c>
-      <c r="DH9" s="21">
+      <c r="DN9" s="21">
         <v>3028976789</v>
       </c>
-      <c r="DI9" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="DJ9" s="21" t="s">
+      <c r="DO9" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="DP9" s="21" t="s">
         <v>246</v>
       </c>
-      <c r="DK9" s="21" t="s">
+      <c r="DQ9" s="21" t="s">
         <v>123</v>
       </c>
-      <c r="DL9" s="21" t="s">
+      <c r="DR9" s="21" t="s">
         <v>122</v>
       </c>
-      <c r="DM9" s="21" t="s">
+      <c r="DS9" s="21" t="s">
         <v>124</v>
       </c>
-      <c r="DN9" s="21" t="s">
+      <c r="DT9" s="21" t="s">
         <v>121</v>
       </c>
-      <c r="DO9" s="21" t="s">
+      <c r="DU9" s="21" t="s">
         <v>125</v>
       </c>
-      <c r="DP9" s="21" t="s">
+      <c r="DV9" s="21" t="s">
         <v>120</v>
       </c>
-      <c r="DQ9" s="21" t="s">
+      <c r="DW9" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="DR9" s="21" t="s">
+      <c r="DX9" s="21" t="s">
         <v>119</v>
       </c>
-      <c r="DS9" s="21" t="s">
-        <v>137</v>
-      </c>
-      <c r="DT9" s="21" t="s">
-        <v>137</v>
-      </c>
-      <c r="DU9" s="21" t="s">
-        <v>137</v>
-      </c>
-      <c r="DV9" s="21" t="s">
-        <v>137</v>
-      </c>
-      <c r="DW9" s="21" t="s">
-        <v>137</v>
-      </c>
-      <c r="DX9" s="21" t="s">
-        <v>137</v>
-      </c>
       <c r="DY9" s="21" t="s">
         <v>137</v>
       </c>
@@ -4513,26 +4586,44 @@
       <c r="ED9" s="21" t="s">
         <v>137</v>
       </c>
-      <c r="EE9" s="27" t="s">
+      <c r="EE9" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="EF9" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="EG9" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="EH9" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="EI9" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="EJ9" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="EK9" s="27" t="s">
         <v>425</v>
       </c>
-      <c r="EF9" s="21" t="s">
-        <v>137</v>
-      </c>
-      <c r="EG9" s="21" t="s">
-        <v>137</v>
-      </c>
-      <c r="EH9" s="21" t="s">
-        <v>137</v>
-      </c>
-      <c r="EI9" s="21" t="s">
-        <v>137</v>
-      </c>
-      <c r="EJ9" s="21" t="s">
+      <c r="EL9" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="EM9" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="EN9" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="EO9" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="EP9" s="21" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="10" spans="1:140" s="21" customFormat="1" ht="85" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:146" s="21" customFormat="1" ht="85" x14ac:dyDescent="0.2">
       <c r="A10" s="21" t="s">
         <v>134</v>
       </c>
@@ -4575,295 +4666,281 @@
       <c r="R10" s="22" t="s">
         <v>411</v>
       </c>
-      <c r="S10" s="21" t="s">
+      <c r="S10" s="22"/>
+      <c r="T10" s="22"/>
+      <c r="U10" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="V10" s="26"/>
-      <c r="X10" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="Y10" s="21" t="s">
+      <c r="X10" s="26"/>
+      <c r="Z10" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="AB10" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="Z10" s="21" t="s">
+      <c r="AC10" s="21" t="s">
         <v>199</v>
       </c>
-      <c r="AA10" s="21" t="s">
+      <c r="AD10" s="21" t="s">
         <v>200</v>
       </c>
-      <c r="AB10" s="21" t="s">
+      <c r="AE10" s="21" t="s">
         <v>201</v>
       </c>
-      <c r="AC10" s="21" t="s">
+      <c r="AF10" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="AD10" s="21">
+      <c r="AG10" s="21">
         <v>28907</v>
       </c>
-      <c r="AE10" s="19" t="s">
+      <c r="AH10" s="19" t="s">
         <v>331</v>
       </c>
-      <c r="AF10" s="18" t="s">
+      <c r="AI10" s="18" t="s">
         <v>331</v>
       </c>
-      <c r="AG10" s="21">
+      <c r="AJ10" s="18"/>
+      <c r="AK10" s="18"/>
+      <c r="AL10" s="21">
         <v>3015774089</v>
       </c>
-      <c r="AH10" s="21">
+      <c r="AM10" s="21">
         <v>3014524258</v>
       </c>
-      <c r="AI10" s="21">
+      <c r="AN10" s="21">
         <v>3015567865</v>
       </c>
-      <c r="AJ10" s="21">
+      <c r="AO10" s="21">
         <v>3015774089</v>
       </c>
-      <c r="AK10" s="21" t="s">
+      <c r="AP10" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="AL10" s="21" t="s">
+      <c r="AQ10" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="AM10" s="21" t="s">
+      <c r="AR10" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="AN10" s="21" t="s">
+      <c r="AS10" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="AO10" s="21" t="s">
+      <c r="AT10" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="AP10" s="21" t="s">
+      <c r="AU10" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="AQ10" s="21" t="s">
+      <c r="AV10" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="AR10" s="21" t="s">
+      <c r="AW10" s="21" t="s">
         <v>40</v>
       </c>
-      <c r="AS10" s="21" t="s">
+      <c r="AX10" s="21" t="s">
         <v>192</v>
       </c>
-      <c r="AT10" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="AU10" s="21" t="s">
+      <c r="AZ10" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="BA10" s="21" t="s">
         <v>304</v>
       </c>
-      <c r="AV10" s="21" t="s">
+      <c r="BB10" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="AW10" s="21" t="s">
+      <c r="BC10" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="AX10" s="21" t="s">
+      <c r="BD10" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="AY10" s="21" t="s">
+      <c r="BE10" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="AZ10" s="21" t="s">
+      <c r="BF10" s="21" t="s">
         <v>56</v>
       </c>
-      <c r="BA10" s="21" t="s">
+      <c r="BG10" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="BB10" s="21" t="s">
+      <c r="BH10" s="21" t="s">
         <v>57</v>
       </c>
-      <c r="BC10" s="21" t="s">
+      <c r="BI10" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="BD10" s="21" t="s">
+      <c r="BJ10" s="21" t="s">
         <v>58</v>
       </c>
-      <c r="BE10" s="21" t="s">
+      <c r="BK10" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="BF10" s="21" t="s">
+      <c r="BL10" s="21" t="s">
         <v>59</v>
       </c>
-      <c r="BG10" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="BH10" s="21" t="s">
+      <c r="BM10" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="BN10" s="21" t="s">
         <v>149</v>
       </c>
-      <c r="BI10" s="22" t="s">
+      <c r="BO10" s="22" t="s">
         <v>393</v>
       </c>
-      <c r="BK10" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="BL10" s="21" t="s">
+      <c r="BQ10" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="BR10" s="21" t="s">
         <v>171</v>
       </c>
-      <c r="BP10" s="21" t="s">
+      <c r="BV10" s="21" t="s">
         <v>66</v>
       </c>
-      <c r="BQ10" s="23" t="s">
+      <c r="BW10" s="23" t="s">
         <v>268</v>
       </c>
-      <c r="BR10" s="23" t="s">
+      <c r="BX10" s="23" t="s">
         <v>268</v>
       </c>
-      <c r="BS10" s="21" t="s">
+      <c r="BY10" s="21" t="s">
         <v>67</v>
       </c>
-      <c r="BT10" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="BU10" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="BY10" s="21" t="s">
+      <c r="BZ10" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="CA10" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="CE10" s="21" t="s">
         <v>432</v>
       </c>
-      <c r="BZ10" s="21" t="s">
+      <c r="CF10" s="21" t="s">
         <v>372</v>
       </c>
-      <c r="CA10" s="21" t="s">
+      <c r="CG10" s="21" t="s">
         <v>73</v>
       </c>
-      <c r="CB10" s="21" t="s">
+      <c r="CH10" s="21" t="s">
         <v>373</v>
       </c>
-      <c r="CC10" s="21" t="s">
+      <c r="CI10" s="21" t="s">
         <v>73</v>
       </c>
-      <c r="CD10" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="CE10" s="21" t="s">
+      <c r="CJ10" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="CK10" s="21" t="s">
         <v>67</v>
       </c>
-      <c r="CF10" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="CG10" s="21" t="s">
+      <c r="CL10" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="CM10" s="21" t="s">
         <v>78</v>
       </c>
-      <c r="CH10" s="21" t="s">
+      <c r="CN10" s="21" t="s">
         <v>77</v>
       </c>
-      <c r="CI10" s="21">
+      <c r="CO10" s="21">
         <v>1997</v>
       </c>
-      <c r="CK10" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="CL10" s="21" t="s">
+      <c r="CQ10" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="CR10" s="21" t="s">
         <v>76</v>
       </c>
-      <c r="CM10" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="CN10" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="CO10" s="21" t="s">
+      <c r="CS10" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="CT10" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="CU10" s="21" t="s">
         <v>79</v>
       </c>
-      <c r="CQ10" s="21">
+      <c r="CW10" s="21">
         <v>103</v>
       </c>
-      <c r="CR10" s="21" t="s">
+      <c r="CX10" s="21" t="s">
         <v>374</v>
       </c>
-      <c r="CS10" s="21" t="s">
+      <c r="CY10" s="21" t="s">
         <v>82</v>
       </c>
-      <c r="CT10" s="21" t="s">
+      <c r="CZ10" s="21" t="s">
         <v>78</v>
       </c>
-      <c r="CU10" s="21" t="s">
+      <c r="DA10" s="21" t="s">
         <v>85</v>
       </c>
-      <c r="CV10" s="21">
+      <c r="DB10" s="21">
         <v>1985</v>
       </c>
-      <c r="CX10" s="21" t="s">
+      <c r="DD10" s="21" t="s">
         <v>88</v>
       </c>
-      <c r="CY10" s="21" t="s">
+      <c r="DE10" s="21" t="s">
         <v>89</v>
       </c>
-      <c r="CZ10" s="21" t="s">
+      <c r="DF10" s="21" t="s">
         <v>93</v>
       </c>
-      <c r="DA10" s="21" t="s">
-        <v>137</v>
-      </c>
-      <c r="DB10" s="21" t="s">
+      <c r="DG10" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="DH10" s="21" t="s">
         <v>109</v>
       </c>
-      <c r="DC10" s="21" t="s">
+      <c r="DI10" s="21" t="s">
         <v>111</v>
       </c>
-      <c r="DD10" s="21" t="s">
+      <c r="DJ10" s="21" t="s">
         <v>112</v>
       </c>
-      <c r="DE10" s="21" t="s">
+      <c r="DK10" s="21" t="s">
         <v>113</v>
       </c>
-      <c r="DF10" s="21" t="s">
+      <c r="DL10" s="21" t="s">
         <v>115</v>
       </c>
-      <c r="DG10" s="21" t="s">
+      <c r="DM10" s="21" t="s">
         <v>117</v>
       </c>
-      <c r="DH10" s="21">
+      <c r="DN10" s="21">
         <v>3028976789</v>
       </c>
-      <c r="DI10" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="DJ10" s="21" t="s">
+      <c r="DO10" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="DP10" s="21" t="s">
         <v>246</v>
       </c>
-      <c r="DK10" s="21" t="s">
+      <c r="DQ10" s="21" t="s">
         <v>123</v>
       </c>
-      <c r="DL10" s="21" t="s">
+      <c r="DR10" s="21" t="s">
         <v>122</v>
       </c>
-      <c r="DM10" s="21" t="s">
+      <c r="DS10" s="21" t="s">
         <v>124</v>
       </c>
-      <c r="DN10" s="21" t="s">
+      <c r="DT10" s="21" t="s">
         <v>121</v>
       </c>
-      <c r="DO10" s="21" t="s">
+      <c r="DU10" s="21" t="s">
         <v>125</v>
       </c>
-      <c r="DP10" s="21" t="s">
+      <c r="DV10" s="21" t="s">
         <v>120</v>
       </c>
-      <c r="DQ10" s="21" t="s">
+      <c r="DW10" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="DR10" s="21" t="s">
+      <c r="DX10" s="21" t="s">
         <v>119</v>
       </c>
-      <c r="DS10" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="DT10" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="DU10" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="DV10" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="DW10" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="DX10" s="21" t="s">
-        <v>0</v>
-      </c>
       <c r="DY10" s="21" t="s">
         <v>0</v>
       </c>
@@ -4882,26 +4959,44 @@
       <c r="ED10" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="EE10" s="27" t="s">
+      <c r="EE10" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="EF10" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="EG10" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="EH10" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="EI10" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="EJ10" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="EK10" s="27" t="s">
         <v>425</v>
       </c>
-      <c r="EF10" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="EG10" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="EH10" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="EI10" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="EJ10" s="21" t="s">
+      <c r="EL10" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="EM10" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="EN10" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="EO10" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="EP10" s="21" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:140" s="21" customFormat="1" ht="68" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:146" s="21" customFormat="1" ht="68" x14ac:dyDescent="0.2">
       <c r="A11" s="21" t="s">
         <v>134</v>
       </c>
@@ -4947,197 +5042,183 @@
       <c r="R11" s="22" t="s">
         <v>412</v>
       </c>
-      <c r="S11" s="21" t="s">
+      <c r="S11" s="22"/>
+      <c r="T11" s="22"/>
+      <c r="U11" s="21" t="s">
         <v>144</v>
       </c>
-      <c r="X11" s="21" t="s">
-        <v>137</v>
-      </c>
-      <c r="Y11" s="21" t="s">
+      <c r="Z11" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="AB11" s="21" t="s">
         <v>169</v>
       </c>
-      <c r="AE11" s="18" t="s">
+      <c r="AH11" s="18" t="s">
         <v>332</v>
       </c>
-      <c r="AF11" s="19" t="s">
+      <c r="AI11" s="19" t="s">
         <v>332</v>
       </c>
-      <c r="AG11" s="21">
+      <c r="AJ11" s="19"/>
+      <c r="AK11" s="19"/>
+      <c r="AL11" s="21">
         <v>3015774089</v>
       </c>
-      <c r="AH11" s="21">
+      <c r="AM11" s="21">
         <v>3014524258</v>
       </c>
-      <c r="AI11" s="21">
+      <c r="AN11" s="21">
         <v>3015567865</v>
       </c>
-      <c r="AJ11" s="21">
+      <c r="AO11" s="21">
         <v>3014524258</v>
       </c>
-      <c r="AK11" s="21" t="s">
-        <v>148</v>
-      </c>
-      <c r="AL11" s="21" t="s">
-        <v>148</v>
-      </c>
-      <c r="AT11" s="21" t="s">
-        <v>148</v>
-      </c>
-      <c r="BG11" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="BH11" s="21" t="s">
-        <v>148</v>
-      </c>
-      <c r="BI11" s="24"/>
-      <c r="BK11" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="BL11" s="21" t="s">
+      <c r="AP11" s="21" t="s">
+        <v>148</v>
+      </c>
+      <c r="AQ11" s="21" t="s">
+        <v>148</v>
+      </c>
+      <c r="AZ11" s="21" t="s">
+        <v>148</v>
+      </c>
+      <c r="BM11" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="BN11" s="21" t="s">
+        <v>148</v>
+      </c>
+      <c r="BO11" s="24"/>
+      <c r="BQ11" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="BR11" s="21" t="s">
         <v>150</v>
       </c>
-      <c r="BP11" s="21" t="s">
+      <c r="BV11" s="21" t="s">
         <v>151</v>
       </c>
-      <c r="BS11" s="21" t="s">
+      <c r="BY11" s="21" t="s">
         <v>152</v>
       </c>
-      <c r="BT11" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="BU11" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="BY11" s="21" t="s">
+      <c r="BZ11" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="CA11" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="CE11" s="21" t="s">
         <v>432</v>
       </c>
-      <c r="BZ11" s="21" t="s">
+      <c r="CF11" s="21" t="s">
         <v>75</v>
       </c>
-      <c r="CA11" s="21" t="s">
-        <v>148</v>
-      </c>
-      <c r="CB11" s="21" t="s">
+      <c r="CG11" s="21" t="s">
+        <v>148</v>
+      </c>
+      <c r="CH11" s="21" t="s">
         <v>74</v>
       </c>
-      <c r="CC11" s="21" t="s">
-        <v>148</v>
-      </c>
-      <c r="CD11" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="CE11" s="21" t="s">
+      <c r="CI11" s="21" t="s">
+        <v>148</v>
+      </c>
+      <c r="CJ11" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="CK11" s="21" t="s">
         <v>172</v>
       </c>
-      <c r="CF11" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="CG11" s="21" t="s">
+      <c r="CL11" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="CM11" s="21" t="s">
         <v>173</v>
       </c>
-      <c r="CK11" s="21" t="s">
+      <c r="CQ11" s="21" t="s">
         <v>173</v>
       </c>
-      <c r="CL11" s="21" t="s">
+      <c r="CR11" s="21" t="s">
         <v>76</v>
       </c>
-      <c r="CM11" s="21" t="s">
-        <v>137</v>
-      </c>
-      <c r="CN11" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="CO11" s="21" t="s">
-        <v>148</v>
-      </c>
-      <c r="CP11" s="24"/>
-      <c r="CR11" s="21" t="s">
+      <c r="CS11" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="CT11" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="CU11" s="21" t="s">
+        <v>148</v>
+      </c>
+      <c r="CV11" s="24"/>
+      <c r="CX11" s="21" t="s">
         <v>374</v>
       </c>
-      <c r="CS11" s="21" t="s">
+      <c r="CY11" s="21" t="s">
         <v>82</v>
       </c>
-      <c r="CT11" s="21" t="s">
+      <c r="CZ11" s="21" t="s">
         <v>173</v>
       </c>
-      <c r="CX11" s="21" t="s">
+      <c r="DD11" s="21" t="s">
         <v>174</v>
       </c>
-      <c r="CY11" s="21" t="s">
+      <c r="DE11" s="21" t="s">
         <v>363</v>
       </c>
-      <c r="CZ11" s="21" t="s">
+      <c r="DF11" s="21" t="s">
         <v>175</v>
       </c>
-      <c r="DA11" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="DB11" s="21" t="s">
+      <c r="DG11" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="DH11" s="21" t="s">
         <v>109</v>
       </c>
-      <c r="DC11" s="21" t="s">
+      <c r="DI11" s="21" t="s">
         <v>385</v>
       </c>
-      <c r="DD11" s="21" t="s">
+      <c r="DJ11" s="21" t="s">
         <v>178</v>
       </c>
-      <c r="DF11" s="21" t="s">
+      <c r="DL11" s="21" t="s">
         <v>115</v>
       </c>
-      <c r="DG11" s="21" t="s">
+      <c r="DM11" s="21" t="s">
         <v>117</v>
       </c>
-      <c r="DH11" s="21">
+      <c r="DN11" s="21">
         <v>3028976789</v>
       </c>
-      <c r="DI11" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="DJ11" s="21" t="s">
+      <c r="DO11" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="DP11" s="21" t="s">
         <v>246</v>
       </c>
-      <c r="DK11" s="21" t="s">
+      <c r="DQ11" s="21" t="s">
         <v>123</v>
       </c>
-      <c r="DL11" s="21" t="s">
+      <c r="DR11" s="21" t="s">
         <v>122</v>
       </c>
-      <c r="DM11" s="21" t="s">
+      <c r="DS11" s="21" t="s">
         <v>124</v>
       </c>
-      <c r="DN11" s="21" t="s">
+      <c r="DT11" s="21" t="s">
         <v>121</v>
       </c>
-      <c r="DO11" s="21" t="s">
+      <c r="DU11" s="21" t="s">
         <v>125</v>
       </c>
-      <c r="DP11" s="21" t="s">
+      <c r="DV11" s="21" t="s">
         <v>120</v>
       </c>
-      <c r="DQ11" s="21" t="s">
+      <c r="DW11" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="DR11" s="21" t="s">
+      <c r="DX11" s="21" t="s">
         <v>119</v>
       </c>
-      <c r="DS11" s="21" t="s">
-        <v>137</v>
-      </c>
-      <c r="DT11" s="21" t="s">
-        <v>137</v>
-      </c>
-      <c r="DU11" s="21" t="s">
-        <v>137</v>
-      </c>
-      <c r="DV11" s="21" t="s">
-        <v>137</v>
-      </c>
-      <c r="DW11" s="21" t="s">
-        <v>137</v>
-      </c>
-      <c r="DX11" s="21" t="s">
-        <v>137</v>
-      </c>
       <c r="DY11" s="21" t="s">
         <v>137</v>
       </c>
@@ -5156,26 +5237,44 @@
       <c r="ED11" s="21" t="s">
         <v>137</v>
       </c>
-      <c r="EE11" s="27" t="s">
+      <c r="EE11" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="EF11" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="EG11" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="EH11" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="EI11" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="EJ11" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="EK11" s="27" t="s">
         <v>425</v>
       </c>
-      <c r="EF11" s="21" t="s">
-        <v>137</v>
-      </c>
-      <c r="EG11" s="21" t="s">
-        <v>137</v>
-      </c>
-      <c r="EH11" s="21" t="s">
-        <v>137</v>
-      </c>
-      <c r="EI11" s="21" t="s">
-        <v>137</v>
-      </c>
-      <c r="EJ11" s="21" t="s">
+      <c r="EL11" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="EM11" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="EN11" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="EO11" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="EP11" s="21" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="12" spans="1:140" s="21" customFormat="1" ht="68" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:146" s="21" customFormat="1" ht="68" x14ac:dyDescent="0.2">
       <c r="A12" s="21" t="s">
         <v>134</v>
       </c>
@@ -5218,127 +5317,113 @@
       <c r="R12" s="22" t="s">
         <v>407</v>
       </c>
-      <c r="S12" s="21" t="s">
+      <c r="S12" s="22"/>
+      <c r="T12" s="22"/>
+      <c r="U12" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="X12" s="21" t="s">
-        <v>137</v>
-      </c>
-      <c r="Y12" s="21" t="s">
+      <c r="Z12" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="AB12" s="21" t="s">
         <v>391</v>
       </c>
-      <c r="AE12" s="19" t="s">
+      <c r="AH12" s="19" t="s">
         <v>378</v>
       </c>
-      <c r="AF12" s="19" t="s">
+      <c r="AI12" s="19" t="s">
         <v>378</v>
       </c>
-      <c r="AG12" s="21">
+      <c r="AJ12" s="19"/>
+      <c r="AK12" s="19"/>
+      <c r="AL12" s="21">
         <v>3015774089</v>
       </c>
-      <c r="AH12" s="21">
+      <c r="AM12" s="21">
         <v>3014524258</v>
       </c>
-      <c r="AI12" s="21">
+      <c r="AN12" s="21">
         <v>3015567865</v>
       </c>
-      <c r="AJ12" s="21">
+      <c r="AO12" s="21">
         <v>3014524258</v>
       </c>
-      <c r="AK12" s="21" t="s">
+      <c r="AP12" s="21" t="s">
         <v>146</v>
       </c>
-      <c r="AL12" s="21" t="s">
+      <c r="AQ12" s="21" t="s">
         <v>170</v>
       </c>
-      <c r="AT12" s="21" t="s">
-        <v>137</v>
-      </c>
-      <c r="BG12" s="21" t="s">
-        <v>137</v>
-      </c>
-      <c r="BK12" s="21" t="s">
-        <v>137</v>
-      </c>
-      <c r="BT12" s="21" t="s">
-        <v>137</v>
-      </c>
-      <c r="BY12" s="21" t="s">
+      <c r="AZ12" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="BM12" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="BQ12" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="BZ12" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="CE12" s="21" t="s">
         <v>432</v>
       </c>
-      <c r="CF12" s="21" t="s">
-        <v>137</v>
-      </c>
-      <c r="CP12" s="24"/>
-      <c r="DA12" s="21" t="s">
-        <v>137</v>
-      </c>
-      <c r="DB12" s="21" t="s">
+      <c r="CL12" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="CV12" s="24"/>
+      <c r="DG12" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="DH12" s="21" t="s">
         <v>109</v>
       </c>
-      <c r="DC12" s="21" t="s">
+      <c r="DI12" s="21" t="s">
         <v>386</v>
       </c>
-      <c r="DD12" s="21" t="s">
+      <c r="DJ12" s="21" t="s">
         <v>178</v>
       </c>
-      <c r="DF12" s="21" t="s">
+      <c r="DL12" s="21" t="s">
         <v>115</v>
       </c>
-      <c r="DG12" s="21" t="s">
+      <c r="DM12" s="21" t="s">
         <v>117</v>
       </c>
-      <c r="DH12" s="21">
+      <c r="DN12" s="21">
         <v>3028976789</v>
       </c>
-      <c r="DI12" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="DJ12" s="21" t="s">
+      <c r="DO12" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="DP12" s="21" t="s">
         <v>246</v>
       </c>
-      <c r="DK12" s="21" t="s">
+      <c r="DQ12" s="21" t="s">
         <v>123</v>
       </c>
-      <c r="DL12" s="21" t="s">
+      <c r="DR12" s="21" t="s">
         <v>122</v>
       </c>
-      <c r="DM12" s="21" t="s">
+      <c r="DS12" s="21" t="s">
         <v>124</v>
       </c>
-      <c r="DN12" s="21" t="s">
+      <c r="DT12" s="21" t="s">
         <v>121</v>
       </c>
-      <c r="DO12" s="21" t="s">
+      <c r="DU12" s="21" t="s">
         <v>125</v>
       </c>
-      <c r="DP12" s="21" t="s">
+      <c r="DV12" s="21" t="s">
         <v>120</v>
       </c>
-      <c r="DQ12" s="21" t="s">
+      <c r="DW12" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="DR12" s="21" t="s">
+      <c r="DX12" s="21" t="s">
         <v>119</v>
       </c>
-      <c r="DS12" s="21" t="s">
-        <v>137</v>
-      </c>
-      <c r="DT12" s="21" t="s">
-        <v>137</v>
-      </c>
-      <c r="DU12" s="21" t="s">
-        <v>137</v>
-      </c>
-      <c r="DV12" s="21" t="s">
-        <v>137</v>
-      </c>
-      <c r="DW12" s="21" t="s">
-        <v>137</v>
-      </c>
-      <c r="DX12" s="21" t="s">
-        <v>137</v>
-      </c>
       <c r="DY12" s="21" t="s">
         <v>137</v>
       </c>
@@ -5357,26 +5442,44 @@
       <c r="ED12" s="21" t="s">
         <v>137</v>
       </c>
-      <c r="EE12" s="27" t="s">
+      <c r="EE12" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="EF12" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="EG12" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="EH12" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="EI12" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="EJ12" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="EK12" s="27" t="s">
         <v>425</v>
       </c>
-      <c r="EF12" s="21" t="s">
-        <v>137</v>
-      </c>
-      <c r="EG12" s="21" t="s">
-        <v>137</v>
-      </c>
-      <c r="EH12" s="21" t="s">
-        <v>137</v>
-      </c>
-      <c r="EI12" s="21" t="s">
-        <v>137</v>
-      </c>
-      <c r="EJ12" s="21" t="s">
+      <c r="EL12" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="EM12" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="EN12" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="EO12" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="EP12" s="21" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="13" spans="1:140" s="21" customFormat="1" ht="68" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:146" s="21" customFormat="1" ht="68" x14ac:dyDescent="0.2">
       <c r="A13" s="21" t="s">
         <v>134</v>
       </c>
@@ -5419,114 +5522,100 @@
       <c r="R13" s="22" t="s">
         <v>299</v>
       </c>
-      <c r="S13" s="21" t="s">
+      <c r="S13" s="22"/>
+      <c r="T13" s="22"/>
+      <c r="U13" s="21" t="s">
         <v>144</v>
       </c>
-      <c r="X13" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="Y13" s="21" t="s">
+      <c r="Z13" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="AB13" s="21" t="s">
         <v>392</v>
       </c>
-      <c r="AE13" s="19" t="s">
+      <c r="AH13" s="19" t="s">
         <v>382</v>
       </c>
-      <c r="AF13" s="19" t="s">
+      <c r="AI13" s="19" t="s">
         <v>382</v>
       </c>
-      <c r="AG13" s="21">
+      <c r="AJ13" s="19"/>
+      <c r="AK13" s="19"/>
+      <c r="AL13" s="21">
         <v>3015774089</v>
       </c>
-      <c r="AH13" s="21">
+      <c r="AM13" s="21">
         <v>3014524258</v>
       </c>
-      <c r="AI13" s="21">
+      <c r="AN13" s="21">
         <v>3015567865</v>
       </c>
-      <c r="AJ13" s="21">
+      <c r="AO13" s="21">
         <v>3014524258</v>
       </c>
-      <c r="AK13" s="21" t="s">
+      <c r="AP13" s="21" t="s">
         <v>170</v>
       </c>
-      <c r="AL13" s="21" t="s">
-        <v>148</v>
-      </c>
-      <c r="AT13" s="21" t="s">
-        <v>137</v>
-      </c>
-      <c r="BG13" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="BH13" s="21" t="s">
-        <v>148</v>
-      </c>
-      <c r="BY13" s="21" t="s">
+      <c r="AQ13" s="21" t="s">
+        <v>148</v>
+      </c>
+      <c r="AZ13" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="BM13" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="BN13" s="21" t="s">
+        <v>148</v>
+      </c>
+      <c r="CE13" s="21" t="s">
         <v>432</v>
       </c>
-      <c r="BZ13" s="21" t="s">
+      <c r="CF13" s="21" t="s">
         <v>75</v>
       </c>
-      <c r="CA13" s="21" t="s">
+      <c r="CG13" s="21" t="s">
         <v>153</v>
       </c>
-      <c r="CB13" s="21" t="s">
+      <c r="CH13" s="21" t="s">
         <v>74</v>
       </c>
-      <c r="CC13" s="21" t="s">
+      <c r="CI13" s="21" t="s">
         <v>73</v>
       </c>
-      <c r="CD13" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="CE13" s="21" t="s">
+      <c r="CJ13" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="CK13" s="21" t="s">
         <v>67</v>
       </c>
-      <c r="DJ13" s="21" t="s">
+      <c r="DP13" s="21" t="s">
         <v>246</v>
       </c>
-      <c r="DK13" s="21" t="s">
+      <c r="DQ13" s="21" t="s">
         <v>123</v>
       </c>
-      <c r="DL13" s="21" t="s">
+      <c r="DR13" s="21" t="s">
         <v>122</v>
       </c>
-      <c r="DM13" s="21" t="s">
+      <c r="DS13" s="21" t="s">
         <v>124</v>
       </c>
-      <c r="DN13" s="21" t="s">
+      <c r="DT13" s="21" t="s">
         <v>121</v>
       </c>
-      <c r="DO13" s="21" t="s">
+      <c r="DU13" s="21" t="s">
         <v>125</v>
       </c>
-      <c r="DP13" s="21" t="s">
+      <c r="DV13" s="21" t="s">
         <v>120</v>
       </c>
-      <c r="DQ13" s="21" t="s">
+      <c r="DW13" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="DR13" s="21" t="s">
+      <c r="DX13" s="21" t="s">
         <v>119</v>
       </c>
-      <c r="DS13" s="21" t="s">
-        <v>148</v>
-      </c>
-      <c r="DT13" s="21" t="s">
-        <v>148</v>
-      </c>
-      <c r="DU13" s="21" t="s">
-        <v>148</v>
-      </c>
-      <c r="DV13" s="21" t="s">
-        <v>148</v>
-      </c>
-      <c r="DW13" s="21" t="s">
-        <v>148</v>
-      </c>
-      <c r="DX13" s="21" t="s">
-        <v>148</v>
-      </c>
       <c r="DY13" s="21" t="s">
         <v>148</v>
       </c>
@@ -5545,101 +5634,129 @@
       <c r="ED13" s="21" t="s">
         <v>148</v>
       </c>
-      <c r="EE13" s="27" t="s">
+      <c r="EE13" s="21" t="s">
+        <v>148</v>
+      </c>
+      <c r="EF13" s="21" t="s">
+        <v>148</v>
+      </c>
+      <c r="EG13" s="21" t="s">
+        <v>148</v>
+      </c>
+      <c r="EH13" s="21" t="s">
+        <v>148</v>
+      </c>
+      <c r="EI13" s="21" t="s">
+        <v>148</v>
+      </c>
+      <c r="EJ13" s="21" t="s">
+        <v>148</v>
+      </c>
+      <c r="EK13" s="27" t="s">
         <v>425</v>
       </c>
-      <c r="EF13" s="21" t="s">
-        <v>148</v>
-      </c>
-      <c r="EG13" s="21" t="s">
-        <v>148</v>
-      </c>
-      <c r="EH13" s="21" t="s">
-        <v>148</v>
-      </c>
-      <c r="EI13" s="21" t="s">
-        <v>148</v>
-      </c>
-      <c r="EJ13" s="21" t="s">
+      <c r="EL13" s="21" t="s">
+        <v>148</v>
+      </c>
+      <c r="EM13" s="21" t="s">
+        <v>148</v>
+      </c>
+      <c r="EN13" s="21" t="s">
+        <v>148</v>
+      </c>
+      <c r="EO13" s="21" t="s">
+        <v>148</v>
+      </c>
+      <c r="EP13" s="21" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="14" spans="1:140" s="21" customFormat="1" ht="88" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:146" s="21" customFormat="1" ht="88" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K14" s="25" t="s">
         <v>388</v>
       </c>
-      <c r="AE14" s="19" t="s">
+      <c r="AH14" s="19" t="s">
         <v>403</v>
       </c>
-      <c r="AF14" s="19" t="s">
+      <c r="AI14" s="19" t="s">
         <v>403</v>
       </c>
+      <c r="AJ14" s="19"/>
+      <c r="AK14" s="19"/>
     </row>
-    <row r="15" spans="1:140" s="21" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:146" s="21" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="K15" s="21" t="s">
         <v>389</v>
       </c>
-      <c r="AE15" s="19" t="s">
+      <c r="AH15" s="19" t="s">
         <v>404</v>
       </c>
-      <c r="AF15" s="19" t="s">
+      <c r="AI15" s="19" t="s">
         <v>404</v>
       </c>
+      <c r="AJ15" s="19"/>
+      <c r="AK15" s="19"/>
     </row>
-    <row r="16" spans="1:140" s="21" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:146" s="21" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="K16" s="21" t="s">
         <v>390</v>
       </c>
-      <c r="AE16" s="19" t="s">
+      <c r="AH16" s="19" t="s">
         <v>405</v>
       </c>
-      <c r="AF16" s="19" t="s">
+      <c r="AI16" s="19" t="s">
         <v>405</v>
       </c>
+      <c r="AJ16" s="19"/>
+      <c r="AK16" s="19"/>
     </row>
-    <row r="17" spans="11:32" s="21" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+    <row r="17" spans="11:37" s="21" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="K17" s="21" t="s">
         <v>142</v>
       </c>
-      <c r="AE17" s="19" t="s">
+      <c r="AH17" s="19" t="s">
         <v>406</v>
       </c>
-      <c r="AF17" s="19" t="s">
+      <c r="AI17" s="19" t="s">
         <v>406</v>
       </c>
+      <c r="AJ17" s="19"/>
+      <c r="AK17" s="19"/>
     </row>
-    <row r="18" spans="11:32" s="21" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="18" spans="11:37" s="21" customFormat="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <autoFilter ref="A1:EJ13" xr:uid="{D6C03A80-53F5-C744-BC65-FAA91BD85774}"/>
+  <autoFilter ref="A1:EP13" xr:uid="{D6C03A80-53F5-C744-BC65-FAA91BD85774}"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="AE7" r:id="rId1" xr:uid="{CC8E0D0F-8C4A-1647-BD51-330F10CD9EE7}"/>
-    <hyperlink ref="AE4" r:id="rId2" xr:uid="{54A26098-2C02-B14A-A8B8-E895ACEFE8FC}"/>
-    <hyperlink ref="AF4" r:id="rId3" xr:uid="{19B8EC6B-4DE1-EF45-9AC5-07A97297CA08}"/>
-    <hyperlink ref="AE2" r:id="rId4" xr:uid="{CE9060F8-46A2-8E4A-9049-D259F5FF8833}"/>
-    <hyperlink ref="AF2" r:id="rId5" xr:uid="{9F426852-B12C-F246-BBD4-2DFF4046F17B}"/>
-    <hyperlink ref="AF7" r:id="rId6" xr:uid="{F867FCEE-CDE3-774C-AA60-18F374257445}"/>
-    <hyperlink ref="AE8" r:id="rId7" xr:uid="{FF13954F-3772-2244-8624-0759DAAA195B}"/>
-    <hyperlink ref="AF8" r:id="rId8" xr:uid="{DEA58592-D611-1446-A2DF-45ED1084017D}"/>
-    <hyperlink ref="AE5" r:id="rId9" xr:uid="{AE8E2947-9665-444E-BB61-535EF103703A}"/>
-    <hyperlink ref="AF5" r:id="rId10" xr:uid="{03D22372-21FE-6647-9FB7-E611341DF12C}"/>
-    <hyperlink ref="AE6" r:id="rId11" xr:uid="{38E74D40-B9B2-9F4F-A95C-07E96ED19969}"/>
-    <hyperlink ref="AE13" r:id="rId12" xr:uid="{A84CFFC5-66D9-2E4D-9EAF-A805310521D0}"/>
-    <hyperlink ref="AE12" r:id="rId13" xr:uid="{EE58DF3D-4E06-D242-A11C-C73725F63244}"/>
-    <hyperlink ref="AE9" r:id="rId14" xr:uid="{9561474B-13C0-5C45-A0AF-651803129C22}"/>
-    <hyperlink ref="AF9" r:id="rId15" xr:uid="{A1121A3E-E434-0D46-8060-8CC9554A173E}"/>
-    <hyperlink ref="AE10" r:id="rId16" xr:uid="{74DEEA39-9EE3-DA40-986A-18AB27D7AF3D}"/>
-    <hyperlink ref="AF10" r:id="rId17" xr:uid="{10D6E031-35FA-1A41-812A-AC8A67918A79}"/>
-    <hyperlink ref="AE11" r:id="rId18" xr:uid="{E72B4306-86EB-094D-A7D7-3CE674C9E99B}"/>
-    <hyperlink ref="AF11" r:id="rId19" xr:uid="{BBD42CF8-45B8-BC4C-8616-E5054108E74E}"/>
-    <hyperlink ref="AF12" r:id="rId20" xr:uid="{CB1028F2-6BEB-9845-BBBF-2CCF7E196D7E}"/>
-    <hyperlink ref="AF13" r:id="rId21" xr:uid="{38A05DA8-5083-B64C-9BB7-7515D994A102}"/>
-    <hyperlink ref="AE14:AE17" r:id="rId22" display="charmsparticipant12@yopmail.com" xr:uid="{F7B2D757-0C7A-4D43-8200-C0254FB3451B}"/>
-    <hyperlink ref="AE14" r:id="rId23" xr:uid="{00D2EC9C-C0B0-A94F-A0A4-8DCEB003125B}"/>
-    <hyperlink ref="AE15" r:id="rId24" xr:uid="{4B08829F-C727-1F4D-8585-8623FDC25445}"/>
-    <hyperlink ref="AE16" r:id="rId25" xr:uid="{D67C22F6-0FF5-2A43-9F6B-E465DA043CCB}"/>
-    <hyperlink ref="AE17" r:id="rId26" xr:uid="{39CD3A02-5AC2-A349-A912-CB63C565E8B1}"/>
-    <hyperlink ref="AF14:AF17" r:id="rId27" display="charmsparticipant12@yopmail.com" xr:uid="{0D113990-F28B-4045-82B3-3B329AB1A52B}"/>
+    <hyperlink ref="AH7" r:id="rId1" xr:uid="{CC8E0D0F-8C4A-1647-BD51-330F10CD9EE7}"/>
+    <hyperlink ref="AH4" r:id="rId2" xr:uid="{54A26098-2C02-B14A-A8B8-E895ACEFE8FC}"/>
+    <hyperlink ref="AI4" r:id="rId3" xr:uid="{19B8EC6B-4DE1-EF45-9AC5-07A97297CA08}"/>
+    <hyperlink ref="AH2" r:id="rId4" xr:uid="{CE9060F8-46A2-8E4A-9049-D259F5FF8833}"/>
+    <hyperlink ref="AI2" r:id="rId5" xr:uid="{9F426852-B12C-F246-BBD4-2DFF4046F17B}"/>
+    <hyperlink ref="AI7" r:id="rId6" xr:uid="{F867FCEE-CDE3-774C-AA60-18F374257445}"/>
+    <hyperlink ref="AH8" r:id="rId7" xr:uid="{FF13954F-3772-2244-8624-0759DAAA195B}"/>
+    <hyperlink ref="AI8" r:id="rId8" xr:uid="{DEA58592-D611-1446-A2DF-45ED1084017D}"/>
+    <hyperlink ref="AH5" r:id="rId9" xr:uid="{AE8E2947-9665-444E-BB61-535EF103703A}"/>
+    <hyperlink ref="AI5" r:id="rId10" xr:uid="{03D22372-21FE-6647-9FB7-E611341DF12C}"/>
+    <hyperlink ref="AH6" r:id="rId11" xr:uid="{38E74D40-B9B2-9F4F-A95C-07E96ED19969}"/>
+    <hyperlink ref="AH13" r:id="rId12" xr:uid="{A84CFFC5-66D9-2E4D-9EAF-A805310521D0}"/>
+    <hyperlink ref="AH12" r:id="rId13" xr:uid="{EE58DF3D-4E06-D242-A11C-C73725F63244}"/>
+    <hyperlink ref="AH9" r:id="rId14" xr:uid="{9561474B-13C0-5C45-A0AF-651803129C22}"/>
+    <hyperlink ref="AI9" r:id="rId15" xr:uid="{A1121A3E-E434-0D46-8060-8CC9554A173E}"/>
+    <hyperlink ref="AH10" r:id="rId16" xr:uid="{74DEEA39-9EE3-DA40-986A-18AB27D7AF3D}"/>
+    <hyperlink ref="AI10" r:id="rId17" xr:uid="{10D6E031-35FA-1A41-812A-AC8A67918A79}"/>
+    <hyperlink ref="AH11" r:id="rId18" xr:uid="{E72B4306-86EB-094D-A7D7-3CE674C9E99B}"/>
+    <hyperlink ref="AI11" r:id="rId19" xr:uid="{BBD42CF8-45B8-BC4C-8616-E5054108E74E}"/>
+    <hyperlink ref="AI12" r:id="rId20" xr:uid="{CB1028F2-6BEB-9845-BBBF-2CCF7E196D7E}"/>
+    <hyperlink ref="AI13" r:id="rId21" xr:uid="{38A05DA8-5083-B64C-9BB7-7515D994A102}"/>
+    <hyperlink ref="AH14:AH17" r:id="rId22" display="charmsparticipant12@yopmail.com" xr:uid="{F7B2D757-0C7A-4D43-8200-C0254FB3451B}"/>
+    <hyperlink ref="AH14" r:id="rId23" xr:uid="{00D2EC9C-C0B0-A94F-A0A4-8DCEB003125B}"/>
+    <hyperlink ref="AH15" r:id="rId24" xr:uid="{4B08829F-C727-1F4D-8585-8623FDC25445}"/>
+    <hyperlink ref="AH16" r:id="rId25" xr:uid="{D67C22F6-0FF5-2A43-9F6B-E465DA043CCB}"/>
+    <hyperlink ref="AH17" r:id="rId26" xr:uid="{39CD3A02-5AC2-A349-A912-CB63C565E8B1}"/>
+    <hyperlink ref="AI14:AI17" r:id="rId27" display="charmsparticipant12@yopmail.com" xr:uid="{0D113990-F28B-4045-82B3-3B329AB1A52B}"/>
+    <hyperlink ref="AJ2" r:id="rId28" xr:uid="{E22D24ED-7C96-1446-A5F8-21D1507C6179}"/>
+    <hyperlink ref="AJ3" r:id="rId29" xr:uid="{70C65664-4427-354A-B785-E0B132A43F5C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
Fanconi Screener Contact Information, Demographics, Fanconi History Information
</commit_message>
<xml_diff>
--- a/src/test/java/CHARMS/resources/data.xlsx
+++ b/src/test/java/CHARMS/resources/data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jains18/git/CBIIT-Test-Automation/CBIIT-Test-Automation/src/test/java/CHARMS/Resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jains18/git/CBIIT-Test-Automation/CBIIT-Test-Automation/src/test/java/CHARMS/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEB6D4EE-562D-834F-91FE-8C3F1DEBBD78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9E2A62E-2815-344C-B861-01B8D3565E08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4280" yWindow="500" windowWidth="26000" windowHeight="17640" xr2:uid="{B3E53782-D40D-CC47-BA00-27DFD8C445AF}"/>
+    <workbookView xWindow="4240" yWindow="760" windowWidth="26000" windowHeight="17640" xr2:uid="{B3E53782-D40D-CC47-BA00-27DFD8C445AF}"/>
   </bookViews>
   <sheets>
     <sheet name="FanconiScreener" sheetId="1" r:id="rId1"/>
@@ -1989,9 +1989,9 @@
   </sheetPr>
   <dimension ref="A1:EP18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="113" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="M1" zoomScale="113" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K2" sqref="K2"/>
+      <selection pane="bottomLeft" activeCell="T1" sqref="T1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2520,7 +2520,7 @@
         <v>269</v>
       </c>
       <c r="S2" s="22"/>
-      <c r="T2" s="22">
+      <c r="T2" s="21">
         <v>76</v>
       </c>
       <c r="U2" s="21" t="s">

</xml_diff>

<commit_message>
assert the Demographic Information on Participant Details
</commit_message>
<xml_diff>
--- a/src/test/java/CHARMS/resources/data.xlsx
+++ b/src/test/java/CHARMS/resources/data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10112"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jains18/git/CBIIT-Test-Automation/CBIIT-Test-Automation/src/test/java/CHARMS/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9E2A62E-2815-344C-B861-01B8D3565E08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A6888A2-8E7B-8245-A041-13A541A451DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4240" yWindow="760" windowWidth="26000" windowHeight="17640" xr2:uid="{B3E53782-D40D-CC47-BA00-27DFD8C445AF}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1223" uniqueCount="443">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1222" uniqueCount="442">
   <si>
     <t>Yes</t>
   </si>
@@ -850,9 +850,6 @@
     <t>-- None --</t>
   </si>
   <si>
-    <t>04/21/1948</t>
-  </si>
-  <si>
     <t>SpecifyParticipationInOtherStudies</t>
   </si>
   <si>
@@ -940,9 +937,6 @@
     <t>Physician 4</t>
   </si>
   <si>
-    <t>04/21/1940</t>
-  </si>
-  <si>
     <t>12/11/2009</t>
   </si>
   <si>
@@ -1264,24 +1258,6 @@
     <t>charmsparticipant16@yopmail.com</t>
   </si>
   <si>
-    <t>04/30/1930</t>
-  </si>
-  <si>
-    <t>04/29/1935</t>
-  </si>
-  <si>
-    <t>04/26/1950</t>
-  </si>
-  <si>
-    <t>04/11/1940</t>
-  </si>
-  <si>
-    <t>04/27/1937</t>
-  </si>
-  <si>
-    <t>04/21/1935</t>
-  </si>
-  <si>
     <t>Fanconi-10</t>
   </si>
   <si>
@@ -1300,15 +1276,6 @@
     <t>Proxy-12</t>
   </si>
   <si>
-    <t>04/23/1920</t>
-  </si>
-  <si>
-    <t>04/21/1910</t>
-  </si>
-  <si>
-    <t>04/21/1925</t>
-  </si>
-  <si>
     <t>Other research fund at Study3</t>
   </si>
   <si>
@@ -1370,6 +1337,36 @@
   </si>
   <si>
     <t>CalculatedAge</t>
+  </si>
+  <si>
+    <t>01/23/1920</t>
+  </si>
+  <si>
+    <t>01/21/1910</t>
+  </si>
+  <si>
+    <t>01/21/1925</t>
+  </si>
+  <si>
+    <t>01/26/1950</t>
+  </si>
+  <si>
+    <t>01/11/1940</t>
+  </si>
+  <si>
+    <t>01/30/1930</t>
+  </si>
+  <si>
+    <t>01/29/1935</t>
+  </si>
+  <si>
+    <t>01/27/1937</t>
+  </si>
+  <si>
+    <t>01/21/1935</t>
+  </si>
+  <si>
+    <t>01/21/1940</t>
   </si>
 </sst>
 </file>
@@ -1989,9 +1986,9 @@
   </sheetPr>
   <dimension ref="A1:EP18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" zoomScale="113" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="T1" sqref="T1"/>
+    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="113" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="T12" sqref="T12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2086,7 +2083,7 @@
         <v>141</v>
       </c>
       <c r="L1" s="7" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="M1" s="7" t="s">
         <v>143</v>
@@ -2107,10 +2104,10 @@
         <v>128</v>
       </c>
       <c r="S1" s="9" t="s">
-        <v>436</v>
+        <v>425</v>
       </c>
       <c r="T1" s="9" t="s">
-        <v>442</v>
+        <v>431</v>
       </c>
       <c r="U1" s="10" t="s">
         <v>4</v>
@@ -2131,7 +2128,7 @@
         <v>198</v>
       </c>
       <c r="AA1" s="11" t="s">
-        <v>434</v>
+        <v>423</v>
       </c>
       <c r="AB1" s="7" t="s">
         <v>7</v>
@@ -2158,10 +2155,10 @@
         <v>39</v>
       </c>
       <c r="AJ1" s="12" t="s">
-        <v>440</v>
+        <v>429</v>
       </c>
       <c r="AK1" s="12" t="s">
-        <v>441</v>
+        <v>430</v>
       </c>
       <c r="AL1" s="14" t="s">
         <v>14</v>
@@ -2203,7 +2200,7 @@
         <v>191</v>
       </c>
       <c r="AY1" s="15" t="s">
-        <v>437</v>
+        <v>426</v>
       </c>
       <c r="AZ1" s="16" t="s">
         <v>203</v>
@@ -2266,10 +2263,10 @@
         <v>207</v>
       </c>
       <c r="BT1" s="13" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="BU1" s="13" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="BV1" s="13" t="s">
         <v>212</v>
@@ -2290,7 +2287,7 @@
         <v>214</v>
       </c>
       <c r="CB1" s="13" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="CC1" s="13" t="s">
         <v>188</v>
@@ -2395,7 +2392,7 @@
         <v>226</v>
       </c>
       <c r="DK1" s="13" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="DL1" s="13" t="s">
         <v>114</v>
@@ -2496,13 +2493,13 @@
         <v>38</v>
       </c>
       <c r="B2" s="21" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="C2" s="21" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="D2" s="21" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="N2" s="21" t="s">
         <v>0</v>
@@ -2516,8 +2513,8 @@
       <c r="Q2" s="21">
         <v>21</v>
       </c>
-      <c r="R2" s="22" t="s">
-        <v>269</v>
+      <c r="R2" s="22">
+        <v>17553</v>
       </c>
       <c r="S2" s="22"/>
       <c r="T2" s="21">
@@ -2536,7 +2533,7 @@
         <v>0</v>
       </c>
       <c r="AA2" s="21" t="s">
-        <v>435</v>
+        <v>424</v>
       </c>
       <c r="AB2" s="21" t="s">
         <v>22</v>
@@ -2557,13 +2554,13 @@
         <v>28907</v>
       </c>
       <c r="AH2" s="18" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="AI2" s="18" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="AJ2" s="19" t="s">
-        <v>438</v>
+        <v>427</v>
       </c>
       <c r="AK2" s="19"/>
       <c r="AL2" s="21">
@@ -2603,7 +2600,7 @@
         <v>40</v>
       </c>
       <c r="AX2" s="21" t="s">
-        <v>433</v>
+        <v>422</v>
       </c>
       <c r="AY2" s="21" t="s">
         <v>0</v>
@@ -2612,7 +2609,7 @@
         <v>0</v>
       </c>
       <c r="BA2" s="21" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="BB2" s="21" t="s">
         <v>37</v>
@@ -2681,7 +2678,7 @@
         <v>0</v>
       </c>
       <c r="CE2" s="21" t="s">
-        <v>432</v>
+        <v>421</v>
       </c>
       <c r="CF2" s="21" t="s">
         <v>75</v>
@@ -2846,7 +2843,7 @@
         <v>0</v>
       </c>
       <c r="EK2" s="27" t="s">
-        <v>425</v>
+        <v>414</v>
       </c>
       <c r="EL2" s="21" t="s">
         <v>0</v>
@@ -2875,7 +2872,7 @@
         <v>136</v>
       </c>
       <c r="D3" s="21" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="N3" s="21" t="s">
         <v>137</v>
@@ -2890,7 +2887,7 @@
         <v>23</v>
       </c>
       <c r="R3" s="22" t="s">
-        <v>419</v>
+        <v>432</v>
       </c>
       <c r="S3" s="22"/>
       <c r="T3" s="22"/>
@@ -2916,7 +2913,7 @@
         <v>145</v>
       </c>
       <c r="AJ3" s="19" t="s">
-        <v>439</v>
+        <v>428</v>
       </c>
       <c r="AK3" s="19"/>
       <c r="AL3" s="21">
@@ -2968,7 +2965,7 @@
         <v>149</v>
       </c>
       <c r="BO3" s="22" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="BQ3" s="21" t="s">
         <v>0</v>
@@ -2989,7 +2986,7 @@
         <v>0</v>
       </c>
       <c r="CE3" s="21" t="s">
-        <v>432</v>
+        <v>421</v>
       </c>
       <c r="CF3" s="21" t="s">
         <v>75</v>
@@ -3034,7 +3031,7 @@
         <v>149</v>
       </c>
       <c r="CV3" s="22" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="CX3" s="21" t="s">
         <v>80</v>
@@ -3067,10 +3064,10 @@
         <v>160</v>
       </c>
       <c r="DL3" s="21" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="DM3" s="21" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="DN3" s="21">
         <v>3028976789</v>
@@ -3142,7 +3139,7 @@
         <v>0</v>
       </c>
       <c r="EK3" s="27" t="s">
-        <v>425</v>
+        <v>414</v>
       </c>
       <c r="EL3" s="21" t="s">
         <v>0</v>
@@ -3171,7 +3168,7 @@
         <v>162</v>
       </c>
       <c r="D4" s="21" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="N4" s="21" t="s">
         <v>148</v>
@@ -3186,7 +3183,7 @@
         <v>21</v>
       </c>
       <c r="R4" s="22" t="s">
-        <v>420</v>
+        <v>433</v>
       </c>
       <c r="S4" s="22"/>
       <c r="T4" s="22"/>
@@ -3203,7 +3200,7 @@
         <v>137</v>
       </c>
       <c r="AB4" s="21" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="AH4" s="19" t="s">
         <v>147</v>
@@ -3262,7 +3259,7 @@
         <v>0</v>
       </c>
       <c r="CE4" s="21" t="s">
-        <v>432</v>
+        <v>421</v>
       </c>
       <c r="CF4" s="21" t="s">
         <v>75</v>
@@ -3316,7 +3313,7 @@
         <v>174</v>
       </c>
       <c r="DE4" s="21" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="DF4" s="21" t="s">
         <v>175</v>
@@ -3334,10 +3331,10 @@
         <v>178</v>
       </c>
       <c r="DL4" s="21" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="DM4" s="21" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="DN4" s="21">
         <v>3028976789</v>
@@ -3409,7 +3406,7 @@
         <v>137</v>
       </c>
       <c r="EK4" s="27" t="s">
-        <v>425</v>
+        <v>414</v>
       </c>
       <c r="EL4" s="21" t="s">
         <v>137</v>
@@ -3438,7 +3435,7 @@
         <v>164</v>
       </c>
       <c r="D5" s="21" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="N5" s="21" t="s">
         <v>148</v>
@@ -3453,7 +3450,7 @@
         <v>21</v>
       </c>
       <c r="R5" s="22" t="s">
-        <v>421</v>
+        <v>434</v>
       </c>
       <c r="S5" s="22"/>
       <c r="T5" s="22"/>
@@ -3464,7 +3461,7 @@
         <v>183</v>
       </c>
       <c r="W5" s="21" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="X5" s="21" t="s">
         <v>183</v>
@@ -3535,7 +3532,7 @@
         <v>0</v>
       </c>
       <c r="CE5" s="21" t="s">
-        <v>432</v>
+        <v>421</v>
       </c>
       <c r="CF5" s="21" t="s">
         <v>75</v>
@@ -3577,7 +3574,7 @@
         <v>149</v>
       </c>
       <c r="CV5" s="22" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="CX5" s="21" t="s">
         <v>80</v>
@@ -3589,13 +3586,13 @@
         <v>173</v>
       </c>
       <c r="DD5" s="21" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="DE5" s="21" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="DF5" s="21" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="DG5" s="21" t="s">
         <v>0</v>
@@ -3607,13 +3604,13 @@
         <v>37</v>
       </c>
       <c r="DK5" s="21" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="DL5" s="21" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="DM5" s="21" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="DN5" s="21">
         <v>3028976789</v>
@@ -3685,7 +3682,7 @@
         <v>148</v>
       </c>
       <c r="EK5" s="27" t="s">
-        <v>425</v>
+        <v>414</v>
       </c>
       <c r="EL5" s="21" t="s">
         <v>148</v>
@@ -3714,7 +3711,7 @@
         <v>180</v>
       </c>
       <c r="D6" s="21" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="N6" s="21" t="s">
         <v>148</v>
@@ -3729,7 +3726,7 @@
         <v>26</v>
       </c>
       <c r="R6" s="22" t="s">
-        <v>409</v>
+        <v>435</v>
       </c>
       <c r="S6" s="22"/>
       <c r="T6" s="22"/>
@@ -3746,7 +3743,7 @@
         <v>0</v>
       </c>
       <c r="AB6" s="21" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="AH6" s="18" t="s">
         <v>181</v>
@@ -3795,7 +3792,7 @@
         <v>148</v>
       </c>
       <c r="CE6" s="21" t="s">
-        <v>432</v>
+        <v>421</v>
       </c>
       <c r="CL6" s="21" t="s">
         <v>148</v>
@@ -3811,10 +3808,10 @@
         <v>177</v>
       </c>
       <c r="DJ6" s="21" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="DK6" s="21" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="DL6" s="21" t="s">
         <v>115</v>
@@ -3892,7 +3889,7 @@
         <v>137</v>
       </c>
       <c r="EK6" s="27" t="s">
-        <v>425</v>
+        <v>414</v>
       </c>
       <c r="EL6" s="21" t="s">
         <v>137</v>
@@ -3915,13 +3912,13 @@
         <v>38</v>
       </c>
       <c r="B7" s="21" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="C7" s="21" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="D7" s="21" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="N7" s="21" t="s">
         <v>137</v>
@@ -3936,7 +3933,7 @@
         <v>11</v>
       </c>
       <c r="R7" s="22" t="s">
-        <v>410</v>
+        <v>436</v>
       </c>
       <c r="S7" s="22"/>
       <c r="T7" s="22"/>
@@ -3956,10 +3953,10 @@
         <v>186</v>
       </c>
       <c r="AH7" s="18" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="AI7" s="18" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="AJ7" s="18"/>
       <c r="AK7" s="18"/>
@@ -3998,7 +3995,7 @@
         <v>187</v>
       </c>
       <c r="BT7" s="21" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="BU7" s="21" t="s">
         <v>0</v>
@@ -4016,10 +4013,10 @@
         <v>137</v>
       </c>
       <c r="CB7" s="21" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="CE7" s="21" t="s">
-        <v>432</v>
+        <v>421</v>
       </c>
       <c r="CJ7" s="21" t="s">
         <v>137</v>
@@ -4038,7 +4035,7 @@
         <v>111</v>
       </c>
       <c r="DJ7" s="21" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="DL7" s="21" t="s">
         <v>115</v>
@@ -4116,7 +4113,7 @@
         <v>0</v>
       </c>
       <c r="EK7" s="27" t="s">
-        <v>425</v>
+        <v>414</v>
       </c>
       <c r="EL7" s="21" t="s">
         <v>0</v>
@@ -4139,13 +4136,13 @@
         <v>38</v>
       </c>
       <c r="B8" s="21" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="C8" s="21" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="D8" s="21" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="N8" s="21" t="s">
         <v>137</v>
@@ -4160,7 +4157,7 @@
         <v>30</v>
       </c>
       <c r="R8" s="22" t="s">
-        <v>407</v>
+        <v>437</v>
       </c>
       <c r="S8" s="22"/>
       <c r="T8" s="22"/>
@@ -4195,10 +4192,10 @@
         <v>28907</v>
       </c>
       <c r="AH8" s="18" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="AI8" s="18" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="AJ8" s="18"/>
       <c r="AK8" s="18"/>
@@ -4234,7 +4231,7 @@
         <v>137</v>
       </c>
       <c r="CE8" s="21" t="s">
-        <v>432</v>
+        <v>421</v>
       </c>
       <c r="CL8" s="21" t="s">
         <v>137</v>
@@ -4250,7 +4247,7 @@
         <v>48</v>
       </c>
       <c r="DK8" s="21" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="DL8" s="21" t="s">
         <v>115</v>
@@ -4328,7 +4325,7 @@
         <v>0</v>
       </c>
       <c r="EK8" s="27" t="s">
-        <v>425</v>
+        <v>414</v>
       </c>
       <c r="EL8" s="21" t="s">
         <v>0</v>
@@ -4351,13 +4348,13 @@
         <v>38</v>
       </c>
       <c r="B9" s="21" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="C9" s="21" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="D9" s="21" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="N9" s="21" t="s">
         <v>0</v>
@@ -4372,7 +4369,7 @@
         <v>29</v>
       </c>
       <c r="R9" s="22" t="s">
-        <v>408</v>
+        <v>438</v>
       </c>
       <c r="S9" s="22"/>
       <c r="T9" s="22"/>
@@ -4389,13 +4386,13 @@
         <v>0</v>
       </c>
       <c r="AB9" s="21" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="AH9" s="18" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="AI9" s="18" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="AJ9" s="18"/>
       <c r="AK9" s="18"/>
@@ -4421,7 +4418,7 @@
         <v>0</v>
       </c>
       <c r="BA9" s="21" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="BB9" s="21" t="s">
         <v>37</v>
@@ -4475,7 +4472,7 @@
         <v>0</v>
       </c>
       <c r="CE9" s="21" t="s">
-        <v>432</v>
+        <v>421</v>
       </c>
       <c r="CF9" s="21" t="s">
         <v>75</v>
@@ -4505,7 +4502,7 @@
         <v>137</v>
       </c>
       <c r="CR9" s="21" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="CS9" s="21" t="s">
         <v>137</v>
@@ -4605,7 +4602,7 @@
         <v>137</v>
       </c>
       <c r="EK9" s="27" t="s">
-        <v>425</v>
+        <v>414</v>
       </c>
       <c r="EL9" s="21" t="s">
         <v>137</v>
@@ -4628,25 +4625,25 @@
         <v>134</v>
       </c>
       <c r="E10" s="21" t="s">
-        <v>426</v>
+        <v>415</v>
       </c>
       <c r="F10" s="21" t="s">
-        <v>431</v>
+        <v>420</v>
       </c>
       <c r="G10" s="21" t="s">
-        <v>427</v>
+        <v>416</v>
       </c>
       <c r="H10" s="21" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="I10" s="21" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="J10" s="21" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="K10" s="21" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="M10" s="21" t="s">
         <v>0</v>
@@ -4664,7 +4661,7 @@
         <v>27</v>
       </c>
       <c r="R10" s="22" t="s">
-        <v>411</v>
+        <v>439</v>
       </c>
       <c r="S10" s="22"/>
       <c r="T10" s="22"/>
@@ -4694,10 +4691,10 @@
         <v>28907</v>
       </c>
       <c r="AH10" s="19" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="AI10" s="18" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="AJ10" s="18"/>
       <c r="AK10" s="18"/>
@@ -4744,7 +4741,7 @@
         <v>0</v>
       </c>
       <c r="BA10" s="21" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="BB10" s="21" t="s">
         <v>37</v>
@@ -4786,7 +4783,7 @@
         <v>149</v>
       </c>
       <c r="BO10" s="22" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="BQ10" s="21" t="s">
         <v>0</v>
@@ -4813,16 +4810,16 @@
         <v>0</v>
       </c>
       <c r="CE10" s="21" t="s">
-        <v>432</v>
+        <v>421</v>
       </c>
       <c r="CF10" s="21" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="CG10" s="21" t="s">
         <v>73</v>
       </c>
       <c r="CH10" s="21" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="CI10" s="21" t="s">
         <v>73</v>
@@ -4864,7 +4861,7 @@
         <v>103</v>
       </c>
       <c r="CX10" s="21" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="CY10" s="21" t="s">
         <v>82</v>
@@ -4978,7 +4975,7 @@
         <v>0</v>
       </c>
       <c r="EK10" s="27" t="s">
-        <v>425</v>
+        <v>414</v>
       </c>
       <c r="EL10" s="21" t="s">
         <v>0</v>
@@ -5001,28 +4998,28 @@
         <v>134</v>
       </c>
       <c r="E11" s="21" t="s">
-        <v>413</v>
+        <v>405</v>
       </c>
       <c r="F11" s="21" t="s">
-        <v>430</v>
+        <v>419</v>
       </c>
       <c r="G11" s="21" t="s">
-        <v>414</v>
+        <v>406</v>
       </c>
       <c r="H11" s="21" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="I11" s="21" t="s">
         <v>136</v>
       </c>
       <c r="J11" s="21" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="K11" s="21" t="s">
         <v>48</v>
       </c>
       <c r="L11" s="21" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="M11" s="21" t="s">
         <v>137</v>
@@ -5040,7 +5037,7 @@
         <v>21</v>
       </c>
       <c r="R11" s="22" t="s">
-        <v>412</v>
+        <v>440</v>
       </c>
       <c r="S11" s="22"/>
       <c r="T11" s="22"/>
@@ -5054,10 +5051,10 @@
         <v>169</v>
       </c>
       <c r="AH11" s="18" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="AI11" s="19" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="AJ11" s="19"/>
       <c r="AK11" s="19"/>
@@ -5108,7 +5105,7 @@
         <v>0</v>
       </c>
       <c r="CE11" s="21" t="s">
-        <v>432</v>
+        <v>421</v>
       </c>
       <c r="CF11" s="21" t="s">
         <v>75</v>
@@ -5151,7 +5148,7 @@
       </c>
       <c r="CV11" s="24"/>
       <c r="CX11" s="21" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="CY11" s="21" t="s">
         <v>82</v>
@@ -5163,7 +5160,7 @@
         <v>174</v>
       </c>
       <c r="DE11" s="21" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="DF11" s="21" t="s">
         <v>175</v>
@@ -5175,7 +5172,7 @@
         <v>109</v>
       </c>
       <c r="DI11" s="21" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="DJ11" s="21" t="s">
         <v>178</v>
@@ -5256,7 +5253,7 @@
         <v>137</v>
       </c>
       <c r="EK11" s="27" t="s">
-        <v>425</v>
+        <v>414</v>
       </c>
       <c r="EL11" s="21" t="s">
         <v>137</v>
@@ -5279,25 +5276,25 @@
         <v>134</v>
       </c>
       <c r="E12" s="21" t="s">
-        <v>415</v>
+        <v>407</v>
       </c>
       <c r="F12" s="21" t="s">
-        <v>428</v>
+        <v>417</v>
       </c>
       <c r="G12" s="21" t="s">
-        <v>417</v>
+        <v>409</v>
       </c>
       <c r="H12" s="21" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="I12" s="21" t="s">
         <v>162</v>
       </c>
       <c r="J12" s="21" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="K12" s="21" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="M12" s="21" t="s">
         <v>0</v>
@@ -5315,7 +5312,7 @@
         <v>30</v>
       </c>
       <c r="R12" s="22" t="s">
-        <v>407</v>
+        <v>437</v>
       </c>
       <c r="S12" s="22"/>
       <c r="T12" s="22"/>
@@ -5326,13 +5323,13 @@
         <v>137</v>
       </c>
       <c r="AB12" s="21" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="AH12" s="19" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="AI12" s="19" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="AJ12" s="19"/>
       <c r="AK12" s="19"/>
@@ -5367,7 +5364,7 @@
         <v>137</v>
       </c>
       <c r="CE12" s="21" t="s">
-        <v>432</v>
+        <v>421</v>
       </c>
       <c r="CL12" s="21" t="s">
         <v>137</v>
@@ -5380,7 +5377,7 @@
         <v>109</v>
       </c>
       <c r="DI12" s="21" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="DJ12" s="21" t="s">
         <v>178</v>
@@ -5461,7 +5458,7 @@
         <v>137</v>
       </c>
       <c r="EK12" s="27" t="s">
-        <v>425</v>
+        <v>414</v>
       </c>
       <c r="EL12" s="21" t="s">
         <v>137</v>
@@ -5484,22 +5481,22 @@
         <v>134</v>
       </c>
       <c r="E13" s="21" t="s">
-        <v>416</v>
+        <v>408</v>
       </c>
       <c r="F13" s="21" t="s">
-        <v>429</v>
+        <v>418</v>
       </c>
       <c r="G13" s="21" t="s">
-        <v>418</v>
+        <v>410</v>
       </c>
       <c r="H13" s="21" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="I13" s="21" t="s">
         <v>164</v>
       </c>
       <c r="J13" s="21" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="K13" s="21" t="s">
         <v>88</v>
@@ -5520,7 +5517,7 @@
         <v>21</v>
       </c>
       <c r="R13" s="22" t="s">
-        <v>299</v>
+        <v>441</v>
       </c>
       <c r="S13" s="22"/>
       <c r="T13" s="22"/>
@@ -5531,13 +5528,13 @@
         <v>0</v>
       </c>
       <c r="AB13" s="21" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="AH13" s="19" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="AI13" s="19" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="AJ13" s="19"/>
       <c r="AK13" s="19"/>
@@ -5569,7 +5566,7 @@
         <v>148</v>
       </c>
       <c r="CE13" s="21" t="s">
-        <v>432</v>
+        <v>421</v>
       </c>
       <c r="CF13" s="21" t="s">
         <v>75</v>
@@ -5653,7 +5650,7 @@
         <v>148</v>
       </c>
       <c r="EK13" s="27" t="s">
-        <v>425</v>
+        <v>414</v>
       </c>
       <c r="EL13" s="21" t="s">
         <v>148</v>
@@ -5673,39 +5670,39 @@
     </row>
     <row r="14" spans="1:146" s="21" customFormat="1" ht="88" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K14" s="25" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="AH14" s="19" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="AI14" s="19" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="AJ14" s="19"/>
       <c r="AK14" s="19"/>
     </row>
     <row r="15" spans="1:146" s="21" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="K15" s="21" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="AH15" s="19" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="AI15" s="19" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="AJ15" s="19"/>
       <c r="AK15" s="19"/>
     </row>
     <row r="16" spans="1:146" s="21" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="K16" s="21" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="AH16" s="19" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="AI16" s="19" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="AJ16" s="19"/>
       <c r="AK16" s="19"/>
@@ -5715,10 +5712,10 @@
         <v>142</v>
       </c>
       <c r="AH17" s="19" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="AI17" s="19" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="AJ17" s="19"/>
       <c r="AK17" s="19"/>
@@ -5785,25 +5782,25 @@
   <sheetData>
     <row r="1" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B1" s="5" t="s">
+        <v>276</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>277</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="D1" s="5" t="s">
         <v>278</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="E1" s="5" t="s">
         <v>279</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="F1" s="5" t="s">
         <v>280</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="G1" s="5" t="s">
         <v>281</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>282</v>
       </c>
       <c r="H1" s="5" t="s">
         <v>126</v>
@@ -5812,7 +5809,7 @@
         <v>127</v>
       </c>
       <c r="J1" s="5" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="17" x14ac:dyDescent="0.2">
@@ -5820,7 +5817,7 @@
         <v>37</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>60</v>
@@ -5849,10 +5846,10 @@
         <v>44</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>62</v>
@@ -5873,7 +5870,7 @@
         <v>1991</v>
       </c>
       <c r="J3" s="6" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="17" x14ac:dyDescent="0.2">
@@ -5881,10 +5878,10 @@
         <v>44</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>132</v>
@@ -5905,7 +5902,7 @@
         <v>1992</v>
       </c>
       <c r="J4" s="6" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="17" x14ac:dyDescent="0.2">
@@ -5913,19 +5910,19 @@
         <v>48</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="E5" s="4">
         <v>3013454562</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="G5" s="4" t="s">
         <v>0</v>
@@ -5937,7 +5934,7 @@
         <v>1993</v>
       </c>
       <c r="J5" s="6" t="s">
-        <v>422</v>
+        <v>411</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="17" x14ac:dyDescent="0.2">
@@ -5945,19 +5942,19 @@
         <v>48</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="E6" s="4">
         <v>3013454562</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="G6" s="4" t="s">
         <v>0</v>
@@ -5969,7 +5966,7 @@
         <v>1994</v>
       </c>
       <c r="J6" s="6" t="s">
-        <v>423</v>
+        <v>412</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="17" x14ac:dyDescent="0.2">
@@ -5977,19 +5974,19 @@
         <v>48</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="E7" s="4">
         <v>3013454562</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="G7" s="4" t="s">
         <v>0</v>
@@ -6001,12 +5998,12 @@
         <v>1995</v>
       </c>
       <c r="J7" s="6" t="s">
-        <v>424</v>
+        <v>413</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="I12" s="6" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
   </sheetData>
@@ -6121,16 +6118,16 @@
         <v>137</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="17" x14ac:dyDescent="0.2">
@@ -6138,7 +6135,7 @@
         <v>176</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>173</v>
@@ -6150,24 +6147,24 @@
         <v>137</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
+        <v>284</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>285</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>286</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>79</v>
@@ -6181,24 +6178,24 @@
         <v>0</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="51" x14ac:dyDescent="0.2">
       <c r="A6" s="20" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="B6" s="20" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="C6" s="20" t="s">
         <v>78</v>
@@ -6214,24 +6211,24 @@
         <v>0</v>
       </c>
       <c r="H6" s="20" t="s">
+        <v>338</v>
+      </c>
+      <c r="I6" s="20" t="s">
+        <v>339</v>
+      </c>
+      <c r="J6" s="20" t="s">
         <v>340</v>
       </c>
-      <c r="I6" s="20" t="s">
+      <c r="K6" s="20" t="s">
         <v>341</v>
-      </c>
-      <c r="J6" s="20" t="s">
-        <v>342</v>
-      </c>
-      <c r="K6" s="20" t="s">
-        <v>343</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="34" x14ac:dyDescent="0.2">
       <c r="A7" s="20" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="B7" s="20" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="C7" s="20" t="s">
         <v>79</v>
@@ -6245,16 +6242,16 @@
         <v>137</v>
       </c>
       <c r="H7" s="20" t="s">
+        <v>342</v>
+      </c>
+      <c r="I7" s="20" t="s">
+        <v>343</v>
+      </c>
+      <c r="J7" s="20" t="s">
         <v>344</v>
       </c>
-      <c r="I7" s="20" t="s">
+      <c r="K7" s="20" t="s">
         <v>345</v>
-      </c>
-      <c r="J7" s="20" t="s">
-        <v>346</v>
-      </c>
-      <c r="K7" s="20" t="s">
-        <v>347</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="17" x14ac:dyDescent="0.2">
@@ -6262,7 +6259,7 @@
         <v>190</v>
       </c>
       <c r="B8" s="20" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="C8" s="20" t="s">
         <v>173</v>
@@ -6274,24 +6271,24 @@
         <v>137</v>
       </c>
       <c r="H8" s="20" t="s">
+        <v>346</v>
+      </c>
+      <c r="I8" s="20" t="s">
+        <v>347</v>
+      </c>
+      <c r="J8" s="20" t="s">
         <v>348</v>
       </c>
-      <c r="I8" s="20" t="s">
+      <c r="K8" s="20" t="s">
         <v>349</v>
-      </c>
-      <c r="J8" s="20" t="s">
-        <v>350</v>
-      </c>
-      <c r="K8" s="20" t="s">
-        <v>351</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="34" x14ac:dyDescent="0.2">
       <c r="A9" s="20" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="B9" s="20" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="C9" s="20" t="s">
         <v>79</v>
@@ -6305,16 +6302,16 @@
         <v>0</v>
       </c>
       <c r="H9" s="20" t="s">
+        <v>350</v>
+      </c>
+      <c r="I9" s="20" t="s">
+        <v>351</v>
+      </c>
+      <c r="J9" s="20" t="s">
         <v>352</v>
       </c>
-      <c r="I9" s="20" t="s">
+      <c r="K9" s="20" t="s">
         <v>353</v>
-      </c>
-      <c r="J9" s="20" t="s">
-        <v>354</v>
-      </c>
-      <c r="K9" s="20" t="s">
-        <v>355</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
CHARMS - Fanconi CGB IIQ data verification in Native View
</commit_message>
<xml_diff>
--- a/src/test/java/CHARMS/resources/data.xlsx
+++ b/src/test/java/CHARMS/resources/data.xlsx
@@ -5,17 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jains18/git/CBIIT-Test-Automation/CBIIT-Test-Automation/src/test/java/CHARMS/Resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/muzipovay2/AquaProjects/CBIIT-Test-Automation/src/test/java/CHARMS/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEB6D4EE-562D-834F-91FE-8C3F1DEBBD78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03F5B58D-9188-D341-ABD0-7139A7806C49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4280" yWindow="500" windowWidth="26000" windowHeight="17640" xr2:uid="{B3E53782-D40D-CC47-BA00-27DFD8C445AF}"/>
+    <workbookView xWindow="4240" yWindow="760" windowWidth="26000" windowHeight="17600" activeTab="3" xr2:uid="{B3E53782-D40D-CC47-BA00-27DFD8C445AF}"/>
   </bookViews>
   <sheets>
     <sheet name="FanconiScreener" sheetId="1" r:id="rId1"/>
     <sheet name="OtherStudies" sheetId="3" r:id="rId2"/>
     <sheet name="Cancer" sheetId="6" r:id="rId3"/>
+    <sheet name="fanconiScreenerScenario" sheetId="7" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">FanconiScreener!$A$1:$EP$13</definedName>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1223" uniqueCount="443">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1292" uniqueCount="491">
   <si>
     <t>Yes</t>
   </si>
@@ -1370,6 +1371,153 @@
   </si>
   <si>
     <t>CalculatedAge</t>
+  </si>
+  <si>
+    <t>Question</t>
+  </si>
+  <si>
+    <t>Answer</t>
+  </si>
+  <si>
+    <t>Are you completing this form for someone else or for yourself?</t>
+  </si>
+  <si>
+    <t>I am completing this form for myself</t>
+  </si>
+  <si>
+    <t>First name</t>
+  </si>
+  <si>
+    <t>Middle Initial</t>
+  </si>
+  <si>
+    <t>Last name</t>
+  </si>
+  <si>
+    <t>What is your date of birth?</t>
+  </si>
+  <si>
+    <t>Date of birth month</t>
+  </si>
+  <si>
+    <t>Date of birth year</t>
+  </si>
+  <si>
+    <t>What was your sex assigned at birth?</t>
+  </si>
+  <si>
+    <t>Are you adopted?</t>
+  </si>
+  <si>
+    <t>In which country do you currently live?</t>
+  </si>
+  <si>
+    <t>Please provide the mailing address where study materials can be sent, as needed.</t>
+  </si>
+  <si>
+    <t>Street</t>
+  </si>
+  <si>
+    <t>12-34 home address</t>
+  </si>
+  <si>
+    <t>Street 2 (optional)</t>
+  </si>
+  <si>
+    <t>Apt 600</t>
+  </si>
+  <si>
+    <t>Burke</t>
+  </si>
+  <si>
+    <t>State (Abbreviation)</t>
+  </si>
+  <si>
+    <t>VA</t>
+  </si>
+  <si>
+    <t>Zip Code</t>
+  </si>
+  <si>
+    <t>What is your email address?</t>
+  </si>
+  <si>
+    <t>Please confirm your email address</t>
+  </si>
+  <si>
+    <t>Home phone number</t>
+  </si>
+  <si>
+    <t>Cell phone number</t>
+  </si>
+  <si>
+    <t>Work phone number</t>
+  </si>
+  <si>
+    <t>What is your ethnicity?</t>
+  </si>
+  <si>
+    <t>What is your race? Please select all that apply.</t>
+  </si>
+  <si>
+    <t>Are you a participant in any other research study or registry group?  Please specify.</t>
+  </si>
+  <si>
+    <t>I am not involved in any other research study or registry group</t>
+  </si>
+  <si>
+    <t>Have you ever been diagnosed with the following conditions?  Select all that apply.  If you do not see the exact condition diagnosed, please select the closest answer.</t>
+  </si>
+  <si>
+    <t>Never diagnosed with any of these conditions</t>
+  </si>
+  <si>
+    <t>Have you ever been diagnosed with cancer?</t>
+  </si>
+  <si>
+    <t>Have you been diagnosed with a RASopathy such as Noonan syndrome, Noonan syndrome with multiple lentigines, Costello syndrome, cardiofaciocutaneous syndrome, Legius syndrome, capillary arteriovenous malformation syndrome, hereditary gingival fibromatosis or SYNGAP1 syndrome?</t>
+  </si>
+  <si>
+    <t>Have any of your biological relatives been diagnosed with a RASopathy?</t>
+  </si>
+  <si>
+    <t>Have you ever had genetic testing?</t>
+  </si>
+  <si>
+    <t>How did you hear about this study?  If a specific health care provider referred you to this study, please include their name in the corresponding text box.</t>
+  </si>
+  <si>
+    <t>How did you hear about this study?  If a specific health care provider referred you to this study, please include their name in the corresponding text box. Other reason</t>
+  </si>
+  <si>
+    <t>JUST TESTING</t>
+  </si>
+  <si>
+    <t>Have you or other family members ever participated in another study on RASopathies at another medical institution, university, government agency or other site?</t>
+  </si>
+  <si>
+    <t>What are the main reasons for participating in this study?  Select all that apply.  Please elaborate on the reason in the corresponding textbox.</t>
+  </si>
+  <si>
+    <t>What are the main reasons for participating in this study?  Select all that apply.  Please elaborate on the reason in the corresponding textbox. Other reason</t>
+  </si>
+  <si>
+    <t>TESTING REASONS</t>
+  </si>
+  <si>
+    <t>You are almost done!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You are almost done!
+  To submit your responses, you must continue in the questionnaire by clicking the forward arrow below.  
+The information you have provided will be reviewed by our study team.  If it is determined that you are eligible to participate in the RASopathy Study, you will receive an email with further details, including instructions to log in to a secure study portal. If the team decides that you are not eligible, you will receive an email explaining why. In the meantime, you should receive an email confirming this submission.
+  Please feel free to call at any time if you have any questions regarding this protocol and ask to speak with the RASopathies Study nurse. Our toll-free phone number is 1-800-518-8474 or 301-212-5250. Thank you for your willingness to consider joining our research effort.  We could not do vital studies like this without the help of dedicated patients and families.  </t>
+  </si>
+  <si>
+    <t>April 1, 1948</t>
+  </si>
+  <si>
+    <t>301-577-4089</t>
   </si>
 </sst>
 </file>
@@ -1579,7 +1727,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1659,6 +1807,25 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1989,9 +2156,9 @@
   </sheetPr>
   <dimension ref="A1:EP18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="113" workbookViewId="0">
+    <sheetView topLeftCell="AI1" zoomScale="113" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K2" sqref="K2"/>
+      <selection pane="bottomLeft" activeCell="AK2" sqref="AK2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6321,4 +6488,312 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6599F052-5E19-A342-980D-0163BD929DAC}">
+  <dimension ref="A1:B36"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="98.5" customWidth="1"/>
+    <col min="2" max="2" width="53" style="31" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="28" t="s">
+        <v>443</v>
+      </c>
+      <c r="B1" s="29" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A2" s="30" t="s">
+        <v>445</v>
+      </c>
+      <c r="B2" s="31" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="28" t="s">
+        <v>447</v>
+      </c>
+      <c r="B3" s="31" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="28" t="s">
+        <v>448</v>
+      </c>
+      <c r="B4" s="31" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="28" t="s">
+        <v>449</v>
+      </c>
+      <c r="B5" s="31" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="28" t="s">
+        <v>450</v>
+      </c>
+      <c r="B6" s="32" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="28" t="s">
+        <v>451</v>
+      </c>
+      <c r="B7" s="31" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="28" t="s">
+        <v>452</v>
+      </c>
+      <c r="B8" s="31">
+        <v>1948</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="28" t="s">
+        <v>453</v>
+      </c>
+      <c r="B9" s="31" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" s="28" t="s">
+        <v>454</v>
+      </c>
+      <c r="B10" s="31" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" s="28" t="s">
+        <v>455</v>
+      </c>
+      <c r="B11" s="31" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A12" s="30" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" s="28" t="s">
+        <v>457</v>
+      </c>
+      <c r="B13" s="31" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" s="28" t="s">
+        <v>459</v>
+      </c>
+      <c r="B14" s="31" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="B15" s="31" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" s="28" t="s">
+        <v>462</v>
+      </c>
+      <c r="B16" s="31" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" s="28" t="s">
+        <v>464</v>
+      </c>
+      <c r="B17" s="31">
+        <v>22015</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" s="28" t="s">
+        <v>465</v>
+      </c>
+      <c r="B18" s="33" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" s="28" t="s">
+        <v>466</v>
+      </c>
+      <c r="B19" s="33" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" s="28" t="s">
+        <v>467</v>
+      </c>
+      <c r="B20" s="31" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" s="28" t="s">
+        <v>468</v>
+      </c>
+      <c r="B21" s="31" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" s="28" t="s">
+        <v>469</v>
+      </c>
+      <c r="B22" s="31" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" s="28" t="s">
+        <v>470</v>
+      </c>
+      <c r="B23" s="31" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A24" s="30" t="s">
+        <v>471</v>
+      </c>
+      <c r="B24" s="31" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A25" s="30" t="s">
+        <v>472</v>
+      </c>
+      <c r="B25" s="31" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" ht="34" x14ac:dyDescent="0.2">
+      <c r="A26" s="30" t="s">
+        <v>474</v>
+      </c>
+      <c r="B26" s="31" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A27" s="30" t="s">
+        <v>476</v>
+      </c>
+      <c r="B27" s="31" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" ht="51" x14ac:dyDescent="0.2">
+      <c r="A28" s="30" t="s">
+        <v>477</v>
+      </c>
+      <c r="B28" s="31" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A29" s="30" t="s">
+        <v>478</v>
+      </c>
+      <c r="B29" s="31" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A30" s="30" t="s">
+        <v>479</v>
+      </c>
+      <c r="B30" s="31" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" ht="34" x14ac:dyDescent="0.2">
+      <c r="A31" s="30" t="s">
+        <v>480</v>
+      </c>
+      <c r="B31" s="31" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" ht="34" x14ac:dyDescent="0.2">
+      <c r="A32" s="30" t="s">
+        <v>481</v>
+      </c>
+      <c r="B32" s="31" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" ht="34" x14ac:dyDescent="0.2">
+      <c r="A33" s="30" t="s">
+        <v>483</v>
+      </c>
+      <c r="B33" s="31" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" ht="34" x14ac:dyDescent="0.2">
+      <c r="A34" s="30" t="s">
+        <v>484</v>
+      </c>
+      <c r="B34" s="31" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" ht="34" x14ac:dyDescent="0.2">
+      <c r="A35" s="30" t="s">
+        <v>485</v>
+      </c>
+      <c r="B35" s="31" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" ht="323" x14ac:dyDescent="0.2">
+      <c r="A36" s="30" t="s">
+        <v>487</v>
+      </c>
+      <c r="B36" s="34" t="s">
+        <v>488</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B18" r:id="rId1" display="charmsras1@yahoo.com" xr:uid="{6EA70FB0-A297-224B-9C86-78BA30550547}"/>
+    <hyperlink ref="B19" r:id="rId2" display="charmsras1@yahoo.com" xr:uid="{E702EB55-FE21-CB44-8DAD-949BFDA9CB44}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added Cancer data to Fanconi screener Assertion in NativeView
</commit_message>
<xml_diff>
--- a/src/test/java/CHARMS/resources/data.xlsx
+++ b/src/test/java/CHARMS/resources/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jains18/git/CBIIT-Test-Automation/CBIIT-Test-Automation/src/test/java/CHARMS/Resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8656CF68-2071-6B48-A1DE-CD7E39F5E3A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD510F4C-0F77-D141-9D77-033EC4DE5609}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4240" yWindow="760" windowWidth="26000" windowHeight="17640" xr2:uid="{B3E53782-D40D-CC47-BA00-27DFD8C445AF}"/>
+    <workbookView xWindow="720" yWindow="800" windowWidth="26000" windowHeight="17640" xr2:uid="{B3E53782-D40D-CC47-BA00-27DFD8C445AF}"/>
   </bookViews>
   <sheets>
     <sheet name="FanconiScreener" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1222" uniqueCount="442">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1229" uniqueCount="443">
   <si>
     <t>Yes</t>
   </si>
@@ -379,9 +379,6 @@
     <t>Physician</t>
   </si>
   <si>
-    <t xml:space="preserve">Physician Tester </t>
-  </si>
-  <si>
     <t>HealthCareProviderName</t>
   </si>
   <si>
@@ -400,9 +397,6 @@
     <t>Other Test Reason</t>
   </si>
   <si>
-    <t xml:space="preserve">Receive Genetic Test reason </t>
-  </si>
-  <si>
     <t>Cancer diagnosis Reason</t>
   </si>
   <si>
@@ -1367,6 +1361,15 @@
   </si>
   <si>
     <t>January</t>
+  </si>
+  <si>
+    <t>Receive Genetic Test reason</t>
+  </si>
+  <si>
+    <t>Physician Tester</t>
+  </si>
+  <si>
+    <t>01/21/1948</t>
   </si>
 </sst>
 </file>
@@ -1576,7 +1579,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1655,6 +1658,24 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1986,9 +2007,9 @@
   </sheetPr>
   <dimension ref="A1:EP18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="113" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P2" sqref="P2:P13"/>
+    <sheetView tabSelected="1" topLeftCell="N1" zoomScale="113" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="T2" sqref="T2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2007,7 +2028,8 @@
     <col min="15" max="15" width="8.5" style="3" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="10.1640625" style="3" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="7.83203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="18" max="20" width="13.33203125" style="3" customWidth="1"/>
+    <col min="18" max="18" width="13.33203125" style="33" customWidth="1"/>
+    <col min="19" max="20" width="13.33203125" style="3" customWidth="1"/>
     <col min="21" max="21" width="16" style="3" customWidth="1"/>
     <col min="22" max="22" width="13.1640625" style="3" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="13.1640625" style="3" customWidth="1"/>
@@ -2050,46 +2072,46 @@
   <sheetData>
     <row r="1" spans="1:146" s="13" customFormat="1" ht="85" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
+        <v>190</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>191</v>
+      </c>
+      <c r="C1" s="7" t="s">
         <v>192</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="D1" s="7" t="s">
         <v>193</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="E1" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="I1" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="J1" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="K1" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="L1" s="7" t="s">
+        <v>372</v>
+      </c>
+      <c r="M1" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="N1" s="8" t="s">
         <v>194</v>
-      </c>
-      <c r="D1" s="7" t="s">
-        <v>195</v>
-      </c>
-      <c r="E1" s="7" t="s">
-        <v>128</v>
-      </c>
-      <c r="F1" s="7" t="s">
-        <v>129</v>
-      </c>
-      <c r="G1" s="7" t="s">
-        <v>130</v>
-      </c>
-      <c r="H1" s="7" t="s">
-        <v>137</v>
-      </c>
-      <c r="I1" s="7" t="s">
-        <v>138</v>
-      </c>
-      <c r="J1" s="7" t="s">
-        <v>139</v>
-      </c>
-      <c r="K1" s="7" t="s">
-        <v>140</v>
-      </c>
-      <c r="L1" s="7" t="s">
-        <v>374</v>
-      </c>
-      <c r="M1" s="7" t="s">
-        <v>142</v>
-      </c>
-      <c r="N1" s="8" t="s">
-        <v>196</v>
       </c>
       <c r="O1" s="9" t="s">
         <v>1</v>
@@ -2100,14 +2122,14 @@
       <c r="Q1" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="R1" s="9" t="s">
-        <v>127</v>
+      <c r="R1" s="30" t="s">
+        <v>125</v>
       </c>
       <c r="S1" s="9" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="T1" s="9" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="U1" s="10" t="s">
         <v>4</v>
@@ -2116,19 +2138,19 @@
         <v>5</v>
       </c>
       <c r="W1" s="10" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="X1" s="10" t="s">
         <v>6</v>
       </c>
       <c r="Y1" s="10" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="Z1" s="11" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="AA1" s="11" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="AB1" s="7" t="s">
         <v>7</v>
@@ -2155,10 +2177,10 @@
         <v>39</v>
       </c>
       <c r="AJ1" s="12" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="AK1" s="12" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="AL1" s="14" t="s">
         <v>14</v>
@@ -2197,16 +2219,16 @@
         <v>19</v>
       </c>
       <c r="AX1" s="15" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="AY1" s="15" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="AZ1" s="16" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="BA1" s="16" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="BB1" s="16" t="s">
         <v>53</v>
@@ -2242,58 +2264,58 @@
         <v>52</v>
       </c>
       <c r="BM1" s="13" t="s">
+        <v>201</v>
+      </c>
+      <c r="BN1" s="13" t="s">
+        <v>205</v>
+      </c>
+      <c r="BO1" s="13" t="s">
+        <v>206</v>
+      </c>
+      <c r="BP1" s="13" t="s">
+        <v>207</v>
+      </c>
+      <c r="BQ1" s="13" t="s">
+        <v>202</v>
+      </c>
+      <c r="BR1" s="13" t="s">
         <v>203</v>
       </c>
-      <c r="BN1" s="13" t="s">
-        <v>207</v>
-      </c>
-      <c r="BO1" s="13" t="s">
+      <c r="BS1" s="13" t="s">
+        <v>204</v>
+      </c>
+      <c r="BT1" s="13" t="s">
+        <v>362</v>
+      </c>
+      <c r="BU1" s="13" t="s">
+        <v>361</v>
+      </c>
+      <c r="BV1" s="13" t="s">
+        <v>209</v>
+      </c>
+      <c r="BW1" s="13" t="s">
+        <v>263</v>
+      </c>
+      <c r="BX1" s="13" t="s">
+        <v>264</v>
+      </c>
+      <c r="BY1" s="13" t="s">
         <v>208</v>
       </c>
-      <c r="BP1" s="13" t="s">
-        <v>209</v>
-      </c>
-      <c r="BQ1" s="13" t="s">
-        <v>204</v>
-      </c>
-      <c r="BR1" s="13" t="s">
-        <v>205</v>
-      </c>
-      <c r="BS1" s="13" t="s">
-        <v>206</v>
-      </c>
-      <c r="BT1" s="13" t="s">
-        <v>364</v>
-      </c>
-      <c r="BU1" s="13" t="s">
+      <c r="BZ1" s="13" t="s">
+        <v>210</v>
+      </c>
+      <c r="CA1" s="13" t="s">
+        <v>211</v>
+      </c>
+      <c r="CB1" s="13" t="s">
         <v>363</v>
       </c>
-      <c r="BV1" s="13" t="s">
-        <v>211</v>
-      </c>
-      <c r="BW1" s="13" t="s">
-        <v>265</v>
-      </c>
-      <c r="BX1" s="13" t="s">
-        <v>266</v>
-      </c>
-      <c r="BY1" s="13" t="s">
-        <v>210</v>
-      </c>
-      <c r="BZ1" s="13" t="s">
-        <v>212</v>
-      </c>
-      <c r="CA1" s="13" t="s">
-        <v>213</v>
-      </c>
-      <c r="CB1" s="13" t="s">
-        <v>365</v>
-      </c>
       <c r="CC1" s="13" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="CD1" s="13" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="CE1" s="13" t="s">
         <v>67</v>
@@ -2311,49 +2333,49 @@
         <v>71</v>
       </c>
       <c r="CJ1" s="13" t="s">
+        <v>212</v>
+      </c>
+      <c r="CK1" s="13" t="s">
+        <v>213</v>
+      </c>
+      <c r="CL1" s="13" t="s">
         <v>214</v>
       </c>
-      <c r="CK1" s="13" t="s">
+      <c r="CM1" s="13" t="s">
         <v>215</v>
       </c>
-      <c r="CL1" s="13" t="s">
+      <c r="CN1" s="13" t="s">
+        <v>237</v>
+      </c>
+      <c r="CO1" s="13" t="s">
+        <v>238</v>
+      </c>
+      <c r="CP1" s="13" t="s">
+        <v>239</v>
+      </c>
+      <c r="CQ1" s="13" t="s">
+        <v>240</v>
+      </c>
+      <c r="CR1" s="13" t="s">
+        <v>241</v>
+      </c>
+      <c r="CS1" s="13" t="s">
         <v>216</v>
       </c>
-      <c r="CM1" s="13" t="s">
+      <c r="CT1" s="13" t="s">
         <v>217</v>
       </c>
-      <c r="CN1" s="13" t="s">
-        <v>239</v>
-      </c>
-      <c r="CO1" s="13" t="s">
-        <v>240</v>
-      </c>
-      <c r="CP1" s="13" t="s">
-        <v>241</v>
-      </c>
-      <c r="CQ1" s="13" t="s">
-        <v>242</v>
-      </c>
-      <c r="CR1" s="13" t="s">
-        <v>243</v>
-      </c>
-      <c r="CS1" s="13" t="s">
-        <v>218</v>
-      </c>
-      <c r="CT1" s="13" t="s">
-        <v>219</v>
-      </c>
       <c r="CU1" s="13" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="CV1" s="13" t="s">
+        <v>226</v>
+      </c>
+      <c r="CW1" s="13" t="s">
+        <v>225</v>
+      </c>
+      <c r="CX1" s="13" t="s">
         <v>228</v>
-      </c>
-      <c r="CW1" s="13" t="s">
-        <v>227</v>
-      </c>
-      <c r="CX1" s="13" t="s">
-        <v>230</v>
       </c>
       <c r="CY1" s="13" t="s">
         <v>80</v>
@@ -2380,112 +2402,112 @@
         <v>91</v>
       </c>
       <c r="DG1" s="13" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="DH1" s="13" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="DI1" s="13" t="s">
         <v>109</v>
       </c>
       <c r="DJ1" s="13" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="DK1" s="13" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="DL1" s="13" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="DM1" s="13" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="DN1" s="13" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="DO1" s="13" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="DP1" s="13" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="DQ1" s="13" t="s">
+        <v>229</v>
+      </c>
+      <c r="DR1" s="13" t="s">
+        <v>230</v>
+      </c>
+      <c r="DS1" s="13" t="s">
         <v>231</v>
       </c>
-      <c r="DR1" s="13" t="s">
+      <c r="DT1" s="13" t="s">
         <v>232</v>
       </c>
-      <c r="DS1" s="13" t="s">
+      <c r="DU1" s="13" t="s">
         <v>233</v>
       </c>
-      <c r="DT1" s="13" t="s">
+      <c r="DV1" s="13" t="s">
         <v>234</v>
       </c>
-      <c r="DU1" s="13" t="s">
+      <c r="DW1" s="13" t="s">
         <v>235</v>
       </c>
-      <c r="DV1" s="13" t="s">
+      <c r="DX1" s="13" t="s">
         <v>236</v>
       </c>
-      <c r="DW1" s="13" t="s">
-        <v>237</v>
-      </c>
-      <c r="DX1" s="13" t="s">
-        <v>238</v>
-      </c>
       <c r="DY1" s="17" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="DZ1" s="17" t="s">
+        <v>245</v>
+      </c>
+      <c r="EA1" s="17" t="s">
+        <v>246</v>
+      </c>
+      <c r="EB1" s="17" t="s">
         <v>247</v>
       </c>
-      <c r="EA1" s="17" t="s">
+      <c r="EC1" s="17" t="s">
         <v>248</v>
       </c>
-      <c r="EB1" s="17" t="s">
+      <c r="ED1" s="17" t="s">
         <v>249</v>
       </c>
-      <c r="EC1" s="17" t="s">
+      <c r="EE1" s="17" t="s">
         <v>250</v>
       </c>
-      <c r="ED1" s="17" t="s">
+      <c r="EF1" s="17" t="s">
         <v>251</v>
       </c>
-      <c r="EE1" s="17" t="s">
+      <c r="EG1" s="17" t="s">
         <v>252</v>
       </c>
-      <c r="EF1" s="17" t="s">
+      <c r="EH1" s="17" t="s">
         <v>253</v>
       </c>
-      <c r="EG1" s="17" t="s">
+      <c r="EI1" s="17" t="s">
         <v>254</v>
       </c>
-      <c r="EH1" s="17" t="s">
+      <c r="EJ1" s="17" t="s">
+        <v>256</v>
+      </c>
+      <c r="EK1" s="17" t="s">
         <v>255</v>
       </c>
-      <c r="EI1" s="17" t="s">
-        <v>256</v>
-      </c>
-      <c r="EJ1" s="17" t="s">
+      <c r="EL1" s="17" t="s">
+        <v>257</v>
+      </c>
+      <c r="EM1" s="17" t="s">
         <v>258</v>
       </c>
-      <c r="EK1" s="17" t="s">
-        <v>257</v>
-      </c>
-      <c r="EL1" s="17" t="s">
+      <c r="EN1" s="17" t="s">
         <v>259</v>
       </c>
-      <c r="EM1" s="17" t="s">
+      <c r="EO1" s="17" t="s">
         <v>260</v>
       </c>
-      <c r="EN1" s="17" t="s">
+      <c r="EP1" s="17" t="s">
         <v>261</v>
-      </c>
-      <c r="EO1" s="17" t="s">
-        <v>262</v>
-      </c>
-      <c r="EP1" s="17" t="s">
-        <v>263</v>
       </c>
     </row>
     <row r="2" spans="1:146" s="21" customFormat="1" ht="85" x14ac:dyDescent="0.2">
@@ -2493,13 +2515,13 @@
         <v>38</v>
       </c>
       <c r="B2" s="21" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="C2" s="21" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="D2" s="21" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="N2" s="21" t="s">
         <v>0</v>
@@ -2508,17 +2530,17 @@
         <v>1948</v>
       </c>
       <c r="P2" s="21" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="Q2" s="21">
         <v>21</v>
       </c>
-      <c r="R2" s="22">
-        <v>17553</v>
+      <c r="R2" s="31" t="s">
+        <v>442</v>
       </c>
       <c r="S2" s="22"/>
       <c r="T2" s="21">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="U2" s="21" t="s">
         <v>20</v>
@@ -2533,19 +2555,19 @@
         <v>0</v>
       </c>
       <c r="AA2" s="21" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="AB2" s="21" t="s">
         <v>22</v>
       </c>
       <c r="AC2" s="21" t="s">
+        <v>196</v>
+      </c>
+      <c r="AD2" s="21" t="s">
+        <v>197</v>
+      </c>
+      <c r="AE2" s="21" t="s">
         <v>198</v>
-      </c>
-      <c r="AD2" s="21" t="s">
-        <v>199</v>
-      </c>
-      <c r="AE2" s="21" t="s">
-        <v>200</v>
       </c>
       <c r="AF2" s="21" t="s">
         <v>23</v>
@@ -2554,13 +2576,13 @@
         <v>28907</v>
       </c>
       <c r="AH2" s="18" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="AI2" s="18" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="AJ2" s="19" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="AK2" s="19"/>
       <c r="AL2" s="21">
@@ -2600,7 +2622,7 @@
         <v>40</v>
       </c>
       <c r="AX2" s="21" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="AY2" s="21" t="s">
         <v>0</v>
@@ -2609,7 +2631,7 @@
         <v>0</v>
       </c>
       <c r="BA2" s="21" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="BB2" s="21" t="s">
         <v>37</v>
@@ -2663,10 +2685,10 @@
         <v>65</v>
       </c>
       <c r="BW2" s="23" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="BX2" s="23" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="BY2" s="21" t="s">
         <v>66</v>
@@ -2678,7 +2700,7 @@
         <v>0</v>
       </c>
       <c r="CE2" s="21" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="CF2" s="21" t="s">
         <v>74</v>
@@ -2765,13 +2787,13 @@
         <v>111</v>
       </c>
       <c r="DK2" s="21" t="s">
-        <v>112</v>
+        <v>441</v>
       </c>
       <c r="DL2" s="21" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="DM2" s="21" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="DN2" s="21">
         <v>3028976789</v>
@@ -2780,31 +2802,31 @@
         <v>0</v>
       </c>
       <c r="DP2" s="21" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="DQ2" s="21" t="s">
+        <v>120</v>
+      </c>
+      <c r="DR2" s="21" t="s">
+        <v>119</v>
+      </c>
+      <c r="DS2" s="21" t="s">
+        <v>121</v>
+      </c>
+      <c r="DT2" s="21" t="s">
+        <v>118</v>
+      </c>
+      <c r="DU2" s="21" t="s">
         <v>122</v>
       </c>
-      <c r="DR2" s="21" t="s">
-        <v>121</v>
-      </c>
-      <c r="DS2" s="21" t="s">
-        <v>123</v>
-      </c>
-      <c r="DT2" s="21" t="s">
-        <v>120</v>
-      </c>
-      <c r="DU2" s="21" t="s">
-        <v>124</v>
-      </c>
       <c r="DV2" s="21" t="s">
-        <v>119</v>
+        <v>440</v>
       </c>
       <c r="DW2" s="21" t="s">
         <v>47</v>
       </c>
       <c r="DX2" s="21" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="DY2" s="21" t="s">
         <v>0</v>
@@ -2843,7 +2865,7 @@
         <v>0</v>
       </c>
       <c r="EK2" s="27" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="EL2" s="21" t="s">
         <v>0</v>
@@ -2866,54 +2888,54 @@
         <v>38</v>
       </c>
       <c r="B3" s="21" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C3" s="21" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D3" s="21" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="N3" s="21" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="O3" s="21">
         <v>1920</v>
       </c>
       <c r="P3" s="21" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="Q3" s="21">
         <v>23</v>
       </c>
-      <c r="R3" s="22" t="s">
-        <v>431</v>
+      <c r="R3" s="31" t="s">
+        <v>429</v>
       </c>
       <c r="S3" s="22"/>
       <c r="T3" s="22"/>
       <c r="U3" s="21" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="V3" s="21" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="X3" s="21" t="s">
+        <v>164</v>
+      </c>
+      <c r="Z3" s="21" t="s">
+        <v>134</v>
+      </c>
+      <c r="AB3" s="21" t="s">
         <v>166</v>
       </c>
-      <c r="Z3" s="21" t="s">
-        <v>136</v>
-      </c>
-      <c r="AB3" s="21" t="s">
-        <v>168</v>
-      </c>
       <c r="AH3" s="18" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="AI3" s="18" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="AJ3" s="19" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="AK3" s="19"/>
       <c r="AL3" s="21">
@@ -2929,7 +2951,7 @@
         <v>3014524258</v>
       </c>
       <c r="AP3" s="21" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="AQ3" s="21" t="s">
         <v>25</v>
@@ -2953,32 +2975,32 @@
         <v>40</v>
       </c>
       <c r="AX3" s="21" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="AZ3" s="21" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="BM3" s="21" t="s">
         <v>0</v>
       </c>
       <c r="BN3" s="21" t="s">
+        <v>146</v>
+      </c>
+      <c r="BO3" s="22" t="s">
+        <v>295</v>
+      </c>
+      <c r="BQ3" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="BR3" s="21" t="s">
+        <v>147</v>
+      </c>
+      <c r="BV3" s="21" t="s">
         <v>148</v>
       </c>
-      <c r="BO3" s="22" t="s">
-        <v>297</v>
-      </c>
-      <c r="BQ3" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="BR3" s="21" t="s">
+      <c r="BY3" s="21" t="s">
         <v>149</v>
       </c>
-      <c r="BV3" s="21" t="s">
-        <v>150</v>
-      </c>
-      <c r="BY3" s="21" t="s">
-        <v>151</v>
-      </c>
       <c r="BZ3" s="21" t="s">
         <v>0</v>
       </c>
@@ -2986,25 +3008,25 @@
         <v>0</v>
       </c>
       <c r="CE3" s="21" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="CF3" s="21" t="s">
         <v>74</v>
       </c>
       <c r="CG3" s="21" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="CH3" s="21" t="s">
         <v>73</v>
       </c>
       <c r="CI3" s="21" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="CJ3" s="21" t="s">
         <v>0</v>
       </c>
       <c r="CK3" s="21" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="CL3" s="21" t="s">
         <v>0</v>
@@ -3016,22 +3038,22 @@
         <v>100</v>
       </c>
       <c r="CQ3" s="21" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="CR3" s="21" t="s">
         <v>75</v>
       </c>
       <c r="CS3" s="21" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="CT3" s="21" t="s">
         <v>0</v>
       </c>
       <c r="CU3" s="21" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="CV3" s="22" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="CX3" s="21" t="s">
         <v>79</v>
@@ -3046,61 +3068,61 @@
         <v>102</v>
       </c>
       <c r="DD3" s="21" t="s">
+        <v>151</v>
+      </c>
+      <c r="DE3" s="21" t="s">
+        <v>152</v>
+      </c>
+      <c r="DF3" s="21" t="s">
         <v>153</v>
       </c>
-      <c r="DE3" s="21" t="s">
-        <v>154</v>
-      </c>
-      <c r="DF3" s="21" t="s">
-        <v>155</v>
-      </c>
       <c r="DG3" s="21" t="s">
         <v>0</v>
       </c>
       <c r="DH3" s="21" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="DJ3" s="21" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="DL3" s="21" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="DM3" s="21" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="DN3" s="21">
         <v>3028976789</v>
       </c>
       <c r="DO3" s="21" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="DP3" s="21" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="DQ3" s="21" t="s">
+        <v>120</v>
+      </c>
+      <c r="DR3" s="21" t="s">
+        <v>119</v>
+      </c>
+      <c r="DS3" s="21" t="s">
+        <v>121</v>
+      </c>
+      <c r="DT3" s="21" t="s">
+        <v>118</v>
+      </c>
+      <c r="DU3" s="21" t="s">
         <v>122</v>
       </c>
-      <c r="DR3" s="21" t="s">
-        <v>121</v>
-      </c>
-      <c r="DS3" s="21" t="s">
-        <v>123</v>
-      </c>
-      <c r="DT3" s="21" t="s">
-        <v>120</v>
-      </c>
-      <c r="DU3" s="21" t="s">
-        <v>124</v>
-      </c>
       <c r="DV3" s="21" t="s">
-        <v>119</v>
+        <v>440</v>
       </c>
       <c r="DW3" s="21" t="s">
         <v>47</v>
       </c>
       <c r="DX3" s="21" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="DY3" s="21" t="s">
         <v>0</v>
@@ -3139,7 +3161,7 @@
         <v>0</v>
       </c>
       <c r="EK3" s="27" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="EL3" s="21" t="s">
         <v>0</v>
@@ -3162,51 +3184,51 @@
         <v>38</v>
       </c>
       <c r="B4" s="21" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C4" s="21" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="D4" s="21" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="N4" s="21" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="O4" s="21">
         <v>1910</v>
       </c>
       <c r="P4" s="21" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="Q4" s="21">
         <v>21</v>
       </c>
-      <c r="R4" s="22" t="s">
-        <v>432</v>
+      <c r="R4" s="31" t="s">
+        <v>430</v>
       </c>
       <c r="S4" s="22"/>
       <c r="T4" s="22"/>
       <c r="U4" s="21" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="V4" s="21" t="s">
+        <v>163</v>
+      </c>
+      <c r="X4" s="21" t="s">
         <v>165</v>
       </c>
-      <c r="X4" s="21" t="s">
-        <v>167</v>
-      </c>
       <c r="Z4" s="21" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="AB4" s="21" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="AH4" s="19" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="AI4" s="18" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="AJ4" s="18"/>
       <c r="AK4" s="18"/>
@@ -3223,7 +3245,7 @@
         <v>3015567865</v>
       </c>
       <c r="AP4" s="21" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="AQ4" s="21" t="s">
         <v>27</v>
@@ -3232,25 +3254,25 @@
         <v>27</v>
       </c>
       <c r="AZ4" s="21" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="BM4" s="21" t="s">
         <v>0</v>
       </c>
       <c r="BN4" s="21" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="BQ4" s="21" t="s">
         <v>0</v>
       </c>
       <c r="BR4" s="21" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="BV4" s="21" t="s">
         <v>65</v>
       </c>
       <c r="BY4" s="21" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="BZ4" s="21" t="s">
         <v>0</v>
@@ -3259,34 +3281,34 @@
         <v>0</v>
       </c>
       <c r="CE4" s="21" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="CF4" s="21" t="s">
         <v>74</v>
       </c>
       <c r="CG4" s="21" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="CH4" s="21" t="s">
         <v>73</v>
       </c>
       <c r="CI4" s="21" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="CJ4" s="21" t="s">
         <v>0</v>
       </c>
       <c r="CK4" s="21" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="CL4" s="21" t="s">
         <v>0</v>
       </c>
       <c r="CM4" s="21" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="CQ4" s="21" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="CR4" s="21" t="s">
         <v>75</v>
@@ -3298,7 +3320,7 @@
         <v>0</v>
       </c>
       <c r="CU4" s="21" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="CX4" s="21" t="s">
         <v>79</v>
@@ -3307,16 +3329,16 @@
         <v>81</v>
       </c>
       <c r="CZ4" s="21" t="s">
+        <v>170</v>
+      </c>
+      <c r="DD4" s="21" t="s">
+        <v>171</v>
+      </c>
+      <c r="DE4" s="21" t="s">
+        <v>358</v>
+      </c>
+      <c r="DF4" s="21" t="s">
         <v>172</v>
-      </c>
-      <c r="DD4" s="21" t="s">
-        <v>173</v>
-      </c>
-      <c r="DE4" s="21" t="s">
-        <v>360</v>
-      </c>
-      <c r="DF4" s="21" t="s">
-        <v>174</v>
       </c>
       <c r="DG4" s="21" t="s">
         <v>0</v>
@@ -3328,13 +3350,13 @@
         <v>110</v>
       </c>
       <c r="DJ4" s="23" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="DL4" s="21" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="DM4" s="21" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="DN4" s="21">
         <v>3028976789</v>
@@ -3343,85 +3365,85 @@
         <v>0</v>
       </c>
       <c r="DP4" s="21" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="DQ4" s="21" t="s">
+        <v>120</v>
+      </c>
+      <c r="DR4" s="21" t="s">
+        <v>119</v>
+      </c>
+      <c r="DS4" s="21" t="s">
+        <v>121</v>
+      </c>
+      <c r="DT4" s="21" t="s">
+        <v>118</v>
+      </c>
+      <c r="DU4" s="21" t="s">
         <v>122</v>
       </c>
-      <c r="DR4" s="21" t="s">
-        <v>121</v>
-      </c>
-      <c r="DS4" s="21" t="s">
-        <v>123</v>
-      </c>
-      <c r="DT4" s="21" t="s">
-        <v>120</v>
-      </c>
-      <c r="DU4" s="21" t="s">
-        <v>124</v>
-      </c>
       <c r="DV4" s="21" t="s">
-        <v>119</v>
+        <v>440</v>
       </c>
       <c r="DW4" s="21" t="s">
         <v>47</v>
       </c>
       <c r="DX4" s="21" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="DY4" s="21" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="DZ4" s="21" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="EA4" s="21" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="EB4" s="21" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="EC4" s="21" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="ED4" s="21" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="EE4" s="21" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="EF4" s="21" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="EG4" s="21" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="EH4" s="21" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="EI4" s="21" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="EJ4" s="21" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="EK4" s="27" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="EL4" s="21" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="EM4" s="21" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="EN4" s="21" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="EO4" s="21" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="EP4" s="21" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="5" spans="1:146" s="21" customFormat="1" ht="51" x14ac:dyDescent="0.2">
@@ -3429,57 +3451,57 @@
         <v>38</v>
       </c>
       <c r="B5" s="21" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C5" s="21" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="D5" s="21" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="N5" s="21" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="O5" s="21">
         <v>1925</v>
       </c>
       <c r="P5" s="21" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="Q5" s="21">
         <v>21</v>
       </c>
-      <c r="R5" s="22" t="s">
-        <v>433</v>
+      <c r="R5" s="31" t="s">
+        <v>431</v>
       </c>
       <c r="S5" s="22"/>
       <c r="T5" s="22"/>
       <c r="U5" s="21" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="V5" s="21" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="W5" s="21" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="X5" s="21" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="Y5" s="21" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="Z5" s="21" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="AB5" s="21" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="AH5" s="19" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="AI5" s="19" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="AJ5" s="19"/>
       <c r="AK5" s="19"/>
@@ -3496,19 +3518,19 @@
         <v>3015567865</v>
       </c>
       <c r="AP5" s="21" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="AQ5" s="21" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="AZ5" s="21" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="BM5" s="21" t="s">
         <v>0</v>
       </c>
       <c r="BN5" s="21" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="BQ5" s="21" t="s">
         <v>0</v>
@@ -3517,7 +3539,7 @@
         <v>31</v>
       </c>
       <c r="BS5" s="21" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="BV5" s="21" t="s">
         <v>65</v>
@@ -3532,49 +3554,49 @@
         <v>0</v>
       </c>
       <c r="CE5" s="21" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="CF5" s="21" t="s">
         <v>74</v>
       </c>
       <c r="CG5" s="21" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="CH5" s="21" t="s">
         <v>73</v>
       </c>
       <c r="CI5" s="21" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="CJ5" s="21" t="s">
         <v>0</v>
       </c>
       <c r="CK5" s="21" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="CL5" s="21" t="s">
         <v>0</v>
       </c>
       <c r="CM5" s="21" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="CQ5" s="21" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="CR5" s="21" t="s">
         <v>75</v>
       </c>
       <c r="CS5" s="21" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="CT5" s="21" t="s">
         <v>0</v>
       </c>
       <c r="CU5" s="21" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="CV5" s="22" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="CX5" s="21" t="s">
         <v>79</v>
@@ -3583,34 +3605,34 @@
         <v>81</v>
       </c>
       <c r="CZ5" s="21" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="DD5" s="21" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="DE5" s="21" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="DF5" s="21" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="DG5" s="21" t="s">
         <v>0</v>
       </c>
       <c r="DH5" s="21" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="DJ5" s="21" t="s">
         <v>37</v>
       </c>
       <c r="DK5" s="21" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="DL5" s="21" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="DM5" s="21" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="DN5" s="21">
         <v>3028976789</v>
@@ -3619,85 +3641,85 @@
         <v>0</v>
       </c>
       <c r="DP5" s="21" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="DQ5" s="21" t="s">
+        <v>120</v>
+      </c>
+      <c r="DR5" s="21" t="s">
+        <v>119</v>
+      </c>
+      <c r="DS5" s="21" t="s">
+        <v>121</v>
+      </c>
+      <c r="DT5" s="21" t="s">
+        <v>118</v>
+      </c>
+      <c r="DU5" s="21" t="s">
         <v>122</v>
       </c>
-      <c r="DR5" s="21" t="s">
-        <v>121</v>
-      </c>
-      <c r="DS5" s="21" t="s">
-        <v>123</v>
-      </c>
-      <c r="DT5" s="21" t="s">
-        <v>120</v>
-      </c>
-      <c r="DU5" s="21" t="s">
-        <v>124</v>
-      </c>
       <c r="DV5" s="21" t="s">
-        <v>119</v>
+        <v>440</v>
       </c>
       <c r="DW5" s="21" t="s">
         <v>47</v>
       </c>
       <c r="DX5" s="21" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="DY5" s="21" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="DZ5" s="21" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="EA5" s="21" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="EB5" s="21" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="EC5" s="21" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="ED5" s="21" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="EE5" s="21" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="EF5" s="21" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="EG5" s="21" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="EH5" s="21" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="EI5" s="21" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="EJ5" s="21" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="EK5" s="27" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="EL5" s="21" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="EM5" s="21" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="EN5" s="21" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="EO5" s="21" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="EP5" s="21" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="6" spans="1:146" s="21" customFormat="1" ht="51" x14ac:dyDescent="0.2">
@@ -3705,51 +3727,51 @@
         <v>38</v>
       </c>
       <c r="B6" s="21" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C6" s="21" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D6" s="21" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="N6" s="21" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="O6" s="21">
         <v>1950</v>
       </c>
       <c r="P6" s="21" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="Q6" s="21">
         <v>26</v>
       </c>
-      <c r="R6" s="22" t="s">
-        <v>434</v>
+      <c r="R6" s="31" t="s">
+        <v>432</v>
       </c>
       <c r="S6" s="22"/>
       <c r="T6" s="22"/>
       <c r="U6" s="21" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="V6" s="21" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="X6" s="21" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="Z6" s="21" t="s">
         <v>0</v>
       </c>
       <c r="AB6" s="21" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="AH6" s="18" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="AI6" s="21" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="AL6" s="21">
         <v>3015774089</v>
@@ -3764,147 +3786,147 @@
         <v>3015774089</v>
       </c>
       <c r="AP6" s="21" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="AQ6" s="21" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="AZ6" s="21" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="BM6" s="21" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="BO6" s="24"/>
       <c r="BQ6" s="21" t="s">
         <v>0</v>
       </c>
       <c r="BR6" s="21" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="BV6" s="21" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="BY6" s="21" t="s">
         <v>66</v>
       </c>
       <c r="BZ6" s="21" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="CE6" s="21" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="CL6" s="21" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="CV6" s="24"/>
       <c r="DG6" s="21" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="DH6" s="21" t="s">
         <v>108</v>
       </c>
       <c r="DI6" s="21" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="DJ6" s="21" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="DK6" s="21" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="DL6" s="21" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="DM6" s="21" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="DN6" s="21">
         <v>3028976789</v>
       </c>
       <c r="DO6" s="21" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="DP6" s="21" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="DQ6" s="21" t="s">
+        <v>120</v>
+      </c>
+      <c r="DR6" s="21" t="s">
+        <v>119</v>
+      </c>
+      <c r="DS6" s="21" t="s">
+        <v>121</v>
+      </c>
+      <c r="DT6" s="21" t="s">
+        <v>118</v>
+      </c>
+      <c r="DU6" s="21" t="s">
         <v>122</v>
       </c>
-      <c r="DR6" s="21" t="s">
-        <v>121</v>
-      </c>
-      <c r="DS6" s="21" t="s">
-        <v>123</v>
-      </c>
-      <c r="DT6" s="21" t="s">
-        <v>120</v>
-      </c>
-      <c r="DU6" s="21" t="s">
-        <v>124</v>
-      </c>
       <c r="DV6" s="21" t="s">
-        <v>119</v>
+        <v>440</v>
       </c>
       <c r="DW6" s="21" t="s">
         <v>47</v>
       </c>
       <c r="DX6" s="21" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="DY6" s="21" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="DZ6" s="21" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="EA6" s="21" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="EB6" s="21" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="EC6" s="21" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="ED6" s="21" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="EE6" s="21" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="EF6" s="21" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="EG6" s="21" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="EH6" s="21" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="EI6" s="21" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="EJ6" s="21" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="EK6" s="27" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="EL6" s="21" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="EM6" s="21" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="EN6" s="21" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="EO6" s="21" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="EP6" s="21" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="7" spans="1:146" s="21" customFormat="1" ht="51" x14ac:dyDescent="0.2">
@@ -3912,51 +3934,51 @@
         <v>38</v>
       </c>
       <c r="B7" s="21" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C7" s="21" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="D7" s="21" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="N7" s="21" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="O7" s="21">
         <v>1940</v>
       </c>
       <c r="P7" s="21" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="Q7" s="21">
         <v>11</v>
       </c>
-      <c r="R7" s="22" t="s">
-        <v>435</v>
+      <c r="R7" s="31" t="s">
+        <v>433</v>
       </c>
       <c r="S7" s="22"/>
       <c r="T7" s="22"/>
       <c r="U7" s="21" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="V7" s="21" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="X7" s="21" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="Z7" s="21" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="AB7" s="21" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="AH7" s="18" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="AI7" s="18" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="AJ7" s="18"/>
       <c r="AK7" s="18"/>
@@ -3973,16 +3995,16 @@
         <v>3014524258</v>
       </c>
       <c r="AP7" s="21" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="AQ7" s="21" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="AZ7" s="21" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="BM7" s="21" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="BO7" s="24"/>
       <c r="BQ7" s="21" t="s">
@@ -3992,10 +4014,10 @@
         <v>31</v>
       </c>
       <c r="BS7" s="21" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="BT7" s="21" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="BU7" s="21" t="s">
         <v>0</v>
@@ -4010,23 +4032,23 @@
         <v>0</v>
       </c>
       <c r="CA7" s="21" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="CB7" s="21" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="CE7" s="21" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="CJ7" s="21" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="CL7" s="21" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="CV7" s="24"/>
       <c r="DG7" s="21" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="DH7" s="21" t="s">
         <v>108</v>
@@ -4035,46 +4057,46 @@
         <v>110</v>
       </c>
       <c r="DJ7" s="21" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="DL7" s="21" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="DM7" s="21" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="DN7" s="21">
         <v>3028976789</v>
       </c>
       <c r="DO7" s="21" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="DP7" s="21" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="DQ7" s="21" t="s">
+        <v>120</v>
+      </c>
+      <c r="DR7" s="21" t="s">
+        <v>119</v>
+      </c>
+      <c r="DS7" s="21" t="s">
+        <v>121</v>
+      </c>
+      <c r="DT7" s="21" t="s">
+        <v>118</v>
+      </c>
+      <c r="DU7" s="21" t="s">
         <v>122</v>
       </c>
-      <c r="DR7" s="21" t="s">
-        <v>121</v>
-      </c>
-      <c r="DS7" s="21" t="s">
-        <v>123</v>
-      </c>
-      <c r="DT7" s="21" t="s">
-        <v>120</v>
-      </c>
-      <c r="DU7" s="21" t="s">
-        <v>124</v>
-      </c>
       <c r="DV7" s="21" t="s">
-        <v>119</v>
+        <v>440</v>
       </c>
       <c r="DW7" s="21" t="s">
         <v>47</v>
       </c>
       <c r="DX7" s="21" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="DY7" s="21" t="s">
         <v>0</v>
@@ -4113,7 +4135,7 @@
         <v>0</v>
       </c>
       <c r="EK7" s="27" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="EL7" s="21" t="s">
         <v>0</v>
@@ -4136,54 +4158,54 @@
         <v>38</v>
       </c>
       <c r="B8" s="21" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="C8" s="21" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="D8" s="21" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="N8" s="21" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="O8" s="21">
         <v>1930</v>
       </c>
       <c r="P8" s="21" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="Q8" s="21">
         <v>30</v>
       </c>
-      <c r="R8" s="22" t="s">
-        <v>436</v>
+      <c r="R8" s="31" t="s">
+        <v>434</v>
       </c>
       <c r="S8" s="22"/>
       <c r="T8" s="22"/>
       <c r="U8" s="21" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="V8" s="21" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="X8" s="21" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="Z8" s="21" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="AB8" s="21" t="s">
         <v>22</v>
       </c>
       <c r="AC8" s="21" t="s">
+        <v>196</v>
+      </c>
+      <c r="AD8" s="21" t="s">
+        <v>197</v>
+      </c>
+      <c r="AE8" s="21" t="s">
         <v>198</v>
-      </c>
-      <c r="AD8" s="21" t="s">
-        <v>199</v>
-      </c>
-      <c r="AE8" s="21" t="s">
-        <v>200</v>
       </c>
       <c r="AF8" s="21" t="s">
         <v>23</v>
@@ -4192,10 +4214,10 @@
         <v>28907</v>
       </c>
       <c r="AH8" s="18" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="AI8" s="18" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="AJ8" s="18"/>
       <c r="AK8" s="18"/>
@@ -4212,81 +4234,81 @@
         <v>3015567865</v>
       </c>
       <c r="AP8" s="21" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="AQ8" s="21" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="AZ8" s="21" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="BM8" s="21" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="BP8" s="24"/>
       <c r="BQ8" s="21" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="BZ8" s="21" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="CE8" s="21" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="CL8" s="21" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="CV8" s="24"/>
       <c r="DG8" s="21" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="DH8" s="21" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="DJ8" s="21" t="s">
         <v>47</v>
       </c>
       <c r="DK8" s="21" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="DL8" s="21" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="DM8" s="21" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="DN8" s="21">
         <v>3028976789</v>
       </c>
       <c r="DO8" s="21" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="DP8" s="21" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="DQ8" s="21" t="s">
+        <v>120</v>
+      </c>
+      <c r="DR8" s="21" t="s">
+        <v>119</v>
+      </c>
+      <c r="DS8" s="21" t="s">
+        <v>121</v>
+      </c>
+      <c r="DT8" s="21" t="s">
+        <v>118</v>
+      </c>
+      <c r="DU8" s="21" t="s">
         <v>122</v>
       </c>
-      <c r="DR8" s="21" t="s">
-        <v>121</v>
-      </c>
-      <c r="DS8" s="21" t="s">
-        <v>123</v>
-      </c>
-      <c r="DT8" s="21" t="s">
-        <v>120</v>
-      </c>
-      <c r="DU8" s="21" t="s">
-        <v>124</v>
-      </c>
       <c r="DV8" s="21" t="s">
-        <v>119</v>
+        <v>440</v>
       </c>
       <c r="DW8" s="21" t="s">
         <v>47</v>
       </c>
       <c r="DX8" s="21" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="DY8" s="21" t="s">
         <v>0</v>
@@ -4325,7 +4347,7 @@
         <v>0</v>
       </c>
       <c r="EK8" s="27" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="EL8" s="21" t="s">
         <v>0</v>
@@ -4348,13 +4370,13 @@
         <v>38</v>
       </c>
       <c r="B9" s="21" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="C9" s="21" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="D9" s="21" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="N9" s="21" t="s">
         <v>0</v>
@@ -4363,36 +4385,36 @@
         <v>1935</v>
       </c>
       <c r="P9" s="21" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="Q9" s="21">
         <v>29</v>
       </c>
-      <c r="R9" s="22" t="s">
-        <v>437</v>
+      <c r="R9" s="31" t="s">
+        <v>435</v>
       </c>
       <c r="S9" s="22"/>
       <c r="T9" s="22"/>
       <c r="U9" s="21" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="V9" s="21" t="s">
+        <v>163</v>
+      </c>
+      <c r="X9" s="21" t="s">
         <v>165</v>
       </c>
-      <c r="X9" s="21" t="s">
-        <v>167</v>
-      </c>
       <c r="Z9" s="21" t="s">
         <v>0</v>
       </c>
       <c r="AB9" s="21" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="AH9" s="18" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="AI9" s="18" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="AJ9" s="18"/>
       <c r="AK9" s="18"/>
@@ -4409,16 +4431,16 @@
         <v>3015567865</v>
       </c>
       <c r="AP9" s="21" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="AQ9" s="21" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="AZ9" s="21" t="s">
         <v>0</v>
       </c>
       <c r="BA9" s="21" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="BB9" s="21" t="s">
         <v>37</v>
@@ -4463,7 +4485,7 @@
         <v>119</v>
       </c>
       <c r="BQ9" s="21" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="BZ9" s="21" t="s">
         <v>0</v>
@@ -4472,22 +4494,22 @@
         <v>0</v>
       </c>
       <c r="CE9" s="21" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="CF9" s="21" t="s">
         <v>74</v>
       </c>
       <c r="CG9" s="21" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="CH9" s="21" t="s">
         <v>73</v>
       </c>
       <c r="CI9" s="21" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="CJ9" s="21" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="CL9" s="21" t="s">
         <v>0</v>
@@ -4499,23 +4521,23 @@
         <v>102</v>
       </c>
       <c r="CQ9" s="21" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="CR9" s="21" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="CS9" s="21" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="CT9" s="21" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="CV9" s="24"/>
       <c r="CX9" s="21" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="DG9" s="21" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="DH9" s="21" t="s">
         <v>108</v>
@@ -4524,13 +4546,13 @@
         <v>110</v>
       </c>
       <c r="DJ9" s="23" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="DL9" s="21" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="DM9" s="21" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="DN9" s="21">
         <v>3028976789</v>
@@ -4539,111 +4561,111 @@
         <v>0</v>
       </c>
       <c r="DP9" s="21" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="DQ9" s="21" t="s">
+        <v>120</v>
+      </c>
+      <c r="DR9" s="21" t="s">
+        <v>119</v>
+      </c>
+      <c r="DS9" s="21" t="s">
+        <v>121</v>
+      </c>
+      <c r="DT9" s="21" t="s">
+        <v>118</v>
+      </c>
+      <c r="DU9" s="21" t="s">
         <v>122</v>
       </c>
-      <c r="DR9" s="21" t="s">
-        <v>121</v>
-      </c>
-      <c r="DS9" s="21" t="s">
-        <v>123</v>
-      </c>
-      <c r="DT9" s="21" t="s">
-        <v>120</v>
-      </c>
-      <c r="DU9" s="21" t="s">
-        <v>124</v>
-      </c>
       <c r="DV9" s="21" t="s">
-        <v>119</v>
+        <v>440</v>
       </c>
       <c r="DW9" s="21" t="s">
         <v>47</v>
       </c>
       <c r="DX9" s="21" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="DY9" s="21" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="DZ9" s="21" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="EA9" s="21" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="EB9" s="21" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="EC9" s="21" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="ED9" s="21" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="EE9" s="21" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="EF9" s="21" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="EG9" s="21" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="EH9" s="21" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="EI9" s="21" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="EJ9" s="21" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="EK9" s="27" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="EL9" s="21" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="EM9" s="21" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="EN9" s="21" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="EO9" s="21" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="EP9" s="21" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="10" spans="1:146" s="21" customFormat="1" ht="85" x14ac:dyDescent="0.2">
       <c r="A10" s="21" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E10" s="21" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="F10" s="21" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="G10" s="21" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="H10" s="21" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="I10" s="21" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="J10" s="21" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="K10" s="21" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="M10" s="21" t="s">
         <v>0</v>
@@ -4655,13 +4677,13 @@
         <v>1937</v>
       </c>
       <c r="P10" s="21" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="Q10" s="21">
         <v>27</v>
       </c>
-      <c r="R10" s="22" t="s">
-        <v>438</v>
+      <c r="R10" s="31" t="s">
+        <v>436</v>
       </c>
       <c r="S10" s="22"/>
       <c r="T10" s="22"/>
@@ -4676,13 +4698,13 @@
         <v>22</v>
       </c>
       <c r="AC10" s="21" t="s">
+        <v>196</v>
+      </c>
+      <c r="AD10" s="21" t="s">
+        <v>197</v>
+      </c>
+      <c r="AE10" s="21" t="s">
         <v>198</v>
-      </c>
-      <c r="AD10" s="21" t="s">
-        <v>199</v>
-      </c>
-      <c r="AE10" s="21" t="s">
-        <v>200</v>
       </c>
       <c r="AF10" s="21" t="s">
         <v>23</v>
@@ -4691,10 +4713,10 @@
         <v>28907</v>
       </c>
       <c r="AH10" s="19" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="AI10" s="18" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="AJ10" s="18"/>
       <c r="AK10" s="18"/>
@@ -4735,13 +4757,13 @@
         <v>40</v>
       </c>
       <c r="AX10" s="21" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="AZ10" s="21" t="s">
         <v>0</v>
       </c>
       <c r="BA10" s="21" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="BB10" s="21" t="s">
         <v>37</v>
@@ -4780,25 +4802,25 @@
         <v>0</v>
       </c>
       <c r="BN10" s="21" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="BO10" s="22" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="BQ10" s="21" t="s">
         <v>0</v>
       </c>
       <c r="BR10" s="21" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="BV10" s="21" t="s">
         <v>65</v>
       </c>
       <c r="BW10" s="23" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="BX10" s="23" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="BY10" s="21" t="s">
         <v>66</v>
@@ -4810,16 +4832,16 @@
         <v>0</v>
       </c>
       <c r="CE10" s="21" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="CF10" s="21" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="CG10" s="21" t="s">
         <v>72</v>
       </c>
       <c r="CH10" s="21" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="CI10" s="21" t="s">
         <v>72</v>
@@ -4861,7 +4883,7 @@
         <v>103</v>
       </c>
       <c r="CX10" s="21" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="CY10" s="21" t="s">
         <v>81</v>
@@ -4885,7 +4907,7 @@
         <v>92</v>
       </c>
       <c r="DG10" s="21" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="DH10" s="21" t="s">
         <v>108</v>
@@ -4897,13 +4919,13 @@
         <v>111</v>
       </c>
       <c r="DK10" s="21" t="s">
-        <v>112</v>
+        <v>441</v>
       </c>
       <c r="DL10" s="21" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="DM10" s="21" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="DN10" s="21">
         <v>3028976789</v>
@@ -4912,31 +4934,31 @@
         <v>0</v>
       </c>
       <c r="DP10" s="21" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="DQ10" s="21" t="s">
+        <v>120</v>
+      </c>
+      <c r="DR10" s="21" t="s">
+        <v>119</v>
+      </c>
+      <c r="DS10" s="21" t="s">
+        <v>121</v>
+      </c>
+      <c r="DT10" s="21" t="s">
+        <v>118</v>
+      </c>
+      <c r="DU10" s="21" t="s">
         <v>122</v>
       </c>
-      <c r="DR10" s="21" t="s">
-        <v>121</v>
-      </c>
-      <c r="DS10" s="21" t="s">
-        <v>123</v>
-      </c>
-      <c r="DT10" s="21" t="s">
-        <v>120</v>
-      </c>
-      <c r="DU10" s="21" t="s">
-        <v>124</v>
-      </c>
       <c r="DV10" s="21" t="s">
-        <v>119</v>
+        <v>440</v>
       </c>
       <c r="DW10" s="21" t="s">
         <v>47</v>
       </c>
       <c r="DX10" s="21" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="DY10" s="21" t="s">
         <v>0</v>
@@ -4975,7 +4997,7 @@
         <v>0</v>
       </c>
       <c r="EK10" s="27" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="EL10" s="21" t="s">
         <v>0</v>
@@ -4995,66 +5017,66 @@
     </row>
     <row r="11" spans="1:146" s="21" customFormat="1" ht="68" x14ac:dyDescent="0.2">
       <c r="A11" s="21" t="s">
+        <v>131</v>
+      </c>
+      <c r="E11" s="21" t="s">
+        <v>402</v>
+      </c>
+      <c r="F11" s="21" t="s">
+        <v>416</v>
+      </c>
+      <c r="G11" s="21" t="s">
+        <v>403</v>
+      </c>
+      <c r="H11" s="21" t="s">
+        <v>370</v>
+      </c>
+      <c r="I11" s="21" t="s">
         <v>133</v>
       </c>
-      <c r="E11" s="21" t="s">
-        <v>404</v>
-      </c>
-      <c r="F11" s="21" t="s">
-        <v>418</v>
-      </c>
-      <c r="G11" s="21" t="s">
-        <v>405</v>
-      </c>
-      <c r="H11" s="21" t="s">
-        <v>372</v>
-      </c>
-      <c r="I11" s="21" t="s">
-        <v>135</v>
-      </c>
       <c r="J11" s="21" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="K11" s="21" t="s">
         <v>47</v>
       </c>
       <c r="L11" s="21" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="M11" s="21" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="N11" s="21" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="O11" s="21">
         <v>1935</v>
       </c>
       <c r="P11" s="21" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="Q11" s="21">
         <v>21</v>
       </c>
-      <c r="R11" s="22" t="s">
-        <v>439</v>
+      <c r="R11" s="31" t="s">
+        <v>437</v>
       </c>
       <c r="S11" s="22"/>
       <c r="T11" s="22"/>
       <c r="U11" s="21" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="Z11" s="21" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="AB11" s="21" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="AH11" s="18" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="AI11" s="19" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="AJ11" s="19"/>
       <c r="AK11" s="19"/>
@@ -5071,33 +5093,33 @@
         <v>3014524258</v>
       </c>
       <c r="AP11" s="21" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="AQ11" s="21" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="AZ11" s="21" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="BM11" s="21" t="s">
         <v>0</v>
       </c>
       <c r="BN11" s="21" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="BO11" s="24"/>
       <c r="BQ11" s="21" t="s">
         <v>0</v>
       </c>
       <c r="BR11" s="21" t="s">
+        <v>147</v>
+      </c>
+      <c r="BV11" s="21" t="s">
+        <v>148</v>
+      </c>
+      <c r="BY11" s="21" t="s">
         <v>149</v>
       </c>
-      <c r="BV11" s="21" t="s">
-        <v>150</v>
-      </c>
-      <c r="BY11" s="21" t="s">
-        <v>151</v>
-      </c>
       <c r="BZ11" s="21" t="s">
         <v>0</v>
       </c>
@@ -5105,65 +5127,65 @@
         <v>0</v>
       </c>
       <c r="CE11" s="21" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="CF11" s="21" t="s">
         <v>74</v>
       </c>
       <c r="CG11" s="21" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="CH11" s="21" t="s">
         <v>73</v>
       </c>
       <c r="CI11" s="21" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="CJ11" s="21" t="s">
         <v>0</v>
       </c>
       <c r="CK11" s="21" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="CL11" s="21" t="s">
         <v>0</v>
       </c>
       <c r="CM11" s="21" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="CQ11" s="21" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="CR11" s="21" t="s">
         <v>75</v>
       </c>
       <c r="CS11" s="21" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="CT11" s="21" t="s">
         <v>0</v>
       </c>
       <c r="CU11" s="21" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="CV11" s="24"/>
       <c r="CX11" s="21" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="CY11" s="21" t="s">
         <v>81</v>
       </c>
       <c r="CZ11" s="21" t="s">
+        <v>170</v>
+      </c>
+      <c r="DD11" s="21" t="s">
+        <v>171</v>
+      </c>
+      <c r="DE11" s="21" t="s">
+        <v>358</v>
+      </c>
+      <c r="DF11" s="21" t="s">
         <v>172</v>
-      </c>
-      <c r="DD11" s="21" t="s">
-        <v>173</v>
-      </c>
-      <c r="DE11" s="21" t="s">
-        <v>360</v>
-      </c>
-      <c r="DF11" s="21" t="s">
-        <v>174</v>
       </c>
       <c r="DG11" s="21" t="s">
         <v>0</v>
@@ -5172,16 +5194,16 @@
         <v>108</v>
       </c>
       <c r="DI11" s="21" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="DJ11" s="21" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="DL11" s="21" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="DM11" s="21" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="DN11" s="21">
         <v>3028976789</v>
@@ -5190,129 +5212,129 @@
         <v>0</v>
       </c>
       <c r="DP11" s="21" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="DQ11" s="21" t="s">
+        <v>120</v>
+      </c>
+      <c r="DR11" s="21" t="s">
+        <v>119</v>
+      </c>
+      <c r="DS11" s="21" t="s">
+        <v>121</v>
+      </c>
+      <c r="DT11" s="21" t="s">
+        <v>118</v>
+      </c>
+      <c r="DU11" s="21" t="s">
         <v>122</v>
       </c>
-      <c r="DR11" s="21" t="s">
-        <v>121</v>
-      </c>
-      <c r="DS11" s="21" t="s">
-        <v>123</v>
-      </c>
-      <c r="DT11" s="21" t="s">
-        <v>120</v>
-      </c>
-      <c r="DU11" s="21" t="s">
-        <v>124</v>
-      </c>
       <c r="DV11" s="21" t="s">
-        <v>119</v>
+        <v>440</v>
       </c>
       <c r="DW11" s="21" t="s">
         <v>47</v>
       </c>
       <c r="DX11" s="21" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="DY11" s="21" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="DZ11" s="21" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="EA11" s="21" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="EB11" s="21" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="EC11" s="21" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="ED11" s="21" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="EE11" s="21" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="EF11" s="21" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="EG11" s="21" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="EH11" s="21" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="EI11" s="21" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="EJ11" s="21" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="EK11" s="27" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="EL11" s="21" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="EM11" s="21" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="EN11" s="21" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="EO11" s="21" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="EP11" s="21" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="12" spans="1:146" s="21" customFormat="1" ht="68" x14ac:dyDescent="0.2">
       <c r="A12" s="21" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E12" s="21" t="s">
+        <v>404</v>
+      </c>
+      <c r="F12" s="21" t="s">
+        <v>414</v>
+      </c>
+      <c r="G12" s="21" t="s">
         <v>406</v>
       </c>
-      <c r="F12" s="21" t="s">
-        <v>416</v>
-      </c>
-      <c r="G12" s="21" t="s">
-        <v>408</v>
-      </c>
       <c r="H12" s="21" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="I12" s="21" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="J12" s="21" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="K12" s="21" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="M12" s="21" t="s">
         <v>0</v>
       </c>
       <c r="N12" s="21" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="O12" s="21">
         <v>1930</v>
       </c>
       <c r="P12" s="21" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="Q12" s="21">
         <v>30</v>
       </c>
-      <c r="R12" s="22" t="s">
-        <v>436</v>
+      <c r="R12" s="31" t="s">
+        <v>434</v>
       </c>
       <c r="S12" s="22"/>
       <c r="T12" s="22"/>
@@ -5320,16 +5342,16 @@
         <v>20</v>
       </c>
       <c r="Z12" s="21" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="AB12" s="21" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="AH12" s="19" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="AI12" s="19" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="AJ12" s="19"/>
       <c r="AK12" s="19"/>
@@ -5346,47 +5368,47 @@
         <v>3014524258</v>
       </c>
       <c r="AP12" s="21" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="AQ12" s="21" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="AZ12" s="21" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="BM12" s="21" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="BQ12" s="21" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="BZ12" s="21" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="CE12" s="21" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="CL12" s="21" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="CV12" s="24"/>
       <c r="DG12" s="21" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="DH12" s="21" t="s">
         <v>108</v>
       </c>
       <c r="DI12" s="21" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="DJ12" s="21" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="DL12" s="21" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="DM12" s="21" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="DN12" s="21">
         <v>3028976789</v>
@@ -5395,146 +5417,146 @@
         <v>0</v>
       </c>
       <c r="DP12" s="21" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="DQ12" s="21" t="s">
+        <v>120</v>
+      </c>
+      <c r="DR12" s="21" t="s">
+        <v>119</v>
+      </c>
+      <c r="DS12" s="21" t="s">
+        <v>121</v>
+      </c>
+      <c r="DT12" s="21" t="s">
+        <v>118</v>
+      </c>
+      <c r="DU12" s="21" t="s">
         <v>122</v>
       </c>
-      <c r="DR12" s="21" t="s">
-        <v>121</v>
-      </c>
-      <c r="DS12" s="21" t="s">
-        <v>123</v>
-      </c>
-      <c r="DT12" s="21" t="s">
-        <v>120</v>
-      </c>
-      <c r="DU12" s="21" t="s">
-        <v>124</v>
-      </c>
       <c r="DV12" s="21" t="s">
-        <v>119</v>
+        <v>440</v>
       </c>
       <c r="DW12" s="21" t="s">
         <v>47</v>
       </c>
       <c r="DX12" s="21" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="DY12" s="21" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="DZ12" s="21" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="EA12" s="21" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="EB12" s="21" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="EC12" s="21" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="ED12" s="21" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="EE12" s="21" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="EF12" s="21" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="EG12" s="21" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="EH12" s="21" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="EI12" s="21" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="EJ12" s="21" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="EK12" s="27" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="EL12" s="21" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="EM12" s="21" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="EN12" s="21" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="EO12" s="21" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="EP12" s="21" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="13" spans="1:146" s="21" customFormat="1" ht="68" x14ac:dyDescent="0.2">
       <c r="A13" s="21" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E13" s="21" t="s">
+        <v>405</v>
+      </c>
+      <c r="F13" s="21" t="s">
+        <v>415</v>
+      </c>
+      <c r="G13" s="21" t="s">
         <v>407</v>
       </c>
-      <c r="F13" s="21" t="s">
-        <v>417</v>
-      </c>
-      <c r="G13" s="21" t="s">
-        <v>409</v>
-      </c>
       <c r="H13" s="21" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="I13" s="21" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="J13" s="21" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="K13" s="21" t="s">
         <v>87</v>
       </c>
       <c r="M13" s="21" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="N13" s="21" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="O13" s="21">
         <v>1940</v>
       </c>
       <c r="P13" s="21" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="Q13" s="21">
         <v>21</v>
       </c>
-      <c r="R13" s="22" t="s">
-        <v>440</v>
+      <c r="R13" s="31" t="s">
+        <v>438</v>
       </c>
       <c r="S13" s="22"/>
       <c r="T13" s="22"/>
       <c r="U13" s="21" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="Z13" s="21" t="s">
         <v>0</v>
       </c>
       <c r="AB13" s="21" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="AH13" s="19" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="AI13" s="19" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="AJ13" s="19"/>
       <c r="AK13" s="19"/>
@@ -5551,28 +5573,28 @@
         <v>3014524258</v>
       </c>
       <c r="AP13" s="21" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="AQ13" s="21" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="AZ13" s="21" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="BM13" s="21" t="s">
         <v>0</v>
       </c>
       <c r="BN13" s="21" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="CE13" s="21" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="CF13" s="21" t="s">
         <v>74</v>
       </c>
       <c r="CG13" s="21" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="CH13" s="21" t="s">
         <v>73</v>
@@ -5587,140 +5609,146 @@
         <v>66</v>
       </c>
       <c r="DP13" s="21" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="DQ13" s="21" t="s">
+        <v>120</v>
+      </c>
+      <c r="DR13" s="21" t="s">
+        <v>119</v>
+      </c>
+      <c r="DS13" s="21" t="s">
+        <v>121</v>
+      </c>
+      <c r="DT13" s="21" t="s">
+        <v>118</v>
+      </c>
+      <c r="DU13" s="21" t="s">
         <v>122</v>
       </c>
-      <c r="DR13" s="21" t="s">
-        <v>121</v>
-      </c>
-      <c r="DS13" s="21" t="s">
-        <v>123</v>
-      </c>
-      <c r="DT13" s="21" t="s">
-        <v>120</v>
-      </c>
-      <c r="DU13" s="21" t="s">
-        <v>124</v>
-      </c>
       <c r="DV13" s="21" t="s">
-        <v>119</v>
+        <v>440</v>
       </c>
       <c r="DW13" s="21" t="s">
         <v>47</v>
       </c>
       <c r="DX13" s="21" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="DY13" s="21" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="DZ13" s="21" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="EA13" s="21" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="EB13" s="21" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="EC13" s="21" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="ED13" s="21" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="EE13" s="21" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="EF13" s="21" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="EG13" s="21" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="EH13" s="21" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="EI13" s="21" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="EJ13" s="21" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="EK13" s="27" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="EL13" s="21" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="EM13" s="21" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="EN13" s="21" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="EO13" s="21" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="EP13" s="21" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="14" spans="1:146" s="21" customFormat="1" ht="88" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K14" s="25" t="s">
-        <v>385</v>
-      </c>
+        <v>383</v>
+      </c>
+      <c r="R14" s="32"/>
       <c r="AH14" s="19" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="AI14" s="19" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="AJ14" s="19"/>
       <c r="AK14" s="19"/>
     </row>
     <row r="15" spans="1:146" s="21" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="K15" s="21" t="s">
-        <v>386</v>
-      </c>
+        <v>384</v>
+      </c>
+      <c r="R15" s="32"/>
       <c r="AH15" s="19" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="AI15" s="19" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="AJ15" s="19"/>
       <c r="AK15" s="19"/>
     </row>
     <row r="16" spans="1:146" s="21" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="K16" s="21" t="s">
-        <v>387</v>
-      </c>
+        <v>385</v>
+      </c>
+      <c r="R16" s="32"/>
       <c r="AH16" s="19" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="AI16" s="19" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="AJ16" s="19"/>
       <c r="AK16" s="19"/>
     </row>
     <row r="17" spans="11:37" s="21" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="K17" s="21" t="s">
-        <v>141</v>
-      </c>
+        <v>139</v>
+      </c>
+      <c r="R17" s="32"/>
       <c r="AH17" s="19" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="AI17" s="19" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="AJ17" s="19"/>
       <c r="AK17" s="19"/>
     </row>
-    <row r="18" spans="11:37" s="21" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="18" spans="11:37" s="21" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="R18" s="32"/>
+    </row>
   </sheetData>
   <autoFilter ref="A1:EP13" xr:uid="{D6C03A80-53F5-C744-BC65-FAA91BD85774}"/>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -5782,34 +5810,34 @@
   <sheetData>
     <row r="1" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="B1" s="5" t="s">
+        <v>273</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>274</v>
+      </c>
+      <c r="D1" s="5" t="s">
         <v>275</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="E1" s="5" t="s">
         <v>276</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="F1" s="5" t="s">
         <v>277</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="G1" s="5" t="s">
         <v>278</v>
       </c>
-      <c r="F1" s="5" t="s">
-        <v>279</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>280</v>
-      </c>
       <c r="H1" s="5" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="I1" s="5" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="J1" s="5" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="17" x14ac:dyDescent="0.2">
@@ -5817,7 +5845,7 @@
         <v>37</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>59</v>
@@ -5846,10 +5874,10 @@
         <v>43</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>61</v>
@@ -5870,7 +5898,7 @@
         <v>1991</v>
       </c>
       <c r="J3" s="6" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="17" x14ac:dyDescent="0.2">
@@ -5878,19 +5906,19 @@
         <v>43</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="E4" s="4">
         <v>3013454562</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="G4" s="4" t="s">
         <v>0</v>
@@ -5902,7 +5930,7 @@
         <v>1992</v>
       </c>
       <c r="J4" s="6" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="17" x14ac:dyDescent="0.2">
@@ -5910,19 +5938,19 @@
         <v>47</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="E5" s="4">
         <v>3013454562</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="G5" s="4" t="s">
         <v>0</v>
@@ -5934,7 +5962,7 @@
         <v>1993</v>
       </c>
       <c r="J5" s="6" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="17" x14ac:dyDescent="0.2">
@@ -5942,19 +5970,19 @@
         <v>47</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="E6" s="4">
         <v>3013454562</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="G6" s="4" t="s">
         <v>0</v>
@@ -5966,7 +5994,7 @@
         <v>1994</v>
       </c>
       <c r="J6" s="6" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="17" x14ac:dyDescent="0.2">
@@ -5974,19 +6002,19 @@
         <v>47</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="E7" s="4">
         <v>3013454562</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="G7" s="4" t="s">
         <v>0</v>
@@ -5998,12 +6026,12 @@
         <v>1995</v>
       </c>
       <c r="J7" s="6" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="I12" s="6" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
     </row>
   </sheetData>
@@ -6017,7 +6045,7 @@
   <dimension ref="A1:K9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H6" sqref="H6:K9"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="27" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6051,7 +6079,7 @@
         <v>100</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>102</v>
@@ -6060,10 +6088,10 @@
         <v>103</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="17" x14ac:dyDescent="0.2">
@@ -6101,75 +6129,81 @@
     </row>
     <row r="3" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="D3" s="2"/>
+      <c r="D3" s="28" t="s">
+        <v>265</v>
+      </c>
       <c r="E3" s="2"/>
       <c r="F3" s="2">
         <v>90</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="D4" s="2"/>
+        <v>170</v>
+      </c>
+      <c r="D4" s="28" t="s">
+        <v>265</v>
+      </c>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
       <c r="G4" s="2" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="D5" s="2"/>
+      <c r="D5" s="28" t="s">
+        <v>265</v>
+      </c>
       <c r="E5" s="2"/>
       <c r="F5" s="2">
         <v>100</v>
@@ -6178,24 +6212,24 @@
         <v>0</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="51" x14ac:dyDescent="0.2">
       <c r="A6" s="20" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="B6" s="20" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="C6" s="20" t="s">
         <v>77</v>
@@ -6211,89 +6245,95 @@
         <v>0</v>
       </c>
       <c r="H6" s="20" t="s">
+        <v>335</v>
+      </c>
+      <c r="I6" s="20" t="s">
+        <v>336</v>
+      </c>
+      <c r="J6" s="20" t="s">
         <v>337</v>
       </c>
-      <c r="I6" s="20" t="s">
+      <c r="K6" s="20" t="s">
         <v>338</v>
-      </c>
-      <c r="J6" s="20" t="s">
-        <v>339</v>
-      </c>
-      <c r="K6" s="20" t="s">
-        <v>340</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="34" x14ac:dyDescent="0.2">
       <c r="A7" s="20" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="B7" s="20" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="C7" s="20" t="s">
         <v>78</v>
       </c>
-      <c r="D7" s="20"/>
+      <c r="D7" s="29" t="s">
+        <v>265</v>
+      </c>
       <c r="E7" s="20"/>
       <c r="F7" s="20">
         <v>90</v>
       </c>
       <c r="G7" s="20" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="H7" s="20" t="s">
+        <v>339</v>
+      </c>
+      <c r="I7" s="20" t="s">
+        <v>340</v>
+      </c>
+      <c r="J7" s="20" t="s">
         <v>341</v>
       </c>
-      <c r="I7" s="20" t="s">
+      <c r="K7" s="20" t="s">
         <v>342</v>
-      </c>
-      <c r="J7" s="20" t="s">
-        <v>343</v>
-      </c>
-      <c r="K7" s="20" t="s">
-        <v>344</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="20" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B8" s="20" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="C8" s="20" t="s">
-        <v>172</v>
-      </c>
-      <c r="D8" s="20"/>
+        <v>170</v>
+      </c>
+      <c r="D8" s="29" t="s">
+        <v>265</v>
+      </c>
       <c r="E8" s="20"/>
       <c r="F8" s="20"/>
       <c r="G8" s="20" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="H8" s="20" t="s">
+        <v>343</v>
+      </c>
+      <c r="I8" s="20" t="s">
+        <v>344</v>
+      </c>
+      <c r="J8" s="20" t="s">
         <v>345</v>
       </c>
-      <c r="I8" s="20" t="s">
+      <c r="K8" s="20" t="s">
         <v>346</v>
-      </c>
-      <c r="J8" s="20" t="s">
-        <v>347</v>
-      </c>
-      <c r="K8" s="20" t="s">
-        <v>348</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="34" x14ac:dyDescent="0.2">
       <c r="A9" s="20" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="B9" s="20" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="C9" s="20" t="s">
         <v>78</v>
       </c>
-      <c r="D9" s="20"/>
+      <c r="D9" s="29" t="s">
+        <v>265</v>
+      </c>
       <c r="E9" s="20"/>
       <c r="F9" s="20">
         <v>100</v>
@@ -6302,16 +6342,16 @@
         <v>0</v>
       </c>
       <c r="H9" s="20" t="s">
+        <v>347</v>
+      </c>
+      <c r="I9" s="20" t="s">
+        <v>348</v>
+      </c>
+      <c r="J9" s="20" t="s">
         <v>349</v>
       </c>
-      <c r="I9" s="20" t="s">
+      <c r="K9" s="20" t="s">
         <v>350</v>
-      </c>
-      <c r="J9" s="20" t="s">
-        <v>351</v>
-      </c>
-      <c r="K9" s="20" t="s">
-        <v>352</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changed  Fanconi screener assertion code based on multiple scenarios
</commit_message>
<xml_diff>
--- a/src/test/java/CHARMS/resources/data.xlsx
+++ b/src/test/java/CHARMS/resources/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jains18/git/CBIIT-Test-Automation/CBIIT-Test-Automation/src/test/java/CHARMS/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB65FBF4-05F8-E441-B958-A01DF48600B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B959F6BE-7B6A-A542-9345-B92980057D74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="720" yWindow="760" windowWidth="26000" windowHeight="17640" activeTab="2" xr2:uid="{B3E53782-D40D-CC47-BA00-27DFD8C445AF}"/>
+    <workbookView xWindow="720" yWindow="760" windowWidth="44440" windowHeight="17640" xr2:uid="{B3E53782-D40D-CC47-BA00-27DFD8C445AF}"/>
   </bookViews>
   <sheets>
     <sheet name="FanconiScreener" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1298" uniqueCount="492">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1317" uniqueCount="500">
   <si>
     <t>Yes</t>
   </si>
@@ -609,9 +609,6 @@
   </si>
   <si>
     <t>RaceList</t>
-  </si>
-  <si>
-    <t>Caucasian (white), Black/African American, Native Hawaiian/Other Pacific Islander, American Indian/Alaskan Native, Asian, Other</t>
   </si>
   <si>
     <t>AreYouCompletingThisQuestionnaireForSomeoneElse</t>
@@ -1521,6 +1518,33 @@
   To submit your responses, you must continue in the questionnaire by clicking the forward arrow below.  
 The information you have provided will be reviewed by our study team.  If it is determined that you are eligible to participate in the RASopathy Study, you will receive an email with further details, including instructions to log in to a secure study portal. If the team decides that you are not eligible, you will receive an email explaining why. In the meantime, you should receive an email confirming this submission.
   Please feel free to call at any time if you have any questions regarding this protocol and ask to speak with the RASopathies Study nurse. Our toll-free phone number is 1-800-518-8474 or 301-212-5250. Thank you for your willingness to consider joining our research effort.  We could not do vital studies like this without the help of dedicated patients and families.  </t>
+  </si>
+  <si>
+    <t>sj.fanconitester3@yopmail.com</t>
+  </si>
+  <si>
+    <t>sj.fanconitester4@yopmail.com</t>
+  </si>
+  <si>
+    <t>sj.fanconitester5@yopmail.com</t>
+  </si>
+  <si>
+    <t>sj.fanconitester6@yopmail.com</t>
+  </si>
+  <si>
+    <t>sj.fanconitester7@yopmail.com</t>
+  </si>
+  <si>
+    <t>sj.fanconitester8@yopmail.com</t>
+  </si>
+  <si>
+    <t>sj.fanconitester9@yopmail.com</t>
+  </si>
+  <si>
+    <t>sj.fanconitester10@yopmail.com</t>
+  </si>
+  <si>
+    <t>Caucasian (white), Black/African American, Native Hawaiian/Other Pacific Islander, American Indian/Alaskan Native, Asian,  Other (please specify)</t>
   </si>
 </sst>
 </file>
@@ -2168,9 +2192,9 @@
   </sheetPr>
   <dimension ref="A1:EP18"/>
   <sheetViews>
-    <sheetView topLeftCell="L1" zoomScale="113" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="N1" zoomScale="113" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="T2" sqref="T2"/>
+      <selection pane="bottomLeft" activeCell="AC3" sqref="AC3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2232,16 +2256,16 @@
   <sheetData>
     <row r="1" spans="1:146" s="13" customFormat="1" ht="85" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
+        <v>189</v>
+      </c>
+      <c r="B1" s="7" t="s">
         <v>190</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="C1" s="7" t="s">
         <v>191</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="D1" s="7" t="s">
         <v>192</v>
-      </c>
-      <c r="D1" s="7" t="s">
-        <v>193</v>
       </c>
       <c r="E1" s="7" t="s">
         <v>126</v>
@@ -2265,13 +2289,13 @@
         <v>138</v>
       </c>
       <c r="L1" s="7" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="M1" s="7" t="s">
         <v>140</v>
       </c>
       <c r="N1" s="8" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="O1" s="9" t="s">
         <v>1</v>
@@ -2286,10 +2310,10 @@
         <v>125</v>
       </c>
       <c r="S1" s="9" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="T1" s="9" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="U1" s="10" t="s">
         <v>4</v>
@@ -2307,10 +2331,10 @@
         <v>182</v>
       </c>
       <c r="Z1" s="11" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="AA1" s="11" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="AB1" s="7" t="s">
         <v>7</v>
@@ -2337,10 +2361,10 @@
         <v>39</v>
       </c>
       <c r="AJ1" s="12" t="s">
+        <v>425</v>
+      </c>
+      <c r="AK1" s="12" t="s">
         <v>426</v>
-      </c>
-      <c r="AK1" s="12" t="s">
-        <v>427</v>
       </c>
       <c r="AL1" s="14" t="s">
         <v>14</v>
@@ -2382,13 +2406,13 @@
         <v>188</v>
       </c>
       <c r="AY1" s="15" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="AZ1" s="16" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="BA1" s="16" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="BB1" s="16" t="s">
         <v>53</v>
@@ -2424,52 +2448,52 @@
         <v>52</v>
       </c>
       <c r="BM1" s="13" t="s">
+        <v>200</v>
+      </c>
+      <c r="BN1" s="13" t="s">
+        <v>204</v>
+      </c>
+      <c r="BO1" s="13" t="s">
+        <v>205</v>
+      </c>
+      <c r="BP1" s="13" t="s">
+        <v>206</v>
+      </c>
+      <c r="BQ1" s="13" t="s">
         <v>201</v>
       </c>
-      <c r="BN1" s="13" t="s">
-        <v>205</v>
-      </c>
-      <c r="BO1" s="13" t="s">
-        <v>206</v>
-      </c>
-      <c r="BP1" s="13" t="s">
+      <c r="BR1" s="13" t="s">
+        <v>202</v>
+      </c>
+      <c r="BS1" s="13" t="s">
+        <v>203</v>
+      </c>
+      <c r="BT1" s="13" t="s">
+        <v>361</v>
+      </c>
+      <c r="BU1" s="13" t="s">
+        <v>360</v>
+      </c>
+      <c r="BV1" s="13" t="s">
+        <v>208</v>
+      </c>
+      <c r="BW1" s="13" t="s">
+        <v>262</v>
+      </c>
+      <c r="BX1" s="13" t="s">
+        <v>263</v>
+      </c>
+      <c r="BY1" s="13" t="s">
         <v>207</v>
       </c>
-      <c r="BQ1" s="13" t="s">
-        <v>202</v>
-      </c>
-      <c r="BR1" s="13" t="s">
-        <v>203</v>
-      </c>
-      <c r="BS1" s="13" t="s">
-        <v>204</v>
-      </c>
-      <c r="BT1" s="13" t="s">
+      <c r="BZ1" s="13" t="s">
+        <v>209</v>
+      </c>
+      <c r="CA1" s="13" t="s">
+        <v>210</v>
+      </c>
+      <c r="CB1" s="13" t="s">
         <v>362</v>
-      </c>
-      <c r="BU1" s="13" t="s">
-        <v>361</v>
-      </c>
-      <c r="BV1" s="13" t="s">
-        <v>209</v>
-      </c>
-      <c r="BW1" s="13" t="s">
-        <v>263</v>
-      </c>
-      <c r="BX1" s="13" t="s">
-        <v>264</v>
-      </c>
-      <c r="BY1" s="13" t="s">
-        <v>208</v>
-      </c>
-      <c r="BZ1" s="13" t="s">
-        <v>210</v>
-      </c>
-      <c r="CA1" s="13" t="s">
-        <v>211</v>
-      </c>
-      <c r="CB1" s="13" t="s">
-        <v>363</v>
       </c>
       <c r="CC1" s="13" t="s">
         <v>185</v>
@@ -2493,49 +2517,49 @@
         <v>71</v>
       </c>
       <c r="CJ1" s="13" t="s">
+        <v>211</v>
+      </c>
+      <c r="CK1" s="13" t="s">
         <v>212</v>
       </c>
-      <c r="CK1" s="13" t="s">
+      <c r="CL1" s="13" t="s">
         <v>213</v>
       </c>
-      <c r="CL1" s="13" t="s">
+      <c r="CM1" s="13" t="s">
         <v>214</v>
       </c>
-      <c r="CM1" s="13" t="s">
+      <c r="CN1" s="13" t="s">
+        <v>236</v>
+      </c>
+      <c r="CO1" s="13" t="s">
+        <v>237</v>
+      </c>
+      <c r="CP1" s="13" t="s">
+        <v>238</v>
+      </c>
+      <c r="CQ1" s="13" t="s">
+        <v>239</v>
+      </c>
+      <c r="CR1" s="13" t="s">
+        <v>240</v>
+      </c>
+      <c r="CS1" s="13" t="s">
         <v>215</v>
       </c>
-      <c r="CN1" s="13" t="s">
-        <v>237</v>
-      </c>
-      <c r="CO1" s="13" t="s">
-        <v>238</v>
-      </c>
-      <c r="CP1" s="13" t="s">
-        <v>239</v>
-      </c>
-      <c r="CQ1" s="13" t="s">
-        <v>240</v>
-      </c>
-      <c r="CR1" s="13" t="s">
-        <v>241</v>
-      </c>
-      <c r="CS1" s="13" t="s">
+      <c r="CT1" s="13" t="s">
         <v>216</v>
       </c>
-      <c r="CT1" s="13" t="s">
-        <v>217</v>
-      </c>
       <c r="CU1" s="13" t="s">
+        <v>226</v>
+      </c>
+      <c r="CV1" s="13" t="s">
+        <v>225</v>
+      </c>
+      <c r="CW1" s="13" t="s">
+        <v>224</v>
+      </c>
+      <c r="CX1" s="13" t="s">
         <v>227</v>
-      </c>
-      <c r="CV1" s="13" t="s">
-        <v>226</v>
-      </c>
-      <c r="CW1" s="13" t="s">
-        <v>225</v>
-      </c>
-      <c r="CX1" s="13" t="s">
-        <v>228</v>
       </c>
       <c r="CY1" s="13" t="s">
         <v>80</v>
@@ -2562,19 +2586,19 @@
         <v>91</v>
       </c>
       <c r="DG1" s="13" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="DH1" s="13" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="DI1" s="13" t="s">
         <v>109</v>
       </c>
       <c r="DJ1" s="13" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="DK1" s="13" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="DL1" s="13" t="s">
         <v>112</v>
@@ -2586,88 +2610,88 @@
         <v>116</v>
       </c>
       <c r="DO1" s="13" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="DP1" s="13" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="DQ1" s="13" t="s">
+        <v>228</v>
+      </c>
+      <c r="DR1" s="13" t="s">
         <v>229</v>
       </c>
-      <c r="DR1" s="13" t="s">
+      <c r="DS1" s="13" t="s">
         <v>230</v>
       </c>
-      <c r="DS1" s="13" t="s">
+      <c r="DT1" s="13" t="s">
         <v>231</v>
       </c>
-      <c r="DT1" s="13" t="s">
+      <c r="DU1" s="13" t="s">
         <v>232</v>
       </c>
-      <c r="DU1" s="13" t="s">
+      <c r="DV1" s="13" t="s">
         <v>233</v>
       </c>
-      <c r="DV1" s="13" t="s">
+      <c r="DW1" s="13" t="s">
         <v>234</v>
       </c>
-      <c r="DW1" s="13" t="s">
+      <c r="DX1" s="13" t="s">
         <v>235</v>
       </c>
-      <c r="DX1" s="13" t="s">
-        <v>236</v>
-      </c>
       <c r="DY1" s="17" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="DZ1" s="17" t="s">
+        <v>244</v>
+      </c>
+      <c r="EA1" s="17" t="s">
         <v>245</v>
       </c>
-      <c r="EA1" s="17" t="s">
+      <c r="EB1" s="17" t="s">
         <v>246</v>
       </c>
-      <c r="EB1" s="17" t="s">
+      <c r="EC1" s="17" t="s">
         <v>247</v>
       </c>
-      <c r="EC1" s="17" t="s">
+      <c r="ED1" s="17" t="s">
         <v>248</v>
       </c>
-      <c r="ED1" s="17" t="s">
+      <c r="EE1" s="17" t="s">
         <v>249</v>
       </c>
-      <c r="EE1" s="17" t="s">
+      <c r="EF1" s="17" t="s">
         <v>250</v>
       </c>
-      <c r="EF1" s="17" t="s">
+      <c r="EG1" s="17" t="s">
         <v>251</v>
       </c>
-      <c r="EG1" s="17" t="s">
+      <c r="EH1" s="17" t="s">
         <v>252</v>
       </c>
-      <c r="EH1" s="17" t="s">
+      <c r="EI1" s="17" t="s">
         <v>253</v>
       </c>
-      <c r="EI1" s="17" t="s">
+      <c r="EJ1" s="17" t="s">
+        <v>255</v>
+      </c>
+      <c r="EK1" s="17" t="s">
         <v>254</v>
       </c>
-      <c r="EJ1" s="17" t="s">
+      <c r="EL1" s="17" t="s">
         <v>256</v>
       </c>
-      <c r="EK1" s="17" t="s">
-        <v>255</v>
-      </c>
-      <c r="EL1" s="17" t="s">
+      <c r="EM1" s="17" t="s">
         <v>257</v>
       </c>
-      <c r="EM1" s="17" t="s">
+      <c r="EN1" s="17" t="s">
         <v>258</v>
       </c>
-      <c r="EN1" s="17" t="s">
+      <c r="EO1" s="17" t="s">
         <v>259</v>
       </c>
-      <c r="EO1" s="17" t="s">
+      <c r="EP1" s="17" t="s">
         <v>260</v>
-      </c>
-      <c r="EP1" s="17" t="s">
-        <v>261</v>
       </c>
     </row>
     <row r="2" spans="1:146" s="21" customFormat="1" ht="85" x14ac:dyDescent="0.2">
@@ -2675,13 +2699,13 @@
         <v>38</v>
       </c>
       <c r="B2" s="21" t="s">
+        <v>295</v>
+      </c>
+      <c r="C2" s="21" t="s">
         <v>296</v>
       </c>
-      <c r="C2" s="21" t="s">
-        <v>297</v>
-      </c>
       <c r="D2" s="21" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="N2" s="21" t="s">
         <v>0</v>
@@ -2690,13 +2714,13 @@
         <v>1948</v>
       </c>
       <c r="P2" s="21" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="Q2" s="21">
         <v>21</v>
       </c>
       <c r="R2" s="30" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="S2" s="22"/>
       <c r="T2" s="21">
@@ -2715,19 +2739,19 @@
         <v>0</v>
       </c>
       <c r="AA2" s="21" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="AB2" s="21" t="s">
         <v>22</v>
       </c>
       <c r="AC2" s="21" t="s">
+        <v>195</v>
+      </c>
+      <c r="AD2" s="21" t="s">
         <v>196</v>
       </c>
-      <c r="AD2" s="21" t="s">
+      <c r="AE2" s="21" t="s">
         <v>197</v>
-      </c>
-      <c r="AE2" s="21" t="s">
-        <v>198</v>
       </c>
       <c r="AF2" s="21" t="s">
         <v>23</v>
@@ -2736,13 +2760,13 @@
         <v>28907</v>
       </c>
       <c r="AH2" s="18" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="AI2" s="18" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="AJ2" s="19" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="AK2" s="19"/>
       <c r="AL2" s="21">
@@ -2782,7 +2806,7 @@
         <v>40</v>
       </c>
       <c r="AX2" s="21" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="AY2" s="21" t="s">
         <v>0</v>
@@ -2791,7 +2815,7 @@
         <v>0</v>
       </c>
       <c r="BA2" s="21" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="BB2" s="21" t="s">
         <v>37</v>
@@ -2845,10 +2869,10 @@
         <v>65</v>
       </c>
       <c r="BW2" s="23" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="BX2" s="23" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="BY2" s="21" t="s">
         <v>66</v>
@@ -2860,7 +2884,7 @@
         <v>0</v>
       </c>
       <c r="CE2" s="21" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="CF2" s="21" t="s">
         <v>74</v>
@@ -2947,7 +2971,7 @@
         <v>111</v>
       </c>
       <c r="DK2" s="21" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="DL2" s="21" t="s">
         <v>113</v>
@@ -2962,7 +2986,7 @@
         <v>0</v>
       </c>
       <c r="DP2" s="21" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="DQ2" s="21" t="s">
         <v>120</v>
@@ -2980,7 +3004,7 @@
         <v>122</v>
       </c>
       <c r="DV2" s="21" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="DW2" s="21" t="s">
         <v>47</v>
@@ -3025,7 +3049,7 @@
         <v>0</v>
       </c>
       <c r="EK2" s="27" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="EL2" s="21" t="s">
         <v>0</v>
@@ -3054,7 +3078,7 @@
         <v>133</v>
       </c>
       <c r="D3" s="21" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="N3" s="21" t="s">
         <v>134</v>
@@ -3063,13 +3087,13 @@
         <v>1920</v>
       </c>
       <c r="P3" s="21" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="Q3" s="21">
         <v>23</v>
       </c>
       <c r="R3" s="30" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="S3" s="22"/>
       <c r="T3" s="22"/>
@@ -3085,6 +3109,9 @@
       <c r="Z3" s="21" t="s">
         <v>134</v>
       </c>
+      <c r="AA3" s="21" t="s">
+        <v>420</v>
+      </c>
       <c r="AB3" s="21" t="s">
         <v>166</v>
       </c>
@@ -3095,7 +3122,7 @@
         <v>142</v>
       </c>
       <c r="AJ3" s="19" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="AK3" s="19"/>
       <c r="AL3" s="21">
@@ -3135,7 +3162,7 @@
         <v>40</v>
       </c>
       <c r="AX3" s="21" t="s">
-        <v>189</v>
+        <v>418</v>
       </c>
       <c r="AZ3" s="21" t="s">
         <v>134</v>
@@ -3147,7 +3174,7 @@
         <v>146</v>
       </c>
       <c r="BO3" s="22" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="BQ3" s="21" t="s">
         <v>0</v>
@@ -3168,7 +3195,7 @@
         <v>0</v>
       </c>
       <c r="CE3" s="21" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="CF3" s="21" t="s">
         <v>74</v>
@@ -3213,7 +3240,7 @@
         <v>146</v>
       </c>
       <c r="CV3" s="22" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="CX3" s="21" t="s">
         <v>79</v>
@@ -3246,10 +3273,10 @@
         <v>157</v>
       </c>
       <c r="DL3" s="21" t="s">
+        <v>320</v>
+      </c>
+      <c r="DM3" s="21" t="s">
         <v>321</v>
-      </c>
-      <c r="DM3" s="21" t="s">
-        <v>322</v>
       </c>
       <c r="DN3" s="21">
         <v>3028976789</v>
@@ -3258,7 +3285,7 @@
         <v>134</v>
       </c>
       <c r="DP3" s="21" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="DQ3" s="21" t="s">
         <v>120</v>
@@ -3276,7 +3303,7 @@
         <v>122</v>
       </c>
       <c r="DV3" s="21" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="DW3" s="21" t="s">
         <v>47</v>
@@ -3321,7 +3348,7 @@
         <v>0</v>
       </c>
       <c r="EK3" s="27" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="EL3" s="21" t="s">
         <v>0</v>
@@ -3350,7 +3377,7 @@
         <v>159</v>
       </c>
       <c r="D4" s="21" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="N4" s="21" t="s">
         <v>145</v>
@@ -3359,13 +3386,13 @@
         <v>1910</v>
       </c>
       <c r="P4" s="21" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="Q4" s="21">
         <v>21</v>
       </c>
       <c r="R4" s="30" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="S4" s="22"/>
       <c r="T4" s="22"/>
@@ -3381,8 +3408,11 @@
       <c r="Z4" s="21" t="s">
         <v>134</v>
       </c>
+      <c r="AA4" s="21" t="s">
+        <v>420</v>
+      </c>
       <c r="AB4" s="21" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="AH4" s="19" t="s">
         <v>144</v>
@@ -3390,7 +3420,9 @@
       <c r="AI4" s="18" t="s">
         <v>144</v>
       </c>
-      <c r="AJ4" s="18"/>
+      <c r="AJ4" s="19" t="s">
+        <v>491</v>
+      </c>
       <c r="AK4" s="18"/>
       <c r="AL4" s="21">
         <v>3015774089</v>
@@ -3441,7 +3473,7 @@
         <v>0</v>
       </c>
       <c r="CE4" s="21" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="CF4" s="21" t="s">
         <v>74</v>
@@ -3495,7 +3527,7 @@
         <v>171</v>
       </c>
       <c r="DE4" s="21" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="DF4" s="21" t="s">
         <v>172</v>
@@ -3513,10 +3545,10 @@
         <v>175</v>
       </c>
       <c r="DL4" s="21" t="s">
+        <v>320</v>
+      </c>
+      <c r="DM4" s="21" t="s">
         <v>321</v>
-      </c>
-      <c r="DM4" s="21" t="s">
-        <v>322</v>
       </c>
       <c r="DN4" s="21">
         <v>3028976789</v>
@@ -3525,7 +3557,7 @@
         <v>0</v>
       </c>
       <c r="DP4" s="21" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="DQ4" s="21" t="s">
         <v>120</v>
@@ -3543,7 +3575,7 @@
         <v>122</v>
       </c>
       <c r="DV4" s="21" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="DW4" s="21" t="s">
         <v>47</v>
@@ -3588,7 +3620,7 @@
         <v>134</v>
       </c>
       <c r="EK4" s="27" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="EL4" s="21" t="s">
         <v>134</v>
@@ -3617,7 +3649,7 @@
         <v>161</v>
       </c>
       <c r="D5" s="21" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="N5" s="21" t="s">
         <v>145</v>
@@ -3626,13 +3658,13 @@
         <v>1925</v>
       </c>
       <c r="P5" s="21" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="Q5" s="21">
         <v>21</v>
       </c>
       <c r="R5" s="30" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="S5" s="22"/>
       <c r="T5" s="22"/>
@@ -3643,16 +3675,19 @@
         <v>180</v>
       </c>
       <c r="W5" s="21" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="X5" s="21" t="s">
         <v>180</v>
       </c>
       <c r="Y5" s="21" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="Z5" s="21" t="s">
         <v>134</v>
+      </c>
+      <c r="AA5" s="21" t="s">
+        <v>420</v>
       </c>
       <c r="AB5" s="21" t="s">
         <v>179</v>
@@ -3663,7 +3698,9 @@
       <c r="AI5" s="19" t="s">
         <v>162</v>
       </c>
-      <c r="AJ5" s="19"/>
+      <c r="AJ5" s="19" t="s">
+        <v>492</v>
+      </c>
       <c r="AK5" s="19"/>
       <c r="AL5" s="21">
         <v>3015774089</v>
@@ -3714,7 +3751,7 @@
         <v>0</v>
       </c>
       <c r="CE5" s="21" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="CF5" s="21" t="s">
         <v>74</v>
@@ -3756,7 +3793,7 @@
         <v>146</v>
       </c>
       <c r="CV5" s="22" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="CX5" s="21" t="s">
         <v>79</v>
@@ -3768,13 +3805,13 @@
         <v>170</v>
       </c>
       <c r="DD5" s="21" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="DE5" s="21" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="DF5" s="21" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="DG5" s="21" t="s">
         <v>0</v>
@@ -3786,13 +3823,13 @@
         <v>37</v>
       </c>
       <c r="DK5" s="21" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="DL5" s="21" t="s">
+        <v>320</v>
+      </c>
+      <c r="DM5" s="21" t="s">
         <v>321</v>
-      </c>
-      <c r="DM5" s="21" t="s">
-        <v>322</v>
       </c>
       <c r="DN5" s="21">
         <v>3028976789</v>
@@ -3801,7 +3838,7 @@
         <v>0</v>
       </c>
       <c r="DP5" s="21" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="DQ5" s="21" t="s">
         <v>120</v>
@@ -3819,7 +3856,7 @@
         <v>122</v>
       </c>
       <c r="DV5" s="21" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="DW5" s="21" t="s">
         <v>47</v>
@@ -3864,7 +3901,7 @@
         <v>145</v>
       </c>
       <c r="EK5" s="27" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="EL5" s="21" t="s">
         <v>145</v>
@@ -3893,7 +3930,7 @@
         <v>177</v>
       </c>
       <c r="D6" s="21" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="N6" s="21" t="s">
         <v>145</v>
@@ -3902,13 +3939,13 @@
         <v>1950</v>
       </c>
       <c r="P6" s="21" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="Q6" s="21">
         <v>26</v>
       </c>
       <c r="R6" s="30" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="S6" s="22"/>
       <c r="T6" s="22"/>
@@ -3924,8 +3961,11 @@
       <c r="Z6" s="21" t="s">
         <v>0</v>
       </c>
+      <c r="AA6" s="21" t="s">
+        <v>420</v>
+      </c>
       <c r="AB6" s="21" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="AH6" s="18" t="s">
         <v>178</v>
@@ -3933,6 +3973,9 @@
       <c r="AI6" s="21" t="s">
         <v>178</v>
       </c>
+      <c r="AJ6" s="19" t="s">
+        <v>493</v>
+      </c>
       <c r="AL6" s="21">
         <v>3015774089</v>
       </c>
@@ -3974,7 +4017,7 @@
         <v>145</v>
       </c>
       <c r="CE6" s="21" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="CL6" s="21" t="s">
         <v>145</v>
@@ -3990,10 +4033,10 @@
         <v>174</v>
       </c>
       <c r="DJ6" s="21" t="s">
+        <v>351</v>
+      </c>
+      <c r="DK6" s="21" t="s">
         <v>352</v>
-      </c>
-      <c r="DK6" s="21" t="s">
-        <v>353</v>
       </c>
       <c r="DL6" s="21" t="s">
         <v>113</v>
@@ -4008,7 +4051,7 @@
         <v>134</v>
       </c>
       <c r="DP6" s="21" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="DQ6" s="21" t="s">
         <v>120</v>
@@ -4026,7 +4069,7 @@
         <v>122</v>
       </c>
       <c r="DV6" s="21" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="DW6" s="21" t="s">
         <v>47</v>
@@ -4071,7 +4114,7 @@
         <v>134</v>
       </c>
       <c r="EK6" s="27" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="EL6" s="21" t="s">
         <v>134</v>
@@ -4094,13 +4137,13 @@
         <v>38</v>
       </c>
       <c r="B7" s="21" t="s">
+        <v>313</v>
+      </c>
+      <c r="C7" s="21" t="s">
         <v>314</v>
       </c>
-      <c r="C7" s="21" t="s">
-        <v>315</v>
-      </c>
       <c r="D7" s="21" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="N7" s="21" t="s">
         <v>134</v>
@@ -4109,13 +4152,13 @@
         <v>1940</v>
       </c>
       <c r="P7" s="21" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="Q7" s="21">
         <v>11</v>
       </c>
       <c r="R7" s="30" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="S7" s="22"/>
       <c r="T7" s="22"/>
@@ -4131,16 +4174,21 @@
       <c r="Z7" s="21" t="s">
         <v>134</v>
       </c>
+      <c r="AA7" s="21" t="s">
+        <v>420</v>
+      </c>
       <c r="AB7" s="21" t="s">
         <v>183</v>
       </c>
       <c r="AH7" s="18" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="AI7" s="18" t="s">
-        <v>318</v>
-      </c>
-      <c r="AJ7" s="18"/>
+        <v>317</v>
+      </c>
+      <c r="AJ7" s="19" t="s">
+        <v>494</v>
+      </c>
       <c r="AK7" s="18"/>
       <c r="AL7" s="21">
         <v>3015774089</v>
@@ -4177,7 +4225,7 @@
         <v>184</v>
       </c>
       <c r="BT7" s="21" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="BU7" s="21" t="s">
         <v>0</v>
@@ -4195,10 +4243,10 @@
         <v>134</v>
       </c>
       <c r="CB7" s="21" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="CE7" s="21" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="CJ7" s="21" t="s">
         <v>134</v>
@@ -4217,7 +4265,7 @@
         <v>110</v>
       </c>
       <c r="DJ7" s="21" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="DL7" s="21" t="s">
         <v>113</v>
@@ -4232,7 +4280,7 @@
         <v>134</v>
       </c>
       <c r="DP7" s="21" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="DQ7" s="21" t="s">
         <v>120</v>
@@ -4250,7 +4298,7 @@
         <v>122</v>
       </c>
       <c r="DV7" s="21" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="DW7" s="21" t="s">
         <v>47</v>
@@ -4295,7 +4343,7 @@
         <v>0</v>
       </c>
       <c r="EK7" s="27" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="EL7" s="21" t="s">
         <v>0</v>
@@ -4318,13 +4366,13 @@
         <v>38</v>
       </c>
       <c r="B8" s="21" t="s">
+        <v>315</v>
+      </c>
+      <c r="C8" s="21" t="s">
         <v>316</v>
       </c>
-      <c r="C8" s="21" t="s">
-        <v>317</v>
-      </c>
       <c r="D8" s="21" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="N8" s="21" t="s">
         <v>134</v>
@@ -4333,13 +4381,13 @@
         <v>1930</v>
       </c>
       <c r="P8" s="21" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="Q8" s="21">
         <v>30</v>
       </c>
       <c r="R8" s="30" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="S8" s="22"/>
       <c r="T8" s="22"/>
@@ -4355,17 +4403,20 @@
       <c r="Z8" s="21" t="s">
         <v>134</v>
       </c>
+      <c r="AA8" s="21" t="s">
+        <v>420</v>
+      </c>
       <c r="AB8" s="21" t="s">
         <v>22</v>
       </c>
       <c r="AC8" s="21" t="s">
+        <v>195</v>
+      </c>
+      <c r="AD8" s="21" t="s">
         <v>196</v>
       </c>
-      <c r="AD8" s="21" t="s">
+      <c r="AE8" s="21" t="s">
         <v>197</v>
-      </c>
-      <c r="AE8" s="21" t="s">
-        <v>198</v>
       </c>
       <c r="AF8" s="21" t="s">
         <v>23</v>
@@ -4374,12 +4425,14 @@
         <v>28907</v>
       </c>
       <c r="AH8" s="18" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="AI8" s="18" t="s">
-        <v>319</v>
-      </c>
-      <c r="AJ8" s="18"/>
+        <v>318</v>
+      </c>
+      <c r="AJ8" s="19" t="s">
+        <v>495</v>
+      </c>
       <c r="AK8" s="18"/>
       <c r="AL8" s="21">
         <v>3015774089</v>
@@ -4413,7 +4466,7 @@
         <v>134</v>
       </c>
       <c r="CE8" s="21" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="CL8" s="21" t="s">
         <v>134</v>
@@ -4429,7 +4482,7 @@
         <v>47</v>
       </c>
       <c r="DK8" s="21" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="DL8" s="21" t="s">
         <v>113</v>
@@ -4444,7 +4497,7 @@
         <v>134</v>
       </c>
       <c r="DP8" s="21" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="DQ8" s="21" t="s">
         <v>120</v>
@@ -4462,7 +4515,7 @@
         <v>122</v>
       </c>
       <c r="DV8" s="21" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="DW8" s="21" t="s">
         <v>47</v>
@@ -4507,7 +4560,7 @@
         <v>0</v>
       </c>
       <c r="EK8" s="27" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="EL8" s="21" t="s">
         <v>0</v>
@@ -4530,13 +4583,13 @@
         <v>38</v>
       </c>
       <c r="B9" s="21" t="s">
+        <v>373</v>
+      </c>
+      <c r="C9" s="21" t="s">
         <v>374</v>
       </c>
-      <c r="C9" s="21" t="s">
-        <v>375</v>
-      </c>
       <c r="D9" s="21" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="N9" s="21" t="s">
         <v>0</v>
@@ -4545,13 +4598,13 @@
         <v>1935</v>
       </c>
       <c r="P9" s="21" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="Q9" s="21">
         <v>29</v>
       </c>
       <c r="R9" s="30" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="S9" s="22"/>
       <c r="T9" s="22"/>
@@ -4567,16 +4620,21 @@
       <c r="Z9" s="21" t="s">
         <v>0</v>
       </c>
+      <c r="AA9" s="21" t="s">
+        <v>420</v>
+      </c>
       <c r="AB9" s="21" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="AH9" s="18" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="AI9" s="18" t="s">
-        <v>320</v>
-      </c>
-      <c r="AJ9" s="18"/>
+        <v>319</v>
+      </c>
+      <c r="AJ9" s="19" t="s">
+        <v>496</v>
+      </c>
       <c r="AK9" s="18"/>
       <c r="AL9" s="21">
         <v>3015774089</v>
@@ -4600,7 +4658,7 @@
         <v>0</v>
       </c>
       <c r="BA9" s="21" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="BB9" s="21" t="s">
         <v>37</v>
@@ -4654,7 +4712,7 @@
         <v>0</v>
       </c>
       <c r="CE9" s="21" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="CF9" s="21" t="s">
         <v>74</v>
@@ -4684,7 +4742,7 @@
         <v>134</v>
       </c>
       <c r="CR9" s="21" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="CS9" s="21" t="s">
         <v>134</v>
@@ -4721,7 +4779,7 @@
         <v>0</v>
       </c>
       <c r="DP9" s="21" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="DQ9" s="21" t="s">
         <v>120</v>
@@ -4739,7 +4797,7 @@
         <v>122</v>
       </c>
       <c r="DV9" s="21" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="DW9" s="21" t="s">
         <v>47</v>
@@ -4784,7 +4842,7 @@
         <v>134</v>
       </c>
       <c r="EK9" s="27" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="EL9" s="21" t="s">
         <v>134</v>
@@ -4807,25 +4865,25 @@
         <v>131</v>
       </c>
       <c r="E10" s="21" t="s">
+        <v>411</v>
+      </c>
+      <c r="F10" s="21" t="s">
+        <v>416</v>
+      </c>
+      <c r="G10" s="21" t="s">
         <v>412</v>
       </c>
-      <c r="F10" s="21" t="s">
-        <v>417</v>
-      </c>
-      <c r="G10" s="21" t="s">
-        <v>413</v>
-      </c>
       <c r="H10" s="21" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="I10" s="21" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="J10" s="21" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="K10" s="21" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="M10" s="21" t="s">
         <v>0</v>
@@ -4837,13 +4895,13 @@
         <v>1937</v>
       </c>
       <c r="P10" s="21" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="Q10" s="21">
         <v>27</v>
       </c>
       <c r="R10" s="30" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="S10" s="22"/>
       <c r="T10" s="22"/>
@@ -4854,17 +4912,20 @@
       <c r="Z10" s="21" t="s">
         <v>0</v>
       </c>
+      <c r="AA10" s="21" t="s">
+        <v>420</v>
+      </c>
       <c r="AB10" s="21" t="s">
         <v>22</v>
       </c>
       <c r="AC10" s="21" t="s">
+        <v>195</v>
+      </c>
+      <c r="AD10" s="21" t="s">
         <v>196</v>
       </c>
-      <c r="AD10" s="21" t="s">
+      <c r="AE10" s="21" t="s">
         <v>197</v>
-      </c>
-      <c r="AE10" s="21" t="s">
-        <v>198</v>
       </c>
       <c r="AF10" s="21" t="s">
         <v>23</v>
@@ -4873,12 +4934,14 @@
         <v>28907</v>
       </c>
       <c r="AH10" s="19" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="AI10" s="18" t="s">
-        <v>326</v>
-      </c>
-      <c r="AJ10" s="18"/>
+        <v>325</v>
+      </c>
+      <c r="AJ10" s="19" t="s">
+        <v>497</v>
+      </c>
       <c r="AK10" s="18"/>
       <c r="AL10" s="21">
         <v>3015774089</v>
@@ -4917,13 +4980,13 @@
         <v>40</v>
       </c>
       <c r="AX10" s="21" t="s">
-        <v>189</v>
+        <v>499</v>
       </c>
       <c r="AZ10" s="21" t="s">
         <v>0</v>
       </c>
       <c r="BA10" s="21" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="BB10" s="21" t="s">
         <v>37</v>
@@ -4965,7 +5028,7 @@
         <v>146</v>
       </c>
       <c r="BO10" s="22" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="BQ10" s="21" t="s">
         <v>0</v>
@@ -4977,10 +5040,10 @@
         <v>65</v>
       </c>
       <c r="BW10" s="23" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="BX10" s="23" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="BY10" s="21" t="s">
         <v>66</v>
@@ -4992,16 +5055,16 @@
         <v>0</v>
       </c>
       <c r="CE10" s="21" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="CF10" s="21" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="CG10" s="21" t="s">
         <v>72</v>
       </c>
       <c r="CH10" s="21" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="CI10" s="21" t="s">
         <v>72</v>
@@ -5043,7 +5106,7 @@
         <v>103</v>
       </c>
       <c r="CX10" s="21" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="CY10" s="21" t="s">
         <v>81</v>
@@ -5079,7 +5142,7 @@
         <v>111</v>
       </c>
       <c r="DK10" s="21" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="DL10" s="21" t="s">
         <v>113</v>
@@ -5094,7 +5157,7 @@
         <v>0</v>
       </c>
       <c r="DP10" s="21" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="DQ10" s="21" t="s">
         <v>120</v>
@@ -5112,7 +5175,7 @@
         <v>122</v>
       </c>
       <c r="DV10" s="21" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="DW10" s="21" t="s">
         <v>47</v>
@@ -5157,7 +5220,7 @@
         <v>0</v>
       </c>
       <c r="EK10" s="27" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="EL10" s="21" t="s">
         <v>0</v>
@@ -5180,28 +5243,28 @@
         <v>131</v>
       </c>
       <c r="E11" s="21" t="s">
+        <v>401</v>
+      </c>
+      <c r="F11" s="21" t="s">
+        <v>415</v>
+      </c>
+      <c r="G11" s="21" t="s">
         <v>402</v>
       </c>
-      <c r="F11" s="21" t="s">
-        <v>416</v>
-      </c>
-      <c r="G11" s="21" t="s">
-        <v>403</v>
-      </c>
       <c r="H11" s="21" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="I11" s="21" t="s">
         <v>133</v>
       </c>
       <c r="J11" s="21" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="K11" s="21" t="s">
         <v>47</v>
       </c>
       <c r="L11" s="21" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="M11" s="21" t="s">
         <v>134</v>
@@ -5213,13 +5276,13 @@
         <v>1935</v>
       </c>
       <c r="P11" s="21" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="Q11" s="21">
         <v>21</v>
       </c>
       <c r="R11" s="30" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="S11" s="22"/>
       <c r="T11" s="22"/>
@@ -5229,16 +5292,21 @@
       <c r="Z11" s="21" t="s">
         <v>134</v>
       </c>
+      <c r="AA11" s="21" t="s">
+        <v>420</v>
+      </c>
       <c r="AB11" s="21" t="s">
         <v>166</v>
       </c>
       <c r="AH11" s="18" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="AI11" s="19" t="s">
-        <v>327</v>
-      </c>
-      <c r="AJ11" s="19"/>
+        <v>326</v>
+      </c>
+      <c r="AJ11" s="19" t="s">
+        <v>498</v>
+      </c>
       <c r="AK11" s="19"/>
       <c r="AL11" s="21">
         <v>3015774089</v>
@@ -5287,7 +5355,7 @@
         <v>0</v>
       </c>
       <c r="CE11" s="21" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="CF11" s="21" t="s">
         <v>74</v>
@@ -5330,7 +5398,7 @@
       </c>
       <c r="CV11" s="24"/>
       <c r="CX11" s="21" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="CY11" s="21" t="s">
         <v>81</v>
@@ -5342,7 +5410,7 @@
         <v>171</v>
       </c>
       <c r="DE11" s="21" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="DF11" s="21" t="s">
         <v>172</v>
@@ -5354,7 +5422,7 @@
         <v>108</v>
       </c>
       <c r="DI11" s="21" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="DJ11" s="21" t="s">
         <v>175</v>
@@ -5372,7 +5440,7 @@
         <v>0</v>
       </c>
       <c r="DP11" s="21" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="DQ11" s="21" t="s">
         <v>120</v>
@@ -5390,7 +5458,7 @@
         <v>122</v>
       </c>
       <c r="DV11" s="21" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="DW11" s="21" t="s">
         <v>47</v>
@@ -5435,7 +5503,7 @@
         <v>134</v>
       </c>
       <c r="EK11" s="27" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="EL11" s="21" t="s">
         <v>134</v>
@@ -5458,25 +5526,25 @@
         <v>131</v>
       </c>
       <c r="E12" s="21" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="F12" s="21" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="G12" s="21" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="H12" s="21" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="I12" s="21" t="s">
         <v>159</v>
       </c>
       <c r="J12" s="21" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="K12" s="21" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="M12" s="21" t="s">
         <v>0</v>
@@ -5488,13 +5556,13 @@
         <v>1930</v>
       </c>
       <c r="P12" s="21" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="Q12" s="21">
         <v>30</v>
       </c>
       <c r="R12" s="30" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="S12" s="22"/>
       <c r="T12" s="22"/>
@@ -5504,14 +5572,17 @@
       <c r="Z12" s="21" t="s">
         <v>134</v>
       </c>
+      <c r="AA12" s="21" t="s">
+        <v>420</v>
+      </c>
       <c r="AB12" s="21" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="AH12" s="19" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="AI12" s="19" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="AJ12" s="19"/>
       <c r="AK12" s="19"/>
@@ -5546,7 +5617,7 @@
         <v>134</v>
       </c>
       <c r="CE12" s="21" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="CL12" s="21" t="s">
         <v>134</v>
@@ -5559,7 +5630,7 @@
         <v>108</v>
       </c>
       <c r="DI12" s="21" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="DJ12" s="21" t="s">
         <v>175</v>
@@ -5577,7 +5648,7 @@
         <v>0</v>
       </c>
       <c r="DP12" s="21" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="DQ12" s="21" t="s">
         <v>120</v>
@@ -5595,7 +5666,7 @@
         <v>122</v>
       </c>
       <c r="DV12" s="21" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="DW12" s="21" t="s">
         <v>47</v>
@@ -5640,7 +5711,7 @@
         <v>134</v>
       </c>
       <c r="EK12" s="27" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="EL12" s="21" t="s">
         <v>134</v>
@@ -5663,22 +5734,22 @@
         <v>131</v>
       </c>
       <c r="E13" s="21" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="F13" s="21" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="G13" s="21" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="H13" s="21" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="I13" s="21" t="s">
         <v>161</v>
       </c>
       <c r="J13" s="21" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="K13" s="21" t="s">
         <v>87</v>
@@ -5693,13 +5764,13 @@
         <v>1940</v>
       </c>
       <c r="P13" s="21" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="Q13" s="21">
         <v>21</v>
       </c>
       <c r="R13" s="30" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="S13" s="22"/>
       <c r="T13" s="22"/>
@@ -5709,14 +5780,17 @@
       <c r="Z13" s="21" t="s">
         <v>0</v>
       </c>
+      <c r="AA13" s="21" t="s">
+        <v>420</v>
+      </c>
       <c r="AB13" s="21" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="AH13" s="19" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="AI13" s="19" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="AJ13" s="19"/>
       <c r="AK13" s="19"/>
@@ -5748,7 +5822,7 @@
         <v>145</v>
       </c>
       <c r="CE13" s="21" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="CF13" s="21" t="s">
         <v>74</v>
@@ -5769,7 +5843,7 @@
         <v>66</v>
       </c>
       <c r="DP13" s="21" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="DQ13" s="21" t="s">
         <v>120</v>
@@ -5787,7 +5861,7 @@
         <v>122</v>
       </c>
       <c r="DV13" s="21" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="DW13" s="21" t="s">
         <v>47</v>
@@ -5832,7 +5906,7 @@
         <v>145</v>
       </c>
       <c r="EK13" s="27" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="EL13" s="21" t="s">
         <v>145</v>
@@ -5852,39 +5926,39 @@
     </row>
     <row r="14" spans="1:146" s="21" customFormat="1" ht="88" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K14" s="25" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="AH14" s="19" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="AI14" s="19" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="AJ14" s="19"/>
       <c r="AK14" s="19"/>
     </row>
     <row r="15" spans="1:146" s="21" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="K15" s="21" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="AH15" s="19" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="AI15" s="19" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="AJ15" s="19"/>
       <c r="AK15" s="19"/>
     </row>
     <row r="16" spans="1:146" s="21" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="K16" s="21" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="AH16" s="19" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="AI16" s="19" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="AJ16" s="19"/>
       <c r="AK16" s="19"/>
@@ -5894,10 +5968,10 @@
         <v>139</v>
       </c>
       <c r="AH17" s="19" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="AI17" s="19" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="AJ17" s="19"/>
       <c r="AK17" s="19"/>
@@ -5936,6 +6010,15 @@
     <hyperlink ref="AI14:AI17" r:id="rId27" display="charmsparticipant12@yopmail.com" xr:uid="{0D113990-F28B-4045-82B3-3B329AB1A52B}"/>
     <hyperlink ref="AJ2" r:id="rId28" xr:uid="{E22D24ED-7C96-1446-A5F8-21D1507C6179}"/>
     <hyperlink ref="AJ3" r:id="rId29" xr:uid="{70C65664-4427-354A-B785-E0B132A43F5C}"/>
+    <hyperlink ref="AJ4" r:id="rId30" xr:uid="{CC02BCBB-3BDC-CE48-A7EB-DEE29B97C95A}"/>
+    <hyperlink ref="AJ5:AJ11" r:id="rId31" display="sj.fanconitester3@yopmail.com" xr:uid="{E1A1E55B-77EC-F549-BF2B-EE817EA7E8DB}"/>
+    <hyperlink ref="AJ5" r:id="rId32" xr:uid="{3BFA334B-C797-5844-9469-BDCBE15B724A}"/>
+    <hyperlink ref="AJ6" r:id="rId33" xr:uid="{A23BBEA4-5507-924C-9662-585110B0F717}"/>
+    <hyperlink ref="AJ7" r:id="rId34" xr:uid="{41B062F1-F9CB-704F-818B-85592F6D9883}"/>
+    <hyperlink ref="AJ8" r:id="rId35" xr:uid="{7C53923E-E953-094F-A49D-C82B1F6B95B8}"/>
+    <hyperlink ref="AJ9" r:id="rId36" xr:uid="{DDC7D204-E39A-FC48-A4E1-997987E166A4}"/>
+    <hyperlink ref="AJ10" r:id="rId37" xr:uid="{0AF75C1A-C67C-FB4B-AE7C-3961DA7F4B14}"/>
+    <hyperlink ref="AJ11" r:id="rId38" xr:uid="{8ACA7222-D208-AD4D-8034-E244E11A98B6}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -5964,25 +6047,25 @@
   <sheetData>
     <row r="1" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B1" s="5" t="s">
+        <v>272</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>273</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="D1" s="5" t="s">
         <v>274</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="E1" s="5" t="s">
         <v>275</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="F1" s="5" t="s">
         <v>276</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="G1" s="5" t="s">
         <v>277</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>278</v>
       </c>
       <c r="H1" s="5" t="s">
         <v>123</v>
@@ -5991,7 +6074,7 @@
         <v>124</v>
       </c>
       <c r="J1" s="5" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="17" x14ac:dyDescent="0.2">
@@ -5999,7 +6082,7 @@
         <v>37</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>59</v>
@@ -6028,10 +6111,10 @@
         <v>43</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>61</v>
@@ -6052,7 +6135,7 @@
         <v>1991</v>
       </c>
       <c r="J3" s="6" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="17" x14ac:dyDescent="0.2">
@@ -6060,10 +6143,10 @@
         <v>43</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>129</v>
@@ -6084,7 +6167,7 @@
         <v>1992</v>
       </c>
       <c r="J4" s="6" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="17" x14ac:dyDescent="0.2">
@@ -6092,19 +6175,19 @@
         <v>47</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="E5" s="4">
         <v>3013454562</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="G5" s="4" t="s">
         <v>0</v>
@@ -6116,7 +6199,7 @@
         <v>1993</v>
       </c>
       <c r="J5" s="6" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="17" x14ac:dyDescent="0.2">
@@ -6124,19 +6207,19 @@
         <v>47</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="E6" s="4">
         <v>3013454562</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="G6" s="4" t="s">
         <v>0</v>
@@ -6148,7 +6231,7 @@
         <v>1994</v>
       </c>
       <c r="J6" s="6" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="17" x14ac:dyDescent="0.2">
@@ -6156,19 +6239,19 @@
         <v>47</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="E7" s="4">
         <v>3013454562</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="G7" s="4" t="s">
         <v>0</v>
@@ -6180,12 +6263,12 @@
         <v>1995</v>
       </c>
       <c r="J7" s="6" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="I12" s="6" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
   </sheetData>
@@ -6198,7 +6281,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{288B407C-E01B-5444-BAC5-548BBFB02ADF}">
   <dimension ref="A1:K9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
@@ -6233,7 +6316,7 @@
         <v>100</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>102</v>
@@ -6242,10 +6325,10 @@
         <v>103</v>
       </c>
       <c r="J1" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>220</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="17" x14ac:dyDescent="0.2">
@@ -6292,7 +6375,7 @@
         <v>78</v>
       </c>
       <c r="D3" s="28" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="E3" s="2"/>
       <c r="F3" s="2">
@@ -6302,16 +6385,16 @@
         <v>134</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="17" x14ac:dyDescent="0.2">
@@ -6319,13 +6402,13 @@
         <v>173</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>170</v>
       </c>
       <c r="D4" s="28" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
@@ -6333,30 +6416,30 @@
         <v>134</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>281</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>282</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>78</v>
       </c>
       <c r="D5" s="28" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="2">
@@ -6366,24 +6449,24 @@
         <v>0</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="51" x14ac:dyDescent="0.2">
       <c r="A6" s="20" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B6" s="20" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="C6" s="20" t="s">
         <v>77</v>
@@ -6399,30 +6482,30 @@
         <v>0</v>
       </c>
       <c r="H6" s="20" t="s">
+        <v>334</v>
+      </c>
+      <c r="I6" s="20" t="s">
         <v>335</v>
       </c>
-      <c r="I6" s="20" t="s">
+      <c r="J6" s="20" t="s">
         <v>336</v>
       </c>
-      <c r="J6" s="20" t="s">
+      <c r="K6" s="20" t="s">
         <v>337</v>
-      </c>
-      <c r="K6" s="20" t="s">
-        <v>338</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="34" x14ac:dyDescent="0.2">
       <c r="A7" s="20" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B7" s="20" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C7" s="20" t="s">
         <v>78</v>
       </c>
       <c r="D7" s="29" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="E7" s="20"/>
       <c r="F7" s="20">
@@ -6432,16 +6515,16 @@
         <v>134</v>
       </c>
       <c r="H7" s="20" t="s">
+        <v>338</v>
+      </c>
+      <c r="I7" s="20" t="s">
         <v>339</v>
       </c>
-      <c r="I7" s="20" t="s">
+      <c r="J7" s="20" t="s">
         <v>340</v>
       </c>
-      <c r="J7" s="20" t="s">
+      <c r="K7" s="20" t="s">
         <v>341</v>
-      </c>
-      <c r="K7" s="20" t="s">
-        <v>342</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="17" x14ac:dyDescent="0.2">
@@ -6449,13 +6532,13 @@
         <v>187</v>
       </c>
       <c r="B8" s="20" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="C8" s="20" t="s">
         <v>170</v>
       </c>
       <c r="D8" s="29" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="E8" s="20"/>
       <c r="F8" s="20"/>
@@ -6463,30 +6546,30 @@
         <v>134</v>
       </c>
       <c r="H8" s="20" t="s">
+        <v>342</v>
+      </c>
+      <c r="I8" s="20" t="s">
         <v>343</v>
       </c>
-      <c r="I8" s="20" t="s">
+      <c r="J8" s="20" t="s">
         <v>344</v>
       </c>
-      <c r="J8" s="20" t="s">
+      <c r="K8" s="20" t="s">
         <v>345</v>
-      </c>
-      <c r="K8" s="20" t="s">
-        <v>346</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="34" x14ac:dyDescent="0.2">
       <c r="A9" s="20" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B9" s="20" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="C9" s="20" t="s">
         <v>78</v>
       </c>
       <c r="D9" s="29" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="E9" s="20"/>
       <c r="F9" s="20">
@@ -6496,16 +6579,16 @@
         <v>0</v>
       </c>
       <c r="H9" s="20" t="s">
+        <v>346</v>
+      </c>
+      <c r="I9" s="20" t="s">
         <v>347</v>
       </c>
-      <c r="I9" s="20" t="s">
+      <c r="J9" s="20" t="s">
         <v>348</v>
       </c>
-      <c r="J9" s="20" t="s">
+      <c r="K9" s="20" t="s">
         <v>349</v>
-      </c>
-      <c r="K9" s="20" t="s">
-        <v>350</v>
       </c>
     </row>
   </sheetData>
@@ -6530,63 +6613,63 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="31" t="s">
+        <v>442</v>
+      </c>
+      <c r="B1" s="32" t="s">
         <v>443</v>
-      </c>
-      <c r="B1" s="32" t="s">
-        <v>444</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="33" t="s">
+        <v>444</v>
+      </c>
+      <c r="B2" s="34" t="s">
         <v>445</v>
-      </c>
-      <c r="B2" s="34" t="s">
-        <v>446</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="31" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="B3" s="34" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="31" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="B4" s="34" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="31" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="B5" s="34" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="31" t="s">
+        <v>449</v>
+      </c>
+      <c r="B6" s="35" t="s">
         <v>450</v>
-      </c>
-      <c r="B6" s="35" t="s">
-        <v>451</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="31" t="s">
+        <v>451</v>
+      </c>
+      <c r="B7" s="34" t="s">
         <v>452</v>
-      </c>
-      <c r="B7" s="34" t="s">
-        <v>453</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="31" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="B8" s="34">
         <v>1948</v>
@@ -6594,7 +6677,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="31" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="B9" s="34" t="s">
         <v>20</v>
@@ -6602,7 +6685,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="31" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="B10" s="34" t="s">
         <v>134</v>
@@ -6610,7 +6693,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="31" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="B11" s="34" t="s">
         <v>22</v>
@@ -6618,23 +6701,23 @@
     </row>
     <row r="12" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" s="33" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="31" t="s">
+        <v>458</v>
+      </c>
+      <c r="B13" s="34" t="s">
         <v>459</v>
-      </c>
-      <c r="B13" s="34" t="s">
-        <v>460</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="31" t="s">
+        <v>460</v>
+      </c>
+      <c r="B14" s="34" t="s">
         <v>461</v>
-      </c>
-      <c r="B14" s="34" t="s">
-        <v>462</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
@@ -6642,20 +6725,20 @@
         <v>10</v>
       </c>
       <c r="B15" s="34" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" s="31" t="s">
+        <v>463</v>
+      </c>
+      <c r="B16" s="34" t="s">
         <v>464</v>
-      </c>
-      <c r="B16" s="34" t="s">
-        <v>465</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="31" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="B17" s="34">
         <v>22015</v>
@@ -6663,47 +6746,47 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="31" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="B18" s="36" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" s="31" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="B19" s="36" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="31" t="s">
+        <v>468</v>
+      </c>
+      <c r="B20" s="34" t="s">
         <v>469</v>
-      </c>
-      <c r="B20" s="34" t="s">
-        <v>470</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" s="31" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="B21" s="34" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" s="31" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="B22" s="34" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" s="31" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="B23" s="34" t="s">
         <v>143</v>
@@ -6711,7 +6794,7 @@
     </row>
     <row r="24" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A24" s="33" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="B24" s="34" t="s">
         <v>167</v>
@@ -6719,23 +6802,23 @@
     </row>
     <row r="25" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A25" s="33" t="s">
+        <v>474</v>
+      </c>
+      <c r="B25" s="34" t="s">
         <v>475</v>
-      </c>
-      <c r="B25" s="34" t="s">
-        <v>476</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A26" s="33" t="s">
+        <v>476</v>
+      </c>
+      <c r="B26" s="34" t="s">
         <v>477</v>
-      </c>
-      <c r="B26" s="34" t="s">
-        <v>478</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A27" s="33" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="B27" s="34" t="s">
         <v>134</v>
@@ -6743,7 +6826,7 @@
     </row>
     <row r="28" spans="1:2" ht="51" x14ac:dyDescent="0.2">
       <c r="A28" s="33" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="B28" s="34" t="s">
         <v>134</v>
@@ -6751,7 +6834,7 @@
     </row>
     <row r="29" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A29" s="33" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="B29" s="34" t="s">
         <v>134</v>
@@ -6759,7 +6842,7 @@
     </row>
     <row r="30" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A30" s="33" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="B30" s="34" t="s">
         <v>134</v>
@@ -6767,7 +6850,7 @@
     </row>
     <row r="31" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A31" s="33" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="B31" s="34" t="s">
         <v>47</v>
@@ -6775,15 +6858,15 @@
     </row>
     <row r="32" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A32" s="33" t="s">
+        <v>483</v>
+      </c>
+      <c r="B32" s="34" t="s">
         <v>484</v>
-      </c>
-      <c r="B32" s="34" t="s">
-        <v>485</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A33" s="33" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="B33" s="34" t="s">
         <v>134</v>
@@ -6791,7 +6874,7 @@
     </row>
     <row r="34" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A34" s="33" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="B34" s="34" t="s">
         <v>47</v>
@@ -6799,18 +6882,18 @@
     </row>
     <row r="35" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A35" s="33" t="s">
+        <v>487</v>
+      </c>
+      <c r="B35" s="34" t="s">
         <v>488</v>
-      </c>
-      <c r="B35" s="34" t="s">
-        <v>489</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="323" x14ac:dyDescent="0.2">
       <c r="A36" s="33" t="s">
+        <v>489</v>
+      </c>
+      <c r="B36" s="37" t="s">
         <v>490</v>
-      </c>
-      <c r="B36" s="37" t="s">
-        <v>491</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
made changes based on PR
</commit_message>
<xml_diff>
--- a/src/test/java/CHARMS/resources/data.xlsx
+++ b/src/test/java/CHARMS/resources/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jains18/git/CBIIT-Test-Automation/CBIIT-Test-Automation/src/test/java/CHARMS/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B959F6BE-7B6A-A542-9345-B92980057D74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E2B200A-0E96-304E-B230-078AD98998B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="720" yWindow="760" windowWidth="44440" windowHeight="17640" xr2:uid="{B3E53782-D40D-CC47-BA00-27DFD8C445AF}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17640" xr2:uid="{B3E53782-D40D-CC47-BA00-27DFD8C445AF}"/>
   </bookViews>
   <sheets>
     <sheet name="FanconiScreener" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1317" uniqueCount="500">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1322" uniqueCount="500">
   <si>
     <t>Yes</t>
   </si>
@@ -2192,9 +2192,9 @@
   </sheetPr>
   <dimension ref="A1:EP18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" zoomScale="113" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="AE1" zoomScale="113" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AC3" sqref="AC3"/>
+      <selection pane="bottomLeft" activeCell="A10" sqref="A10:XFD10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3164,6 +3164,9 @@
       <c r="AX3" s="21" t="s">
         <v>418</v>
       </c>
+      <c r="AY3" s="21" t="s">
+        <v>0</v>
+      </c>
       <c r="AZ3" s="21" t="s">
         <v>134</v>
       </c>
@@ -3445,6 +3448,9 @@
       <c r="AX4" s="21" t="s">
         <v>27</v>
       </c>
+      <c r="AY4" s="21" t="s">
+        <v>0</v>
+      </c>
       <c r="AZ4" s="21" t="s">
         <v>134</v>
       </c>
@@ -3720,6 +3726,9 @@
       <c r="AQ5" s="21" t="s">
         <v>145</v>
       </c>
+      <c r="AY5" s="21" t="s">
+        <v>0</v>
+      </c>
       <c r="AZ5" s="21" t="s">
         <v>134</v>
       </c>
@@ -3994,6 +4003,9 @@
       <c r="AQ6" s="21" t="s">
         <v>167</v>
       </c>
+      <c r="AY6" s="21" t="s">
+        <v>0</v>
+      </c>
       <c r="AZ6" s="21" t="s">
         <v>145</v>
       </c>
@@ -4207,6 +4219,9 @@
       </c>
       <c r="AQ7" s="21" t="s">
         <v>167</v>
+      </c>
+      <c r="AY7" s="21" t="s">
+        <v>0</v>
       </c>
       <c r="AZ7" s="21" t="s">
         <v>134</v>

</xml_diff>

<commit_message>
Added code for different scenarios
</commit_message>
<xml_diff>
--- a/src/test/java/CHARMS/resources/data.xlsx
+++ b/src/test/java/CHARMS/resources/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jains18/git/CBIIT-Test-Automation/CBIIT-Test-Automation/src/test/java/CHARMS/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E2B200A-0E96-304E-B230-078AD98998B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC10D563-58D4-BC4C-977E-B0550DAB40FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17640" xr2:uid="{B3E53782-D40D-CC47-BA00-27DFD8C445AF}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1322" uniqueCount="500">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1324" uniqueCount="498">
   <si>
     <t>Yes</t>
   </si>
@@ -1328,28 +1328,10 @@
     <t>CalculatedAge</t>
   </si>
   <si>
-    <t>01/23/1920</t>
-  </si>
-  <si>
     <t>01/21/1910</t>
   </si>
   <si>
     <t>01/21/1925</t>
-  </si>
-  <si>
-    <t>01/26/1950</t>
-  </si>
-  <si>
-    <t>01/11/1940</t>
-  </si>
-  <si>
-    <t>01/30/1930</t>
-  </si>
-  <si>
-    <t>01/29/1935</t>
-  </si>
-  <si>
-    <t>01/27/1937</t>
   </si>
   <si>
     <t>01/21/1935</t>
@@ -1545,6 +1527,18 @@
   </si>
   <si>
     <t>Caucasian (white), Black/African American, Native Hawaiian/Other Pacific Islander, American Indian/Alaskan Native, Asian,  Other (please specify)</t>
+  </si>
+  <si>
+    <t>01/21/1960</t>
+  </si>
+  <si>
+    <t>01/21/1950</t>
+  </si>
+  <si>
+    <t>01/21/1930</t>
+  </si>
+  <si>
+    <t>01/21/1937</t>
   </si>
 </sst>
 </file>
@@ -1754,7 +1748,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1862,6 +1856,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2192,9 +2189,9 @@
   </sheetPr>
   <dimension ref="A1:EP18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AE1" zoomScale="113" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="BP1" zoomScale="113" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A10" sqref="A10:XFD10"/>
+      <selection pane="bottomLeft" activeCell="BX2" sqref="BX2:BX3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2714,13 +2711,13 @@
         <v>1948</v>
       </c>
       <c r="P2" s="21" t="s">
-        <v>438</v>
+        <v>432</v>
       </c>
       <c r="Q2" s="21">
         <v>21</v>
       </c>
       <c r="R2" s="30" t="s">
-        <v>441</v>
+        <v>435</v>
       </c>
       <c r="S2" s="22"/>
       <c r="T2" s="21">
@@ -2868,10 +2865,10 @@
       <c r="BV2" s="21" t="s">
         <v>65</v>
       </c>
-      <c r="BW2" s="23" t="s">
+      <c r="BW2" s="38" t="s">
         <v>264</v>
       </c>
-      <c r="BX2" s="23" t="s">
+      <c r="BX2" s="38" t="s">
         <v>264</v>
       </c>
       <c r="BY2" s="21" t="s">
@@ -2971,7 +2968,7 @@
         <v>111</v>
       </c>
       <c r="DK2" s="21" t="s">
-        <v>440</v>
+        <v>434</v>
       </c>
       <c r="DL2" s="21" t="s">
         <v>113</v>
@@ -3004,7 +3001,7 @@
         <v>122</v>
       </c>
       <c r="DV2" s="21" t="s">
-        <v>439</v>
+        <v>433</v>
       </c>
       <c r="DW2" s="21" t="s">
         <v>47</v>
@@ -3084,19 +3081,21 @@
         <v>134</v>
       </c>
       <c r="O3" s="21">
-        <v>1920</v>
+        <v>1960</v>
       </c>
       <c r="P3" s="21" t="s">
-        <v>438</v>
+        <v>432</v>
       </c>
       <c r="Q3" s="21">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="R3" s="30" t="s">
-        <v>428</v>
+        <v>494</v>
       </c>
       <c r="S3" s="22"/>
-      <c r="T3" s="22"/>
+      <c r="T3" s="22">
+        <v>65</v>
+      </c>
       <c r="U3" s="21" t="s">
         <v>141</v>
       </c>
@@ -3188,6 +3187,12 @@
       <c r="BV3" s="21" t="s">
         <v>148</v>
       </c>
+      <c r="BW3" s="38" t="s">
+        <v>264</v>
+      </c>
+      <c r="BX3" s="38" t="s">
+        <v>264</v>
+      </c>
       <c r="BY3" s="21" t="s">
         <v>149</v>
       </c>
@@ -3306,7 +3311,7 @@
         <v>122</v>
       </c>
       <c r="DV3" s="21" t="s">
-        <v>439</v>
+        <v>433</v>
       </c>
       <c r="DW3" s="21" t="s">
         <v>47</v>
@@ -3389,13 +3394,13 @@
         <v>1910</v>
       </c>
       <c r="P4" s="21" t="s">
-        <v>438</v>
+        <v>432</v>
       </c>
       <c r="Q4" s="21">
         <v>21</v>
       </c>
       <c r="R4" s="30" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="S4" s="22"/>
       <c r="T4" s="22"/>
@@ -3424,7 +3429,7 @@
         <v>144</v>
       </c>
       <c r="AJ4" s="19" t="s">
-        <v>491</v>
+        <v>485</v>
       </c>
       <c r="AK4" s="18"/>
       <c r="AL4" s="21">
@@ -3581,7 +3586,7 @@
         <v>122</v>
       </c>
       <c r="DV4" s="21" t="s">
-        <v>439</v>
+        <v>433</v>
       </c>
       <c r="DW4" s="21" t="s">
         <v>47</v>
@@ -3664,13 +3669,13 @@
         <v>1925</v>
       </c>
       <c r="P5" s="21" t="s">
-        <v>438</v>
+        <v>432</v>
       </c>
       <c r="Q5" s="21">
         <v>21</v>
       </c>
       <c r="R5" s="30" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="S5" s="22"/>
       <c r="T5" s="22"/>
@@ -3705,7 +3710,7 @@
         <v>162</v>
       </c>
       <c r="AJ5" s="19" t="s">
-        <v>492</v>
+        <v>486</v>
       </c>
       <c r="AK5" s="19"/>
       <c r="AL5" s="21">
@@ -3865,7 +3870,7 @@
         <v>122</v>
       </c>
       <c r="DV5" s="21" t="s">
-        <v>439</v>
+        <v>433</v>
       </c>
       <c r="DW5" s="21" t="s">
         <v>47</v>
@@ -3948,13 +3953,13 @@
         <v>1950</v>
       </c>
       <c r="P6" s="21" t="s">
-        <v>438</v>
+        <v>432</v>
       </c>
       <c r="Q6" s="21">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="R6" s="30" t="s">
-        <v>431</v>
+        <v>495</v>
       </c>
       <c r="S6" s="22"/>
       <c r="T6" s="22"/>
@@ -3983,7 +3988,7 @@
         <v>178</v>
       </c>
       <c r="AJ6" s="19" t="s">
-        <v>493</v>
+        <v>487</v>
       </c>
       <c r="AL6" s="21">
         <v>3015774089</v>
@@ -4081,7 +4086,7 @@
         <v>122</v>
       </c>
       <c r="DV6" s="21" t="s">
-        <v>439</v>
+        <v>433</v>
       </c>
       <c r="DW6" s="21" t="s">
         <v>47</v>
@@ -4164,13 +4169,13 @@
         <v>1940</v>
       </c>
       <c r="P7" s="21" t="s">
-        <v>438</v>
+        <v>432</v>
       </c>
       <c r="Q7" s="21">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="R7" s="30" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="S7" s="22"/>
       <c r="T7" s="22"/>
@@ -4199,7 +4204,7 @@
         <v>317</v>
       </c>
       <c r="AJ7" s="19" t="s">
-        <v>494</v>
+        <v>488</v>
       </c>
       <c r="AK7" s="18"/>
       <c r="AL7" s="21">
@@ -4313,7 +4318,7 @@
         <v>122</v>
       </c>
       <c r="DV7" s="21" t="s">
-        <v>439</v>
+        <v>433</v>
       </c>
       <c r="DW7" s="21" t="s">
         <v>47</v>
@@ -4396,13 +4401,13 @@
         <v>1930</v>
       </c>
       <c r="P8" s="21" t="s">
-        <v>438</v>
+        <v>432</v>
       </c>
       <c r="Q8" s="21">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="R8" s="30" t="s">
-        <v>433</v>
+        <v>496</v>
       </c>
       <c r="S8" s="22"/>
       <c r="T8" s="22"/>
@@ -4446,7 +4451,7 @@
         <v>318</v>
       </c>
       <c r="AJ8" s="19" t="s">
-        <v>495</v>
+        <v>489</v>
       </c>
       <c r="AK8" s="18"/>
       <c r="AL8" s="21">
@@ -4530,7 +4535,7 @@
         <v>122</v>
       </c>
       <c r="DV8" s="21" t="s">
-        <v>439</v>
+        <v>433</v>
       </c>
       <c r="DW8" s="21" t="s">
         <v>47</v>
@@ -4613,13 +4618,13 @@
         <v>1935</v>
       </c>
       <c r="P9" s="21" t="s">
-        <v>438</v>
+        <v>432</v>
       </c>
       <c r="Q9" s="21">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="R9" s="30" t="s">
-        <v>434</v>
+        <v>430</v>
       </c>
       <c r="S9" s="22"/>
       <c r="T9" s="22"/>
@@ -4648,7 +4653,7 @@
         <v>319</v>
       </c>
       <c r="AJ9" s="19" t="s">
-        <v>496</v>
+        <v>490</v>
       </c>
       <c r="AK9" s="18"/>
       <c r="AL9" s="21">
@@ -4812,7 +4817,7 @@
         <v>122</v>
       </c>
       <c r="DV9" s="21" t="s">
-        <v>439</v>
+        <v>433</v>
       </c>
       <c r="DW9" s="21" t="s">
         <v>47</v>
@@ -4910,13 +4915,13 @@
         <v>1937</v>
       </c>
       <c r="P10" s="21" t="s">
-        <v>438</v>
+        <v>432</v>
       </c>
       <c r="Q10" s="21">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="R10" s="30" t="s">
-        <v>435</v>
+        <v>497</v>
       </c>
       <c r="S10" s="22"/>
       <c r="T10" s="22"/>
@@ -4955,7 +4960,7 @@
         <v>325</v>
       </c>
       <c r="AJ10" s="19" t="s">
-        <v>497</v>
+        <v>491</v>
       </c>
       <c r="AK10" s="18"/>
       <c r="AL10" s="21">
@@ -4995,7 +5000,7 @@
         <v>40</v>
       </c>
       <c r="AX10" s="21" t="s">
-        <v>499</v>
+        <v>493</v>
       </c>
       <c r="AZ10" s="21" t="s">
         <v>0</v>
@@ -5157,7 +5162,7 @@
         <v>111</v>
       </c>
       <c r="DK10" s="21" t="s">
-        <v>440</v>
+        <v>434</v>
       </c>
       <c r="DL10" s="21" t="s">
         <v>113</v>
@@ -5190,7 +5195,7 @@
         <v>122</v>
       </c>
       <c r="DV10" s="21" t="s">
-        <v>439</v>
+        <v>433</v>
       </c>
       <c r="DW10" s="21" t="s">
         <v>47</v>
@@ -5291,13 +5296,13 @@
         <v>1935</v>
       </c>
       <c r="P11" s="21" t="s">
-        <v>438</v>
+        <v>432</v>
       </c>
       <c r="Q11" s="21">
         <v>21</v>
       </c>
       <c r="R11" s="30" t="s">
-        <v>436</v>
+        <v>430</v>
       </c>
       <c r="S11" s="22"/>
       <c r="T11" s="22"/>
@@ -5320,7 +5325,7 @@
         <v>326</v>
       </c>
       <c r="AJ11" s="19" t="s">
-        <v>498</v>
+        <v>492</v>
       </c>
       <c r="AK11" s="19"/>
       <c r="AL11" s="21">
@@ -5473,7 +5478,7 @@
         <v>122</v>
       </c>
       <c r="DV11" s="21" t="s">
-        <v>439</v>
+        <v>433</v>
       </c>
       <c r="DW11" s="21" t="s">
         <v>47</v>
@@ -5571,13 +5576,13 @@
         <v>1930</v>
       </c>
       <c r="P12" s="21" t="s">
-        <v>438</v>
+        <v>432</v>
       </c>
       <c r="Q12" s="21">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="R12" s="30" t="s">
-        <v>433</v>
+        <v>496</v>
       </c>
       <c r="S12" s="22"/>
       <c r="T12" s="22"/>
@@ -5681,7 +5686,7 @@
         <v>122</v>
       </c>
       <c r="DV12" s="21" t="s">
-        <v>439</v>
+        <v>433</v>
       </c>
       <c r="DW12" s="21" t="s">
         <v>47</v>
@@ -5779,13 +5784,13 @@
         <v>1940</v>
       </c>
       <c r="P13" s="21" t="s">
-        <v>438</v>
+        <v>432</v>
       </c>
       <c r="Q13" s="21">
         <v>21</v>
       </c>
       <c r="R13" s="30" t="s">
-        <v>437</v>
+        <v>431</v>
       </c>
       <c r="S13" s="22"/>
       <c r="T13" s="22"/>
@@ -5876,7 +5881,7 @@
         <v>122</v>
       </c>
       <c r="DV13" s="21" t="s">
-        <v>439</v>
+        <v>433</v>
       </c>
       <c r="DW13" s="21" t="s">
         <v>47</v>
@@ -5942,6 +5947,9 @@
     <row r="14" spans="1:146" s="21" customFormat="1" ht="88" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K14" s="25" t="s">
         <v>382</v>
+      </c>
+      <c r="Q14" s="21">
+        <v>21</v>
       </c>
       <c r="AH14" s="19" t="s">
         <v>397</v>
@@ -5956,6 +5964,9 @@
       <c r="K15" s="21" t="s">
         <v>383</v>
       </c>
+      <c r="Q15" s="21">
+        <v>21</v>
+      </c>
       <c r="AH15" s="19" t="s">
         <v>398</v>
       </c>
@@ -5968,6 +5979,9 @@
     <row r="16" spans="1:146" s="21" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="K16" s="21" t="s">
         <v>384</v>
+      </c>
+      <c r="Q16" s="21">
+        <v>21</v>
       </c>
       <c r="AH16" s="19" t="s">
         <v>399</v>
@@ -6628,23 +6642,23 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="31" t="s">
-        <v>442</v>
+        <v>436</v>
       </c>
       <c r="B1" s="32" t="s">
-        <v>443</v>
+        <v>437</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="33" t="s">
-        <v>444</v>
+        <v>438</v>
       </c>
       <c r="B2" s="34" t="s">
-        <v>445</v>
+        <v>439</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="31" t="s">
-        <v>446</v>
+        <v>440</v>
       </c>
       <c r="B3" s="34" t="s">
         <v>295</v>
@@ -6652,7 +6666,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="31" t="s">
-        <v>447</v>
+        <v>441</v>
       </c>
       <c r="B4" s="34" t="s">
         <v>296</v>
@@ -6660,7 +6674,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="31" t="s">
-        <v>448</v>
+        <v>442</v>
       </c>
       <c r="B5" s="34" t="s">
         <v>389</v>
@@ -6668,23 +6682,23 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="31" t="s">
-        <v>449</v>
+        <v>443</v>
       </c>
       <c r="B6" s="35" t="s">
-        <v>450</v>
+        <v>444</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="31" t="s">
-        <v>451</v>
+        <v>445</v>
       </c>
       <c r="B7" s="34" t="s">
-        <v>452</v>
+        <v>446</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="31" t="s">
-        <v>453</v>
+        <v>447</v>
       </c>
       <c r="B8" s="34">
         <v>1948</v>
@@ -6692,7 +6706,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="31" t="s">
-        <v>454</v>
+        <v>448</v>
       </c>
       <c r="B9" s="34" t="s">
         <v>20</v>
@@ -6700,7 +6714,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="31" t="s">
-        <v>455</v>
+        <v>449</v>
       </c>
       <c r="B10" s="34" t="s">
         <v>134</v>
@@ -6708,7 +6722,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="31" t="s">
-        <v>456</v>
+        <v>450</v>
       </c>
       <c r="B11" s="34" t="s">
         <v>22</v>
@@ -6716,23 +6730,23 @@
     </row>
     <row r="12" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" s="33" t="s">
-        <v>457</v>
+        <v>451</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="31" t="s">
-        <v>458</v>
+        <v>452</v>
       </c>
       <c r="B13" s="34" t="s">
-        <v>459</v>
+        <v>453</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="31" t="s">
-        <v>460</v>
+        <v>454</v>
       </c>
       <c r="B14" s="34" t="s">
-        <v>461</v>
+        <v>455</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
@@ -6740,20 +6754,20 @@
         <v>10</v>
       </c>
       <c r="B15" s="34" t="s">
-        <v>462</v>
+        <v>456</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" s="31" t="s">
-        <v>463</v>
+        <v>457</v>
       </c>
       <c r="B16" s="34" t="s">
-        <v>464</v>
+        <v>458</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="31" t="s">
-        <v>465</v>
+        <v>459</v>
       </c>
       <c r="B17" s="34">
         <v>22015</v>
@@ -6761,7 +6775,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="31" t="s">
-        <v>466</v>
+        <v>460</v>
       </c>
       <c r="B18" s="36" t="s">
         <v>423</v>
@@ -6769,7 +6783,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" s="31" t="s">
-        <v>467</v>
+        <v>461</v>
       </c>
       <c r="B19" s="36" t="s">
         <v>423</v>
@@ -6777,31 +6791,31 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="31" t="s">
-        <v>468</v>
+        <v>462</v>
       </c>
       <c r="B20" s="34" t="s">
-        <v>469</v>
+        <v>463</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" s="31" t="s">
-        <v>470</v>
+        <v>464</v>
       </c>
       <c r="B21" s="34" t="s">
-        <v>469</v>
+        <v>463</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" s="31" t="s">
-        <v>471</v>
+        <v>465</v>
       </c>
       <c r="B22" s="34" t="s">
-        <v>469</v>
+        <v>463</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" s="31" t="s">
-        <v>472</v>
+        <v>466</v>
       </c>
       <c r="B23" s="34" t="s">
         <v>143</v>
@@ -6809,7 +6823,7 @@
     </row>
     <row r="24" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A24" s="33" t="s">
-        <v>473</v>
+        <v>467</v>
       </c>
       <c r="B24" s="34" t="s">
         <v>167</v>
@@ -6817,23 +6831,23 @@
     </row>
     <row r="25" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A25" s="33" t="s">
-        <v>474</v>
+        <v>468</v>
       </c>
       <c r="B25" s="34" t="s">
-        <v>475</v>
+        <v>469</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A26" s="33" t="s">
-        <v>476</v>
+        <v>470</v>
       </c>
       <c r="B26" s="34" t="s">
-        <v>477</v>
+        <v>471</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A27" s="33" t="s">
-        <v>478</v>
+        <v>472</v>
       </c>
       <c r="B27" s="34" t="s">
         <v>134</v>
@@ -6841,7 +6855,7 @@
     </row>
     <row r="28" spans="1:2" ht="51" x14ac:dyDescent="0.2">
       <c r="A28" s="33" t="s">
-        <v>479</v>
+        <v>473</v>
       </c>
       <c r="B28" s="34" t="s">
         <v>134</v>
@@ -6849,7 +6863,7 @@
     </row>
     <row r="29" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A29" s="33" t="s">
-        <v>480</v>
+        <v>474</v>
       </c>
       <c r="B29" s="34" t="s">
         <v>134</v>
@@ -6857,7 +6871,7 @@
     </row>
     <row r="30" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A30" s="33" t="s">
-        <v>481</v>
+        <v>475</v>
       </c>
       <c r="B30" s="34" t="s">
         <v>134</v>
@@ -6865,7 +6879,7 @@
     </row>
     <row r="31" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A31" s="33" t="s">
-        <v>482</v>
+        <v>476</v>
       </c>
       <c r="B31" s="34" t="s">
         <v>47</v>
@@ -6873,15 +6887,15 @@
     </row>
     <row r="32" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A32" s="33" t="s">
-        <v>483</v>
+        <v>477</v>
       </c>
       <c r="B32" s="34" t="s">
-        <v>484</v>
+        <v>478</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A33" s="33" t="s">
-        <v>485</v>
+        <v>479</v>
       </c>
       <c r="B33" s="34" t="s">
         <v>134</v>
@@ -6889,7 +6903,7 @@
     </row>
     <row r="34" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A34" s="33" t="s">
-        <v>486</v>
+        <v>480</v>
       </c>
       <c r="B34" s="34" t="s">
         <v>47</v>
@@ -6897,18 +6911,18 @@
     </row>
     <row r="35" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A35" s="33" t="s">
-        <v>487</v>
+        <v>481</v>
       </c>
       <c r="B35" s="34" t="s">
-        <v>488</v>
+        <v>482</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="323" x14ac:dyDescent="0.2">
       <c r="A36" s="33" t="s">
-        <v>489</v>
+        <v>483</v>
       </c>
       <c r="B36" s="37" t="s">
-        <v>490</v>
+        <v>484</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
CHARMS - Fanconi CGB IIQ verification in Native View
</commit_message>
<xml_diff>
--- a/src/test/java/CHARMS/resources/data.xlsx
+++ b/src/test/java/CHARMS/resources/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/muzipovay2/AquaProjects/CBIIT-Test-Automation/src/test/java/CHARMS/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1245AF7-1D3A-334A-AD41-AFBC682A6562}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B231F39-4D4A-0A49-8DB6-46003D64D32C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4240" yWindow="760" windowWidth="26000" windowHeight="17600" activeTab="3" xr2:uid="{B3E53782-D40D-CC47-BA00-27DFD8C445AF}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1292" uniqueCount="492">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1292" uniqueCount="491">
   <si>
     <t>Yes</t>
   </si>
@@ -1518,9 +1518,6 @@
   </si>
   <si>
     <t>301-577-4089</t>
-  </si>
-  <si>
-    <t>charmsras3@yahoo.com</t>
   </si>
 </sst>
 </file>
@@ -6497,8 +6494,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6599F052-5E19-A342-980D-0163BD929DAC}">
   <dimension ref="A1:B36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6645,7 +6642,7 @@
         <v>465</v>
       </c>
       <c r="B18" s="33" t="s">
-        <v>491</v>
+        <v>438</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
@@ -6653,7 +6650,7 @@
         <v>466</v>
       </c>
       <c r="B19" s="33" t="s">
-        <v>491</v>
+        <v>438</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Update test scenarios to reflect recent changes in gender, pronoun, sex related questions
</commit_message>
<xml_diff>
--- a/src/test/java/CHARMS/resources/data.xlsx
+++ b/src/test/java/CHARMS/resources/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jains18/git/CBIIT-Test-Automation/CBIIT-Test-Automation/src/test/java/CHARMS/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0A27FC9-DA4B-294E-BE34-ED2C04A7B803}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3969A541-1677-E943-A003-4BB22A020631}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17640" xr2:uid="{B3E53782-D40D-CC47-BA00-27DFD8C445AF}"/>
   </bookViews>
@@ -2231,9 +2231,9 @@
   </sheetPr>
   <dimension ref="A1:EQ18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AS1" zoomScale="113" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AZ11" sqref="AZ11"/>
+    <sheetView tabSelected="1" zoomScale="113" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="V6" sqref="V6:V9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3461,7 +3461,7 @@
         <v>115</v>
       </c>
       <c r="V4" s="21" t="s">
-        <v>144</v>
+        <v>20</v>
       </c>
       <c r="W4" s="21" t="s">
         <v>161</v>
@@ -3742,7 +3742,7 @@
         <v>100</v>
       </c>
       <c r="V5" s="21" t="s">
-        <v>165</v>
+        <v>20</v>
       </c>
       <c r="W5" s="21" t="s">
         <v>178</v>
@@ -4035,7 +4035,7 @@
         <v>75</v>
       </c>
       <c r="V6" s="21" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="W6" s="21" t="s">
         <v>144</v>
@@ -4281,7 +4281,7 @@
         <v>85</v>
       </c>
       <c r="V7" s="21" t="s">
-        <v>165</v>
+        <v>140</v>
       </c>
       <c r="W7" s="21" t="s">
         <v>165</v>
@@ -4360,8 +4360,8 @@
       <c r="BX7" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="BY7" s="37" t="s">
-        <v>65</v>
+      <c r="BY7" s="21" t="s">
+        <v>354</v>
       </c>
       <c r="BZ7" s="21" t="s">
         <v>66</v>
@@ -4539,7 +4539,7 @@
         <v>95</v>
       </c>
       <c r="V8" s="21" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="W8" s="21" t="s">
         <v>165</v>
@@ -4800,7 +4800,7 @@
         <v>90</v>
       </c>
       <c r="V9" s="21" t="s">
-        <v>165</v>
+        <v>140</v>
       </c>
       <c r="W9" s="21" t="s">
         <v>161</v>

</xml_diff>

<commit_message>
Added new code to support the PD and PS  enhancements in Native view
</commit_message>
<xml_diff>
--- a/src/test/java/CHARMS/resources/data.xlsx
+++ b/src/test/java/CHARMS/resources/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jains18/git/CBIIT-Test-Automation/CBIIT-Test-Automation/src/test/java/CHARMS/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D30100A1-F255-4E4D-B590-1683BD94667B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA87B5B7-2B65-C243-B1A5-06A2FB12B079}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17640" xr2:uid="{B3E53782-D40D-CC47-BA00-27DFD8C445AF}"/>
+    <workbookView xWindow="10480" yWindow="500" windowWidth="30240" windowHeight="17640" xr2:uid="{B3E53782-D40D-CC47-BA00-27DFD8C445AF}"/>
   </bookViews>
   <sheets>
     <sheet name="FanconiScreener" sheetId="1" r:id="rId1"/>
@@ -2300,9 +2300,9 @@
   </sheetPr>
   <dimension ref="A1:FB18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="113" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="AM1" zoomScale="113" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P1" sqref="P1"/>
+      <selection pane="bottomLeft" activeCell="AU1" sqref="AU1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Added Metformin Screener code and made changes to Fanconi scripts based on new enhancements
</commit_message>
<xml_diff>
--- a/src/test/java/CHARMS/resources/data.xlsx
+++ b/src/test/java/CHARMS/resources/data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10511"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10608"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jains18/git/CBIIT-Test-Automation/CBIIT-Test-Automation/src/test/java/CHARMS/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8C209F2-CDDC-0448-AE83-0A584A69343B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8086E2E-760D-8C4D-B1E4-C46221692874}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10480" yWindow="500" windowWidth="30240" windowHeight="17640" xr2:uid="{B3E53782-D40D-CC47-BA00-27DFD8C445AF}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17640" xr2:uid="{B3E53782-D40D-CC47-BA00-27DFD8C445AF}"/>
   </bookViews>
   <sheets>
     <sheet name="FanconiScreener" sheetId="1" r:id="rId1"/>
@@ -2330,9 +2330,9 @@
   </sheetPr>
   <dimension ref="A1:FF18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AN1" zoomScale="113" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AY10" sqref="AY10:BB11"/>
+    <sheetView tabSelected="1" topLeftCell="AW1" zoomScale="113" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="BB11" sqref="BB11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5437,6 +5437,18 @@
       <c r="AX10" s="43" t="s">
         <v>322</v>
       </c>
+      <c r="AY10" s="21">
+        <v>3015774089</v>
+      </c>
+      <c r="AZ10" s="21">
+        <v>3014524258</v>
+      </c>
+      <c r="BA10" s="21">
+        <v>3015567865</v>
+      </c>
+      <c r="BB10" s="21">
+        <v>3015774089</v>
+      </c>
       <c r="BC10" s="39" t="s">
         <v>520</v>
       </c>
@@ -5829,6 +5841,18 @@
       </c>
       <c r="AX11" s="52" t="s">
         <v>323</v>
+      </c>
+      <c r="AY11" s="21">
+        <v>3015774089</v>
+      </c>
+      <c r="AZ11" s="21">
+        <v>3014524258</v>
+      </c>
+      <c r="BA11" s="21">
+        <v>3015567865</v>
+      </c>
+      <c r="BB11" s="21">
+        <v>3015774089</v>
       </c>
       <c r="BC11" s="47" t="s">
         <v>520</v>

</xml_diff>

<commit_message>
Added the code tot he contact Information tab of the Participant details and study page in Native view for Fanconi Study
</commit_message>
<xml_diff>
--- a/src/test/java/CHARMS/resources/data.xlsx
+++ b/src/test/java/CHARMS/resources/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jains18/git/CBIIT-Test-Automation/CBIIT-Test-Automation/src/test/java/CHARMS/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8086E2E-760D-8C4D-B1E4-C46221692874}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3C3E06B-92B6-C145-A6B5-48E9DAA560DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17640" xr2:uid="{B3E53782-D40D-CC47-BA00-27DFD8C445AF}"/>
+    <workbookView xWindow="10480" yWindow="500" windowWidth="30240" windowHeight="17640" xr2:uid="{B3E53782-D40D-CC47-BA00-27DFD8C445AF}"/>
   </bookViews>
   <sheets>
     <sheet name="FanconiScreener" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1427" uniqueCount="523">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1433" uniqueCount="523">
   <si>
     <t>Yes</t>
   </si>
@@ -2330,9 +2330,9 @@
   </sheetPr>
   <dimension ref="A1:FF18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AW1" zoomScale="113" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="AV1" zoomScale="113" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="BB11" sqref="BB11"/>
+      <selection pane="bottomLeft" activeCell="AO12" sqref="AO12:AO13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5425,6 +5425,24 @@
       <c r="AN10" s="39" t="s">
         <v>414</v>
       </c>
+      <c r="AO10" s="39" t="s">
+        <v>22</v>
+      </c>
+      <c r="AP10" s="21" t="s">
+        <v>193</v>
+      </c>
+      <c r="AQ10" s="21" t="s">
+        <v>194</v>
+      </c>
+      <c r="AR10" s="21" t="s">
+        <v>195</v>
+      </c>
+      <c r="AS10" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="AT10" s="21">
+        <v>28907</v>
+      </c>
       <c r="AU10" s="43" t="s">
         <v>322</v>
       </c>
@@ -5829,6 +5847,9 @@
       </c>
       <c r="AN11" s="47" t="s">
         <v>414</v>
+      </c>
+      <c r="AO11" s="47" t="s">
+        <v>164</v>
       </c>
       <c r="AU11" s="51" t="s">
         <v>323</v>

</xml_diff>